<commit_message>
luffy img format update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A2CAFB-FC52-4344-A27F-83075EFF2AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E16C61-D347-42AB-80BA-73E973759B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -636,15 +636,9 @@
     <t>Zoro Wano.jpg</t>
   </si>
   <si>
-    <t>Nika Luffy color.jpg</t>
-  </si>
-  <si>
     <t>Nika Luffy white.jpg</t>
   </si>
   <si>
-    <t>Luffy (dy).jpg</t>
-  </si>
-  <si>
     <t>nika luffy white tp.jpg</t>
   </si>
   <si>
@@ -703,6 +697,12 @@
   </si>
   <si>
     <t>Moonknight black comic.png</t>
+  </si>
+  <si>
+    <t>nika Luffy color.jpg</t>
+  </si>
+  <si>
+    <t>luffy (dy).jpg</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1843,7 @@
         <v>250</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -1945,7 +1945,7 @@
         <v>250</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2421,7 +2421,7 @@
         <v>300</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>68</v>
@@ -2438,7 +2438,7 @@
         <v>270</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>68</v>
@@ -2455,7 +2455,7 @@
         <v>300</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>68</v>
@@ -2591,7 +2591,7 @@
         <v>300</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>68</v>
@@ -2642,7 +2642,7 @@
         <v>350</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>68</v>
@@ -2659,7 +2659,7 @@
         <v>350</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>68</v>
@@ -2676,7 +2676,7 @@
         <v>320</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>68</v>
@@ -2693,7 +2693,7 @@
         <v>320</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>68</v>
@@ -2710,7 +2710,7 @@
         <v>320</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>68</v>
@@ -2727,7 +2727,7 @@
         <v>320</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>68</v>
@@ -2744,7 +2744,7 @@
         <v>320</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>68</v>
@@ -2761,7 +2761,7 @@
         <v>320</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>68</v>
@@ -2778,7 +2778,7 @@
         <v>320</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>68</v>
@@ -2795,7 +2795,7 @@
         <v>320</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>68</v>
@@ -2812,7 +2812,7 @@
         <v>320</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>68</v>
@@ -2829,7 +2829,7 @@
         <v>320</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>68</v>
@@ -2846,7 +2846,7 @@
         <v>320</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>68</v>
@@ -2863,7 +2863,7 @@
         <v>320</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>68</v>
@@ -2880,7 +2880,7 @@
         <v>320</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>68</v>
@@ -2897,7 +2897,7 @@
         <v>320</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>68</v>
@@ -2914,7 +2914,7 @@
         <v>320</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
sliight spacing causes a lot of prob
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF58FC63-D827-4C0F-A5EC-BCBE7E23A755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C943793-7C4B-4991-AAB9-F57A02BBF255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="253">
   <si>
     <t>Product</t>
   </si>
@@ -727,9 +727,6 @@
   </si>
   <si>
     <t>Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placeholder.jpg  </t>
   </si>
   <si>
     <t>Batmobile black.jpeg</t>
@@ -1315,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,10 +1433,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -2034,7 +2031,7 @@
         <v>250</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2119,7 +2116,7 @@
         <v>150</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>52</v>
@@ -2136,7 +2133,7 @@
         <v>300</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>52</v>
@@ -2153,7 +2150,7 @@
         <v>300</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>52</v>
@@ -2170,7 +2167,7 @@
         <v>180</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>52</v>
@@ -2187,7 +2184,7 @@
         <v>160</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>52</v>
@@ -2238,7 +2235,7 @@
         <v>350</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>52</v>
@@ -2255,7 +2252,7 @@
         <v>350</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>52</v>
@@ -2272,7 +2269,7 @@
         <v>500</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>52</v>
@@ -2289,7 +2286,7 @@
         <v>350</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>52</v>
@@ -2306,7 +2303,7 @@
         <v>350</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>52</v>
@@ -2323,7 +2320,7 @@
         <v>350</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>52</v>
@@ -2340,7 +2337,7 @@
         <v>500</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>52</v>
@@ -2357,7 +2354,7 @@
         <v>500</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>52</v>
@@ -2374,7 +2371,7 @@
         <v>300</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>68</v>
@@ -2408,7 +2405,7 @@
         <v>300</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>68</v>
@@ -3105,7 +3102,7 @@
         <v>300</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>68</v>
@@ -3122,7 +3119,7 @@
         <v>300</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>68</v>
@@ -3139,7 +3136,7 @@
         <v>300</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>68</v>
@@ -3156,7 +3153,7 @@
         <v>300</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>68</v>
@@ -3173,7 +3170,7 @@
         <v>300</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>68</v>
@@ -3190,7 +3187,7 @@
         <v>300</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>68</v>
@@ -3207,7 +3204,7 @@
         <v>300</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>68</v>
@@ -3530,7 +3527,7 @@
         <v>500</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
forgot to change one png
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C943793-7C4B-4991-AAB9-F57A02BBF255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF8A6F-91F1-4A51-B550-9AB54C8B3894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -789,10 +789,10 @@
     <t>Gotham Stand.jpg</t>
   </si>
   <si>
-    <t>Sasuke &amp; Naruto(war).jpg</t>
-  </si>
-  <si>
     <t>Hawkeye.jpeg</t>
+  </si>
+  <si>
+    <t>Sasuke &amp; Naruto(war).png</t>
   </si>
 </sst>
 </file>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1436,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -3527,7 +3527,7 @@
         <v>500</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
price update for dc
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6291AE87-6746-457B-8B48-B58537821B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA4D1B7-D8C6-4EB4-9DDA-25EE846C656B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1065" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -1408,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2209,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="3">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>264</v>
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="3">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>183</v>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="3">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>183</v>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="3">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>245</v>
@@ -2294,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="3">
-        <v>160</v>
+        <v>300</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>265</v>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="3">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>266</v>

</xml_diff>

<commit_message>
image and stock update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA4D1B7-D8C6-4EB4-9DDA-25EE846C656B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD0169-F5E4-4A77-ABA8-B0E0CE2E1AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1065" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="4005" yWindow="1365" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="298">
   <si>
     <t>Product</t>
   </si>
@@ -889,6 +889,45 @@
   </si>
   <si>
     <t>Kaiju no8.jpg</t>
+  </si>
+  <si>
+    <t>Cyclops 97.jpg</t>
+  </si>
+  <si>
+    <t>Magneto 97.jpg</t>
+  </si>
+  <si>
+    <t>Jean 97.jpg</t>
+  </si>
+  <si>
+    <t>Wolverine 97.jpg</t>
+  </si>
+  <si>
+    <t>Beast 97.jpg</t>
+  </si>
+  <si>
+    <t>Storm 97.jpg</t>
+  </si>
+  <si>
+    <t>Wolverine full sleeve.jpg</t>
+  </si>
+  <si>
+    <t>Deadpool Gold gun.jpg</t>
+  </si>
+  <si>
+    <t>Warmachine new.jpg</t>
+  </si>
+  <si>
+    <t>Iron patriot new.jpg</t>
+  </si>
+  <si>
+    <t>Law wano (xinh).jpg</t>
+  </si>
+  <si>
+    <t>Sabo (xinh).jpg</t>
+  </si>
+  <si>
+    <t>Rayleigh (young).jpg</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1622,7 @@
         <v>200</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>183</v>
+        <v>285</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1617,7 +1656,7 @@
         <v>200</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>183</v>
+        <v>286</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -1634,7 +1673,7 @@
         <v>200</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>183</v>
+        <v>287</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1651,7 +1690,7 @@
         <v>200</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>183</v>
+        <v>288</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -1668,7 +1707,7 @@
         <v>200</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>183</v>
+        <v>289</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -1685,7 +1724,7 @@
         <v>200</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>183</v>
+        <v>290</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -1869,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>256</v>
@@ -1886,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>186</v>
@@ -1903,7 +1942,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>257</v>
@@ -1971,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>183</v>
+        <v>291</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -1988,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>183</v>
@@ -2005,10 +2044,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>183</v>
+        <v>292</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2161,7 +2200,7 @@
         <v>360</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2178,7 +2217,7 @@
         <v>360</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>183</v>
+        <v>294</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2804,7 +2843,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="3">
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>194</v>
@@ -3147,7 +3186,7 @@
         <v>300</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>183</v>
+        <v>295</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>67</v>
@@ -3181,7 +3220,7 @@
         <v>300</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>183</v>
+        <v>296</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>67</v>
@@ -3317,7 +3356,7 @@
         <v>300</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>183</v>
+        <v>297</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
price updated for geto
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD0169-F5E4-4A77-ABA8-B0E0CE2E1AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C50AC6-2EE6-4106-8108-BE4D3D17781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="1365" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4016,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="C151" s="3">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
multiverse & luffy g4 added
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FA1B4E-35E7-47AD-8121-074A61A3DF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B84E78-52EC-41B4-9918-EFA8CA765A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="3210" yWindow="1845" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="320">
   <si>
     <t>Product</t>
   </si>
@@ -952,6 +952,48 @@
   </si>
   <si>
     <t>Zoro Topless purple (dy)</t>
+  </si>
+  <si>
+    <t>Luffy G4 WM</t>
+  </si>
+  <si>
+    <t>Luffy G4 WM.jpg</t>
+  </si>
+  <si>
+    <t>Miles Morales</t>
+  </si>
+  <si>
+    <t>Spider-Gwen</t>
+  </si>
+  <si>
+    <t>Spiderman 2099</t>
+  </si>
+  <si>
+    <t>Spot (White)</t>
+  </si>
+  <si>
+    <t>Spider-Punk</t>
+  </si>
+  <si>
+    <t>Spiderman India</t>
+  </si>
+  <si>
+    <t>Miles morales.jpg</t>
+  </si>
+  <si>
+    <t>Spider-Gwen.jpg</t>
+  </si>
+  <si>
+    <t>Spider-Punk.jpg</t>
+  </si>
+  <si>
+    <t>Spiderman2099.jpg</t>
+  </si>
+  <si>
+    <t>Spot(white).jpg</t>
+  </si>
+  <si>
+    <t>Spiderman India.jpg</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,16 +1679,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>308</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
       </c>
       <c r="C10" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1654,16 +1696,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>309</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>177</v>
+        <v>315</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1671,16 +1713,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>310</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -1688,16 +1730,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>311</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>281</v>
+        <v>318</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1705,16 +1747,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>312</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -1722,16 +1764,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>313</v>
       </c>
       <c r="B15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -1739,16 +1781,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>200</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -1756,7 +1798,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -1773,16 +1815,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>200</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -1790,7 +1832,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -1799,7 +1841,7 @@
         <v>200</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>178</v>
+        <v>281</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -1807,16 +1849,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>179</v>
+        <v>282</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -1824,16 +1866,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
       <c r="C21" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>248</v>
+        <v>283</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -1841,16 +1883,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>177</v>
+        <v>284</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -1858,13 +1900,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
       </c>
       <c r="C23" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>177</v>
@@ -1875,16 +1917,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>177</v>
+        <v>246</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -1892,16 +1934,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>247</v>
+        <v>178</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -1909,16 +1951,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26" s="3">
         <v>180</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
@@ -1926,16 +1968,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
       </c>
       <c r="C27" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -1943,16 +1985,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -1960,16 +2002,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C29" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>251</v>
+        <v>177</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -1977,16 +2019,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="3">
-        <v>450</v>
+        <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>252</v>
+        <v>177</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -1994,16 +2036,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="3">
-        <v>380</v>
+        <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2011,16 +2053,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C32" s="3">
-        <v>800</v>
+        <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>184</v>
+        <v>249</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2028,16 +2070,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="3">
         <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2045,16 +2087,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="3">
         <v>270</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2062,7 +2104,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3">
         <v>2</v>
@@ -2071,7 +2113,7 @@
         <v>270</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2079,16 +2121,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="3">
-        <v>850</v>
+        <v>450</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2096,16 +2138,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="3">
-        <v>250</v>
+        <v>380</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -2113,16 +2155,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38" s="3">
-        <v>250</v>
+        <v>800</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>253</v>
+        <v>184</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2130,16 +2172,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2147,16 +2189,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C40" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>255</v>
+        <v>177</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -2164,16 +2206,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>181</v>
+        <v>286</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2181,16 +2223,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="3">
-        <v>250</v>
+        <v>850</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>238</v>
+        <v>183</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2198,16 +2240,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" s="3">
         <v>250</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2215,16 +2257,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
       </c>
       <c r="C44" s="3">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2232,16 +2274,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" s="3">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2249,16 +2291,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>256</v>
+        <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2266,118 +2308,118 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C47" s="3">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="3">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>177</v>
+        <v>238</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="3">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" s="3">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" s="3">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
       <c r="B52" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C52" s="3">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C53" s="3">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>51</v>
@@ -2385,16 +2427,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B54" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C54" s="3">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>241</v>
+        <v>177</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>51</v>
@@ -2402,16 +2444,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>242</v>
+        <v>177</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>51</v>
@@ -2419,16 +2461,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C56" s="3">
-        <v>500</v>
+        <v>160</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>51</v>
@@ -2436,16 +2478,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" s="3">
-        <v>350</v>
+        <v>160</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>51</v>
@@ -2453,16 +2495,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B58" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>51</v>
@@ -2470,16 +2512,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B59" s="3">
         <v>1</v>
       </c>
       <c r="C59" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>51</v>
@@ -2487,16 +2529,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B60" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60" s="3">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>51</v>
@@ -2504,16 +2546,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B61" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C61" s="3">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>51</v>
@@ -2521,118 +2563,118 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B62" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C62" s="3">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
       <c r="B63" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C63" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B64" s="3">
         <v>0</v>
       </c>
       <c r="C64" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B65" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B66" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="3">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B67" s="3">
         <v>0</v>
       </c>
       <c r="C67" s="3">
-        <v>270</v>
+        <v>500</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B68" s="3">
         <v>0</v>
       </c>
       <c r="C68" s="3">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>67</v>
@@ -2640,7 +2682,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
@@ -2649,7 +2691,7 @@
         <v>300</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>67</v>
@@ -2657,7 +2699,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B70" s="3">
         <v>0</v>
@@ -2666,7 +2708,7 @@
         <v>300</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>177</v>
+        <v>230</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>67</v>
@@ -2674,16 +2716,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B71" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" s="3">
         <v>300</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>67</v>
@@ -2691,16 +2733,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B72" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" s="3">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>67</v>
@@ -2708,16 +2750,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="C73" s="3">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>67</v>
@@ -2725,16 +2767,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B74" s="3">
         <v>0</v>
       </c>
       <c r="C74" s="3">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>67</v>
@@ -2742,16 +2784,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B75" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" s="3">
         <v>300</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>67</v>
@@ -2759,7 +2801,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B76" s="3">
         <v>0</v>
@@ -2776,16 +2818,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B77" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" s="3">
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>67</v>
@@ -2793,16 +2835,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B78" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C78" s="3">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>67</v>
@@ -2810,7 +2852,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B79" s="3">
         <v>0</v>
@@ -2819,7 +2861,7 @@
         <v>300</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>67</v>
@@ -2827,7 +2869,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B80" s="3">
         <v>0</v>
@@ -2844,16 +2886,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>85</v>
+        <v>306</v>
       </c>
       <c r="B81" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C81" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>193</v>
+        <v>307</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>67</v>
@@ -2861,16 +2903,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>304</v>
+        <v>79</v>
       </c>
       <c r="B82" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C82" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>67</v>
@@ -2878,16 +2920,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>305</v>
+        <v>80</v>
       </c>
       <c r="B83" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>67</v>
@@ -2895,16 +2937,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B84" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C84" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>67</v>
@@ -2912,16 +2954,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B85" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>67</v>
@@ -2929,16 +2971,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B86" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C86" s="3">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>67</v>
@@ -2946,16 +2988,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B87" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" s="3">
-        <v>320</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>197</v>
+        <v>300</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>67</v>
@@ -2963,16 +3005,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
       </c>
       <c r="C88" s="3">
-        <v>320</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>210</v>
+        <v>300</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>67</v>
@@ -2980,16 +3022,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>304</v>
       </c>
       <c r="B89" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C89" s="3">
-        <v>320</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>198</v>
+        <v>350</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>67</v>
@@ -2997,16 +3039,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>92</v>
+        <v>305</v>
       </c>
       <c r="B90" s="3">
         <v>1</v>
       </c>
       <c r="C90" s="3">
-        <v>320</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>199</v>
+        <v>350</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>67</v>
@@ -3014,16 +3056,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B91" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C91" s="3">
-        <v>320</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>200</v>
+        <v>350</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>67</v>
@@ -3031,16 +3073,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B92" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C92" s="3">
-        <v>320</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>201</v>
+        <v>350</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>67</v>
@@ -3048,16 +3090,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B93" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C93" s="3">
         <v>320</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>202</v>
+      <c r="D93" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>67</v>
@@ -3065,7 +3107,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B94" s="3">
         <v>1</v>
@@ -3074,7 +3116,7 @@
         <v>320</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>67</v>
@@ -3082,7 +3124,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B95" s="3">
         <v>1</v>
@@ -3091,7 +3133,7 @@
         <v>320</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>67</v>
@@ -3099,16 +3141,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B96" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C96" s="3">
         <v>320</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>67</v>
@@ -3116,16 +3158,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B97" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="3">
         <v>320</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>67</v>
@@ -3133,7 +3175,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
@@ -3142,7 +3184,7 @@
         <v>320</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>67</v>
@@ -3150,7 +3192,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B99" s="3">
         <v>2</v>
@@ -3159,7 +3201,7 @@
         <v>320</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>67</v>
@@ -3167,7 +3209,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B100" s="3">
         <v>0</v>
@@ -3176,7 +3218,7 @@
         <v>320</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>67</v>
@@ -3184,16 +3226,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B101" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" s="3">
-        <v>300</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>177</v>
+        <v>320</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>67</v>
@@ -3201,16 +3243,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B102" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C102" s="3">
-        <v>300</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>289</v>
+        <v>320</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>67</v>
@@ -3218,16 +3260,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B103" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C103" s="3">
-        <v>300</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>261</v>
+        <v>320</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>67</v>
@@ -3235,16 +3277,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B104" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C104" s="3">
-        <v>300</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>290</v>
+        <v>320</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>67</v>
@@ -3252,16 +3294,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B105" s="3">
         <v>1</v>
       </c>
       <c r="C105" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>67</v>
@@ -3269,16 +3311,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B106" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C106" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>67</v>
@@ -3286,16 +3328,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B107" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>67</v>
@@ -3303,16 +3345,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B108" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" s="3">
         <v>300</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>234</v>
+      <c r="D108" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>67</v>
@@ -3320,7 +3362,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B109" s="3">
         <v>2</v>
@@ -3328,8 +3370,8 @@
       <c r="C109" s="3">
         <v>300</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>235</v>
+      <c r="D109" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>67</v>
@@ -3337,16 +3379,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B110" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110" s="3">
         <v>300</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>236</v>
+      <c r="D110" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>67</v>
@@ -3354,7 +3396,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
@@ -3362,8 +3404,8 @@
       <c r="C111" s="3">
         <v>300</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>237</v>
+      <c r="D111" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>67</v>
@@ -3371,7 +3413,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B112" s="3">
         <v>1</v>
@@ -3379,8 +3421,8 @@
       <c r="C112" s="3">
         <v>300</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>291</v>
+      <c r="D112" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>67</v>
@@ -3388,16 +3430,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B113" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113" s="3">
-        <v>400</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>262</v>
+        <v>300</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>67</v>
@@ -3405,16 +3447,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B114" s="3">
         <v>1</v>
       </c>
       <c r="C114" s="3">
-        <v>400</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>263</v>
+        <v>300</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>67</v>
@@ -3422,16 +3464,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B115" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" s="3">
         <v>300</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>264</v>
+      <c r="D115" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>67</v>
@@ -3439,7 +3481,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B116" s="3">
         <v>2</v>
@@ -3447,8 +3489,8 @@
       <c r="C116" s="3">
         <v>300</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>265</v>
+      <c r="D116" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>67</v>
@@ -3456,16 +3498,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B117" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C117" s="3">
         <v>300</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>266</v>
+      <c r="D117" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>67</v>
@@ -3473,7 +3515,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B118" s="3">
         <v>1</v>
@@ -3481,8 +3523,8 @@
       <c r="C118" s="3">
         <v>300</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>267</v>
+      <c r="D118" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>67</v>
@@ -3490,7 +3532,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B119" s="3">
         <v>1</v>
@@ -3499,7 +3541,7 @@
         <v>300</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>67</v>
@@ -3507,16 +3549,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B120" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C120" s="3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>67</v>
@@ -3524,16 +3566,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B121" s="3">
         <v>1</v>
       </c>
       <c r="C121" s="3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>67</v>
@@ -3541,16 +3583,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B122" s="3">
         <v>0</v>
       </c>
       <c r="C122" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>67</v>
@@ -3558,16 +3600,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B123" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C123" s="3">
         <v>300</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>67</v>
@@ -3575,7 +3617,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B124" s="3">
         <v>1</v>
@@ -3584,7 +3626,7 @@
         <v>300</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>67</v>
@@ -3592,75 +3634,75 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B125" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C125" s="3">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
       </c>
       <c r="C126" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
       </c>
       <c r="C127" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B128" s="3">
         <v>1</v>
       </c>
       <c r="C128" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B129" s="3">
         <v>0</v>
@@ -3669,58 +3711,58 @@
         <v>500</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>177</v>
+        <v>271</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B130" s="3">
         <v>1</v>
       </c>
       <c r="C130" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B131" s="3">
         <v>1</v>
       </c>
       <c r="C131" s="3">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B132" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C132" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>177</v>
+        <v>292</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>128</v>
@@ -3728,16 +3770,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B133" s="3">
         <v>1</v>
       </c>
       <c r="C133" s="3">
-        <v>220</v>
+        <v>500</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>177</v>
+        <v>293</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>128</v>
@@ -3745,16 +3787,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B134" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134" s="3">
-        <v>220</v>
+        <v>500</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>177</v>
+        <v>294</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>128</v>
@@ -3762,16 +3804,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B135" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135" s="3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>128</v>
@@ -3779,13 +3821,13 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B136" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" s="3">
-        <v>220</v>
+        <v>500</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>177</v>
@@ -3796,16 +3838,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>297</v>
+        <v>133</v>
       </c>
       <c r="B137" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137" s="3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>296</v>
+        <v>245</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>128</v>
@@ -3813,16 +3855,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>298</v>
+        <v>134</v>
       </c>
       <c r="B138" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C138" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>299</v>
+        <v>177</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>128</v>
@@ -3830,16 +3872,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>301</v>
+        <v>135</v>
       </c>
       <c r="B139" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C139" s="3">
         <v>220</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>300</v>
+        <v>177</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>128</v>
@@ -3847,13 +3889,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B140" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C140" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>177</v>
@@ -3864,16 +3906,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>302</v>
+        <v>137</v>
       </c>
       <c r="B141" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C141" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>303</v>
+        <v>177</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>128</v>
@@ -3881,13 +3923,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B142" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C142" s="3">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>177</v>
@@ -3898,13 +3940,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B143" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C143" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>177</v>
@@ -3915,16 +3957,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>143</v>
+        <v>297</v>
       </c>
       <c r="B144" s="3">
         <v>2</v>
       </c>
       <c r="C144" s="3">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>177</v>
+        <v>296</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>128</v>
@@ -3932,16 +3974,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>144</v>
+        <v>298</v>
       </c>
       <c r="B145" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C145" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>177</v>
+        <v>299</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>128</v>
@@ -3949,16 +3991,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>145</v>
+        <v>301</v>
       </c>
       <c r="B146" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C146" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>177</v>
+        <v>300</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>128</v>
@@ -3966,13 +4008,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B147" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C147" s="3">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>177</v>
@@ -3983,16 +4025,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>147</v>
+        <v>302</v>
       </c>
       <c r="B148" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C148" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>177</v>
+        <v>303</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>128</v>
@@ -4000,13 +4042,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B149" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C149" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>177</v>
@@ -4017,13 +4059,13 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B150" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C150" s="3">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>177</v>
@@ -4034,126 +4076,126 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B151" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C151" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>274</v>
+        <v>177</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B152" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C152" s="3">
-        <v>460</v>
+        <v>350</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B153" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C153" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>275</v>
+        <v>177</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B154" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C154" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>276</v>
+        <v>177</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B155" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C155" s="3">
-        <v>240</v>
+        <v>350</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B156" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C156" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B157" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C157" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
@@ -4162,86 +4204,86 @@
         <v>250</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>177</v>
+        <v>274</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B159" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="3">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B160" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C160" s="3">
         <v>250</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>177</v>
+        <v>275</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B161" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C161" s="3">
         <v>250</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>177</v>
+        <v>276</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B162" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162" s="3">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B163" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C163" s="3">
         <v>250</v>
@@ -4255,10 +4297,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B164" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C164" s="3">
         <v>250</v>
@@ -4272,7 +4314,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B165" s="3">
         <v>1</v>
@@ -4289,7 +4331,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B166" s="3">
         <v>1</v>
@@ -4306,7 +4348,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B167" s="3">
         <v>2</v>
@@ -4323,10 +4365,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B168" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C168" s="3">
         <v>250</v>
@@ -4340,10 +4382,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B169" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C169" s="3">
         <v>250</v>
@@ -4357,10 +4399,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B170" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C170" s="3">
         <v>250</v>
@@ -4374,10 +4416,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B171" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C171" s="3">
         <v>250</v>
@@ -4391,26 +4433,26 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B172" s="5">
-        <v>7</v>
+        <v>166</v>
+      </c>
+      <c r="B172" s="3">
+        <v>1</v>
       </c>
       <c r="C172" s="3">
         <v>250</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E172" s="6" t="s">
-        <v>223</v>
+        <v>177</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>216</v>
-      </c>
-      <c r="B173" s="5">
+      <c r="A173" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B173" s="3">
         <v>1</v>
       </c>
       <c r="C173" s="3">
@@ -4419,109 +4461,228 @@
       <c r="D173" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E173" s="6" t="s">
+      <c r="E173" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B174" s="3">
+        <v>2</v>
+      </c>
+      <c r="C174" s="3">
+        <v>250</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B175" s="3">
+        <v>1</v>
+      </c>
+      <c r="C175" s="3">
+        <v>250</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B176" s="3">
+        <v>2</v>
+      </c>
+      <c r="C176" s="3">
+        <v>250</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B177" s="3">
+        <v>1</v>
+      </c>
+      <c r="C177" s="3">
+        <v>250</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B178" s="3">
+        <v>1</v>
+      </c>
+      <c r="C178" s="3">
+        <v>250</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B179" s="5">
+        <v>7</v>
+      </c>
+      <c r="C179" s="3">
+        <v>250</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E179" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>216</v>
+      </c>
+      <c r="B180" s="5">
+        <v>1</v>
+      </c>
+      <c r="C180" s="3">
+        <v>250</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>217</v>
       </c>
-      <c r="B174" s="5">
-        <v>1</v>
-      </c>
-      <c r="C174" s="6">
+      <c r="B181" s="5">
+        <v>1</v>
+      </c>
+      <c r="C181" s="6">
         <v>220</v>
       </c>
-      <c r="D174" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E174" s="6" t="s">
+      <c r="D181" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E181" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>218</v>
       </c>
-      <c r="B175" s="5">
-        <v>1</v>
-      </c>
-      <c r="C175" s="6">
+      <c r="B182" s="5">
+        <v>1</v>
+      </c>
+      <c r="C182" s="6">
         <v>220</v>
       </c>
-      <c r="D175" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E175" s="6" t="s">
+      <c r="D182" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E182" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>219</v>
       </c>
-      <c r="B176" s="5">
+      <c r="B183" s="5">
         <v>2</v>
       </c>
-      <c r="C176" s="6">
+      <c r="C183" s="6">
         <v>220</v>
       </c>
-      <c r="D176" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E176" s="6" t="s">
+      <c r="D183" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E183" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>220</v>
       </c>
-      <c r="B177" s="5">
-        <v>1</v>
-      </c>
-      <c r="C177" s="6">
+      <c r="B184" s="5">
+        <v>1</v>
+      </c>
+      <c r="C184" s="6">
         <v>220</v>
       </c>
-      <c r="D177" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E177" s="6" t="s">
+      <c r="D184" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E184" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>221</v>
       </c>
-      <c r="B178" s="5">
-        <v>1</v>
-      </c>
-      <c r="C178" s="6">
+      <c r="B185" s="5">
+        <v>1</v>
+      </c>
+      <c r="C185" s="6">
         <v>220</v>
       </c>
-      <c r="D178" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E178" s="6" t="s">
+      <c r="D185" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E185" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>222</v>
       </c>
-      <c r="B179" s="5">
+      <c r="B186" s="5">
         <v>5</v>
       </c>
-      <c r="C179" s="6">
+      <c r="C186" s="6">
         <v>350</v>
       </c>
-      <c r="D179" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E179" s="6" t="s">
+      <c r="E186" s="6" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
naruto stock and image update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B84E78-52EC-41B4-9918-EFA8CA765A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B2DF25-3CA9-46CE-A057-166450C20D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="1845" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="3840" yWindow="990" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="334">
   <si>
     <t>Product</t>
   </si>
@@ -994,6 +994,48 @@
   </si>
   <si>
     <t>Spiderman India.jpg</t>
+  </si>
+  <si>
+    <t>sasuke sus.jpg</t>
+  </si>
+  <si>
+    <t>madara sus.jpg</t>
+  </si>
+  <si>
+    <t>kakashi sus.jpg</t>
+  </si>
+  <si>
+    <t>shisui sus.jpg</t>
+  </si>
+  <si>
+    <t>itachi sus.jpg</t>
+  </si>
+  <si>
+    <t>hagoromo sus.jpg</t>
+  </si>
+  <si>
+    <t>kakashi cape.jpg</t>
+  </si>
+  <si>
+    <t>madara six path.jpg</t>
+  </si>
+  <si>
+    <t>madara.jpg</t>
+  </si>
+  <si>
+    <t>minato.jpg</t>
+  </si>
+  <si>
+    <t>sasuke.jpg</t>
+  </si>
+  <si>
+    <t>obito akatsuki.jpg</t>
+  </si>
+  <si>
+    <t>obito war.jpg</t>
+  </si>
+  <si>
+    <t>obito six path.jpg</t>
   </si>
 </sst>
 </file>
@@ -1513,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,10 +2880,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="3">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>213</v>
@@ -2889,7 +2931,7 @@
         <v>306</v>
       </c>
       <c r="B81" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" s="3">
         <v>350</v>
@@ -3756,7 +3798,7 @@
         <v>127</v>
       </c>
       <c r="B132" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132" s="3">
         <v>250</v>
@@ -3858,13 +3900,13 @@
         <v>134</v>
       </c>
       <c r="B138" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" s="3">
         <v>220</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>177</v>
+        <v>326</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>128</v>
@@ -3881,7 +3923,7 @@
         <v>220</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>177</v>
+        <v>333</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>128</v>
@@ -3898,7 +3940,7 @@
         <v>220</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>177</v>
+        <v>327</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>128</v>
@@ -3915,7 +3957,7 @@
         <v>220</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>177</v>
+        <v>328</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>128</v>
@@ -3929,10 +3971,10 @@
         <v>2</v>
       </c>
       <c r="C142" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>177</v>
+        <v>329</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>128</v>
@@ -3946,10 +3988,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>177</v>
+        <v>330</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>128</v>
@@ -3963,7 +4005,7 @@
         <v>2</v>
       </c>
       <c r="C144" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>296</v>
@@ -4014,10 +4056,10 @@
         <v>3</v>
       </c>
       <c r="C147" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>177</v>
+        <v>332</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>128</v>
@@ -4028,7 +4070,7 @@
         <v>302</v>
       </c>
       <c r="B148" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" s="3">
         <v>250</v>
@@ -4051,7 +4093,7 @@
         <v>220</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>128</v>
@@ -4085,7 +4127,7 @@
         <v>350</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>177</v>
+        <v>320</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>128</v>
@@ -4102,7 +4144,7 @@
         <v>350</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>177</v>
+        <v>321</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>128</v>
@@ -4119,7 +4161,7 @@
         <v>350</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>177</v>
+        <v>322</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>128</v>
@@ -4136,7 +4178,7 @@
         <v>350</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>177</v>
+        <v>323</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>128</v>
@@ -4153,7 +4195,7 @@
         <v>350</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>177</v>
+        <v>324</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>128</v>
@@ -4170,7 +4212,7 @@
         <v>350</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>177</v>
+        <v>325</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>128</v>
@@ -4521,7 +4563,7 @@
         <v>171</v>
       </c>
       <c r="B177" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177" s="3">
         <v>250</v>
@@ -4538,7 +4580,7 @@
         <v>172</v>
       </c>
       <c r="B178" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" s="3">
         <v>250</v>

</xml_diff>

<commit_message>
nrauto kid image updated
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B2DF25-3CA9-46CE-A057-166450C20D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD80D47-31A1-4E88-B5CA-B0B9DF18EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="990" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="4170" yWindow="1395" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="335">
   <si>
     <t>Product</t>
   </si>
@@ -1036,6 +1036,9 @@
   </si>
   <si>
     <t>obito six path.jpg</t>
+  </si>
+  <si>
+    <t>naruto kid.jpg</t>
   </si>
 </sst>
 </file>
@@ -1555,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4229,7 +4232,7 @@
         <v>220</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>177</v>
+        <v>334</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
stock update + others and naruto img update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD80D47-31A1-4E88-B5CA-B0B9DF18EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6DE697-B3C4-4C46-A3A1-15745B3961E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1395" windowWidth="21600" windowHeight="11295" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="4170" yWindow="1440" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="342">
   <si>
     <t>Product</t>
   </si>
@@ -159,33 +159,12 @@
     <t>Rhino</t>
   </si>
   <si>
-    <t>Moonknight moon white</t>
-  </si>
-  <si>
-    <t>Moonknight white</t>
-  </si>
-  <si>
     <t>Mr. Moonknight</t>
   </si>
   <si>
     <t>Dr. Strange Supreme</t>
   </si>
   <si>
-    <t>Shang chi</t>
-  </si>
-  <si>
-    <t>Moonknight black</t>
-  </si>
-  <si>
-    <t>Moonknight black comic</t>
-  </si>
-  <si>
-    <t>War Machine new</t>
-  </si>
-  <si>
-    <t>Iron Patriot new</t>
-  </si>
-  <si>
     <t>Joker</t>
   </si>
   <si>
@@ -201,12 +180,6 @@
     <t>Superman</t>
   </si>
   <si>
-    <t>Black Adam hood</t>
-  </si>
-  <si>
-    <t>Black Adam bald</t>
-  </si>
-  <si>
     <t>Dr. Fate Cape</t>
   </si>
   <si>
@@ -423,21 +396,9 @@
     <t>Naruto</t>
   </si>
   <si>
-    <t>boruto &amp; sarada</t>
-  </si>
-  <si>
-    <t>Sasuke &amp; Baryon</t>
-  </si>
-  <si>
-    <t>Baryon &amp; Boruto</t>
-  </si>
-  <si>
     <t>Marriage set</t>
   </si>
   <si>
-    <t>Sasuke &amp; Naruto(war)</t>
-  </si>
-  <si>
     <t>Kakashi cape</t>
   </si>
   <si>
@@ -690,9 +651,6 @@
     <t>Getsuga Ichigo</t>
   </si>
   <si>
-    <t>vasto Ichigo</t>
-  </si>
-  <si>
     <t>Aizen</t>
   </si>
   <si>
@@ -771,9 +729,6 @@
     <t>Hawkeye.jpeg</t>
   </si>
   <si>
-    <t>Sasuke &amp; Naruto(war).png</t>
-  </si>
-  <si>
     <t>Wolverine.png</t>
   </si>
   <si>
@@ -915,15 +870,6 @@
     <t>Naruto sage.jpg</t>
   </si>
   <si>
-    <t>borusara.jpg</t>
-  </si>
-  <si>
-    <t>barsas.jpg</t>
-  </si>
-  <si>
-    <t>barboru.jpg</t>
-  </si>
-  <si>
     <t>Jiraya kdl.jpg</t>
   </si>
   <si>
@@ -1039,6 +985,81 @@
   </si>
   <si>
     <t>naruto kid.jpg</t>
+  </si>
+  <si>
+    <t>Naruto Baryon</t>
+  </si>
+  <si>
+    <t>Sasuke (Adult)</t>
+  </si>
+  <si>
+    <t>Boruto</t>
+  </si>
+  <si>
+    <t>Sarada</t>
+  </si>
+  <si>
+    <t>Naruto(war)</t>
+  </si>
+  <si>
+    <t>Moonknight Moon White</t>
+  </si>
+  <si>
+    <t>Moonknight White</t>
+  </si>
+  <si>
+    <t>Moonknight Black</t>
+  </si>
+  <si>
+    <t>Shang Chi</t>
+  </si>
+  <si>
+    <t>Moonknight Black Comic</t>
+  </si>
+  <si>
+    <t>War Machine New</t>
+  </si>
+  <si>
+    <t>Iron Patriot New</t>
+  </si>
+  <si>
+    <t>Black Adam Hood</t>
+  </si>
+  <si>
+    <t>Black Adam Bald</t>
+  </si>
+  <si>
+    <t>Vasto Ichigo</t>
+  </si>
+  <si>
+    <t>winston.jpg</t>
+  </si>
+  <si>
+    <t>ichigo.jpg</t>
+  </si>
+  <si>
+    <t>aizen.jpg</t>
+  </si>
+  <si>
+    <t>Kenpachi.jpg</t>
+  </si>
+  <si>
+    <t>jaeger.jpg</t>
+  </si>
+  <si>
+    <t>naruto bar.jpg</t>
+  </si>
+  <si>
+    <t>sasuke adult.jpg</t>
+  </si>
+  <si>
+    <t>boruto.jpg</t>
+  </si>
+  <si>
+    <t>sarada.jpg</t>
+  </si>
+  <si>
+    <t>naruto war.jpg</t>
   </si>
 </sst>
 </file>
@@ -1556,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1618,7 @@
         <v>220</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -1614,7 +1635,7 @@
         <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -1631,7 +1652,7 @@
         <v>350</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1648,7 +1669,7 @@
         <v>180</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
@@ -1665,7 +1686,7 @@
         <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
@@ -1682,7 +1703,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -1699,7 +1720,7 @@
         <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -1716,7 +1737,7 @@
         <v>200</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
@@ -1724,7 +1745,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -1733,7 +1754,7 @@
         <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1741,7 +1762,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1750,7 +1771,7 @@
         <v>280</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1758,7 +1779,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -1767,7 +1788,7 @@
         <v>280</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -1775,7 +1796,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1784,7 +1805,7 @@
         <v>280</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1792,7 +1813,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -1801,7 +1822,7 @@
         <v>280</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -1809,7 +1830,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -1818,7 +1839,7 @@
         <v>280</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -1835,7 +1856,7 @@
         <v>200</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -1852,7 +1873,7 @@
         <v>200</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
@@ -1869,7 +1890,7 @@
         <v>200</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -1886,7 +1907,7 @@
         <v>200</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -1903,7 +1924,7 @@
         <v>200</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -1920,7 +1941,7 @@
         <v>200</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -1937,7 +1958,7 @@
         <v>200</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -1954,7 +1975,7 @@
         <v>200</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -1971,7 +1992,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -1985,10 +2006,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -2005,7 +2026,7 @@
         <v>180</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
@@ -2022,7 +2043,7 @@
         <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2039,7 +2060,7 @@
         <v>180</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -2056,7 +2077,7 @@
         <v>180</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -2073,7 +2094,7 @@
         <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -2090,7 +2111,7 @@
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2107,7 +2128,7 @@
         <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2124,7 +2145,7 @@
         <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2141,7 +2162,7 @@
         <v>270</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2158,7 +2179,7 @@
         <v>270</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2175,7 +2196,7 @@
         <v>450</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2192,7 +2213,7 @@
         <v>380</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -2209,7 +2230,7 @@
         <v>800</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2226,7 +2247,7 @@
         <v>270</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2243,7 +2264,7 @@
         <v>270</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -2260,7 +2281,7 @@
         <v>270</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2277,7 +2298,7 @@
         <v>850</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2285,7 +2306,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>322</v>
       </c>
       <c r="B43" s="3">
         <v>2</v>
@@ -2294,7 +2315,7 @@
         <v>250</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2302,7 +2323,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>323</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
@@ -2311,7 +2332,7 @@
         <v>250</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2319,7 +2340,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" s="3">
         <v>2</v>
@@ -2328,7 +2349,7 @@
         <v>250</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2336,16 +2357,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" s="3">
         <v>250</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2353,7 +2374,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
@@ -2362,7 +2383,7 @@
         <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -2370,7 +2391,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>324</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
@@ -2379,7 +2400,7 @@
         <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -2387,7 +2408,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>326</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -2396,7 +2417,7 @@
         <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -2404,7 +2425,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>327</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -2413,7 +2434,7 @@
         <v>360</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -2421,7 +2442,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>328</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -2430,7 +2451,7 @@
         <v>360</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -2438,7 +2459,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -2447,7 +2468,7 @@
         <v>200</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -2455,7 +2476,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B53" s="3">
         <v>4</v>
@@ -2464,15 +2485,15 @@
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B54" s="3">
         <v>0</v>
@@ -2481,15 +2502,15 @@
         <v>150</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B55" s="3">
         <v>0</v>
@@ -2498,15 +2519,15 @@
         <v>180</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>329</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
@@ -2515,15 +2536,15 @@
         <v>160</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>330</v>
       </c>
       <c r="B57" s="3">
         <v>2</v>
@@ -2532,15 +2553,15 @@
         <v>160</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B58" s="3">
         <v>4</v>
@@ -2549,32 +2570,32 @@
         <v>300</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B59" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" s="3">
         <v>300</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B60" s="3">
         <v>2</v>
@@ -2583,15 +2604,15 @@
         <v>350</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B61" s="3">
         <v>3</v>
@@ -2600,15 +2621,15 @@
         <v>350</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B62" s="3">
         <v>4</v>
@@ -2617,15 +2638,15 @@
         <v>500</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B63" s="3">
         <v>3</v>
@@ -2634,15 +2655,15 @@
         <v>350</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B64" s="3">
         <v>0</v>
@@ -2651,15 +2672,15 @@
         <v>350</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B65" s="3">
         <v>1</v>
@@ -2668,15 +2689,15 @@
         <v>350</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B66" s="3">
         <v>0</v>
@@ -2685,15 +2706,15 @@
         <v>500</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B67" s="3">
         <v>0</v>
@@ -2702,15 +2723,15 @@
         <v>500</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B68" s="3">
         <v>0</v>
@@ -2719,15 +2740,15 @@
         <v>300</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
@@ -2736,15 +2757,15 @@
         <v>300</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B70" s="3">
         <v>0</v>
@@ -2753,15 +2774,15 @@
         <v>300</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B71" s="3">
         <v>0</v>
@@ -2770,15 +2791,15 @@
         <v>300</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B72" s="3">
         <v>1</v>
@@ -2787,15 +2808,15 @@
         <v>300</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
@@ -2804,15 +2825,15 @@
         <v>270</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B74" s="3">
         <v>0</v>
@@ -2821,15 +2842,15 @@
         <v>270</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B75" s="3">
         <v>1</v>
@@ -2838,15 +2859,15 @@
         <v>300</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B76" s="3">
         <v>0</v>
@@ -2855,15 +2876,15 @@
         <v>300</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B77" s="3">
         <v>1</v>
@@ -2872,15 +2893,15 @@
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
@@ -2889,15 +2910,15 @@
         <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B79" s="3">
         <v>0</v>
@@ -2906,15 +2927,15 @@
         <v>300</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B80" s="3">
         <v>0</v>
@@ -2923,15 +2944,15 @@
         <v>300</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="B81" s="3">
         <v>2</v>
@@ -2940,15 +2961,15 @@
         <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B82" s="3">
         <v>0</v>
@@ -2957,15 +2978,15 @@
         <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B83" s="3">
         <v>0</v>
@@ -2974,15 +2995,15 @@
         <v>300</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B84" s="3">
         <v>0</v>
@@ -2991,15 +3012,15 @@
         <v>300</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B85" s="3">
         <v>0</v>
@@ -3008,15 +3029,15 @@
         <v>300</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B86" s="3">
         <v>0</v>
@@ -3025,15 +3046,15 @@
         <v>300</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B87" s="3">
         <v>0</v>
@@ -3042,15 +3063,15 @@
         <v>300</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
@@ -3059,32 +3080,32 @@
         <v>300</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="B89" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="3">
         <v>350</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="B90" s="3">
         <v>1</v>
@@ -3093,15 +3114,15 @@
         <v>350</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B91" s="3">
         <v>2</v>
@@ -3110,15 +3131,15 @@
         <v>350</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B92" s="3">
         <v>1</v>
@@ -3127,15 +3148,15 @@
         <v>350</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B93" s="3">
         <v>2</v>
@@ -3144,15 +3165,15 @@
         <v>320</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B94" s="3">
         <v>1</v>
@@ -3161,15 +3182,15 @@
         <v>320</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B95" s="3">
         <v>1</v>
@@ -3178,15 +3199,15 @@
         <v>320</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B96" s="3">
         <v>1</v>
@@ -3195,15 +3216,15 @@
         <v>320</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B97" s="3">
         <v>1</v>
@@ -3212,15 +3233,15 @@
         <v>320</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
@@ -3229,15 +3250,15 @@
         <v>320</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B99" s="3">
         <v>2</v>
@@ -3246,15 +3267,15 @@
         <v>320</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B100" s="3">
         <v>0</v>
@@ -3263,15 +3284,15 @@
         <v>320</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B101" s="3">
         <v>1</v>
@@ -3280,15 +3301,15 @@
         <v>320</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B102" s="3">
         <v>1</v>
@@ -3297,15 +3318,15 @@
         <v>320</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B103" s="3">
         <v>2</v>
@@ -3314,15 +3335,15 @@
         <v>320</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B104" s="3">
         <v>2</v>
@@ -3331,15 +3352,15 @@
         <v>320</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B105" s="3">
         <v>1</v>
@@ -3348,15 +3369,15 @@
         <v>320</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B106" s="3">
         <v>2</v>
@@ -3365,15 +3386,15 @@
         <v>320</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B107" s="3">
         <v>0</v>
@@ -3382,15 +3403,15 @@
         <v>320</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B108" s="3">
         <v>0</v>
@@ -3399,15 +3420,15 @@
         <v>300</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B109" s="3">
         <v>2</v>
@@ -3416,15 +3437,15 @@
         <v>300</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B110" s="3">
         <v>1</v>
@@ -3433,15 +3454,15 @@
         <v>300</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
@@ -3450,15 +3471,15 @@
         <v>300</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B112" s="3">
         <v>1</v>
@@ -3467,15 +3488,15 @@
         <v>300</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
@@ -3484,15 +3505,15 @@
         <v>300</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B114" s="3">
         <v>1</v>
@@ -3501,15 +3522,15 @@
         <v>300</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B115" s="3">
         <v>1</v>
@@ -3518,32 +3539,32 @@
         <v>300</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B116" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C116" s="3">
         <v>300</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B117" s="3">
         <v>2</v>
@@ -3552,15 +3573,15 @@
         <v>300</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B118" s="3">
         <v>1</v>
@@ -3569,15 +3590,15 @@
         <v>300</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B119" s="3">
         <v>1</v>
@@ -3586,15 +3607,15 @@
         <v>300</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B120" s="3">
         <v>0</v>
@@ -3603,15 +3624,15 @@
         <v>400</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B121" s="3">
         <v>1</v>
@@ -3620,15 +3641,15 @@
         <v>400</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B122" s="3">
         <v>0</v>
@@ -3637,15 +3658,15 @@
         <v>300</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B123" s="3">
         <v>2</v>
@@ -3654,15 +3675,15 @@
         <v>300</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B124" s="3">
         <v>1</v>
@@ -3671,15 +3692,15 @@
         <v>300</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B125" s="3">
         <v>1</v>
@@ -3688,15 +3709,15 @@
         <v>300</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
@@ -3705,15 +3726,15 @@
         <v>300</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -3722,15 +3743,15 @@
         <v>300</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B128" s="3">
         <v>1</v>
@@ -3739,15 +3760,15 @@
         <v>300</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B129" s="3">
         <v>0</v>
@@ -3756,15 +3777,15 @@
         <v>500</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B130" s="3">
         <v>1</v>
@@ -3773,15 +3794,15 @@
         <v>300</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B131" s="3">
         <v>1</v>
@@ -3790,15 +3811,15 @@
         <v>300</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B132" s="3">
         <v>1</v>
@@ -3807,389 +3828,389 @@
         <v>250</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>129</v>
+        <v>317</v>
       </c>
       <c r="B133" s="3">
         <v>1</v>
       </c>
       <c r="C133" s="3">
-        <v>500</v>
+        <v>280</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>293</v>
+        <v>337</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>130</v>
+        <v>318</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
       </c>
       <c r="C134" s="3">
-        <v>500</v>
+        <v>280</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>294</v>
+        <v>338</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>131</v>
+        <v>319</v>
       </c>
       <c r="B135" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135" s="3">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>295</v>
+        <v>339</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>132</v>
+        <v>320</v>
       </c>
       <c r="B136" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C136" s="3">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>177</v>
+        <v>340</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B137" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" s="3">
         <v>500</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>245</v>
+        <v>164</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>134</v>
+        <v>321</v>
       </c>
       <c r="B138" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C138" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B139" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C139" s="3">
         <v>220</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B140" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C140" s="3">
         <v>220</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B141" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C141" s="3">
         <v>220</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B142" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142" s="3">
         <v>220</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C143" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>297</v>
+        <v>126</v>
       </c>
       <c r="B144" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C144" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="B145" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C145" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="B146" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C146" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>140</v>
+        <v>283</v>
       </c>
       <c r="B147" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C147" s="3">
         <v>220</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>302</v>
+        <v>127</v>
       </c>
       <c r="B148" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>141</v>
+        <v>284</v>
       </c>
       <c r="B149" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C149" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>331</v>
+        <v>285</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B150" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C150" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>177</v>
+        <v>313</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B151" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C151" s="3">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>320</v>
+        <v>164</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B152" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C152" s="3">
         <v>350</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B153" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C153" s="3">
         <v>350</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B154" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" s="3">
         <v>350</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B155" s="3">
         <v>1</v>
@@ -4198,151 +4219,151 @@
         <v>350</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B156" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C156" s="3">
         <v>350</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B157" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C157" s="3">
-        <v>220</v>
+        <v>350</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
       </c>
       <c r="C158" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B159" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C159" s="3">
-        <v>460</v>
+        <v>250</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B160" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C160" s="3">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>275</v>
+        <v>164</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B161" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C161" s="3">
         <v>250</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B162" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C162" s="3">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>177</v>
+        <v>261</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B163" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C163" s="3">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B164" s="3">
         <v>3</v>
@@ -4351,32 +4372,32 @@
         <v>250</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B165" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C165" s="3">
         <v>250</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B166" s="3">
         <v>1</v>
@@ -4385,32 +4406,32 @@
         <v>250</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B167" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C167" s="3">
         <v>250</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B168" s="3">
         <v>2</v>
@@ -4419,83 +4440,83 @@
         <v>250</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B169" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C169" s="3">
         <v>250</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B170" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170" s="3">
         <v>250</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B171" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C171" s="3">
         <v>250</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B172" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C172" s="3">
         <v>250</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B173" s="3">
         <v>1</v>
@@ -4504,83 +4525,83 @@
         <v>250</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B174" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C174" s="3">
         <v>250</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B175" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C175" s="3">
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B176" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C176" s="3">
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B177" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C177" s="3">
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B178" s="3">
         <v>0</v>
@@ -4589,66 +4610,66 @@
         <v>250</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B179" s="5">
-        <v>7</v>
+        <v>159</v>
+      </c>
+      <c r="B179" s="3">
+        <v>0</v>
       </c>
       <c r="C179" s="3">
         <v>250</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E179" s="6" t="s">
-        <v>223</v>
+        <v>164</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>216</v>
+      <c r="A180" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B180" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C180" s="3">
         <v>250</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>177</v>
+        <v>262</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B181" s="5">
         <v>1</v>
       </c>
-      <c r="C181" s="6">
-        <v>220</v>
+      <c r="C181" s="3">
+        <v>250</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>177</v>
+        <v>332</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B182" s="5">
         <v>1</v>
@@ -4657,49 +4678,49 @@
         <v>220</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>177</v>
+        <v>333</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>219</v>
+        <v>331</v>
       </c>
       <c r="B183" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C183" s="6">
         <v>220</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B184" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C184" s="6">
         <v>220</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>177</v>
+        <v>334</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B185" s="5">
         <v>1</v>
@@ -4708,27 +4729,44 @@
         <v>220</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>177</v>
+        <v>335</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B186" s="5">
+        <v>1</v>
+      </c>
+      <c r="C186" s="6">
+        <v>220</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>208</v>
+      </c>
+      <c r="B187" s="5">
         <v>5</v>
       </c>
-      <c r="C186" s="6">
+      <c r="C187" s="6">
         <v>350</v>
       </c>
-      <c r="D186" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E186" s="6" t="s">
-        <v>223</v>
+      <c r="D187" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock + image ds update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6DE697-B3C4-4C46-A3A1-15745B3961E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78E2A00-725D-4D8D-AC33-67B25DD762CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4170" yWindow="1440" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="357">
   <si>
     <t>Product</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Marco Blue</t>
   </si>
   <si>
-    <t>Luffy cape (xinh)</t>
-  </si>
-  <si>
     <t>Law Wano (xinh)</t>
   </si>
   <si>
@@ -1060,6 +1057,54 @@
   </si>
   <si>
     <t>naruto war.jpg</t>
+  </si>
+  <si>
+    <t>Zoro Topless Green (WM)</t>
+  </si>
+  <si>
+    <t>zoro topless green WM.jpg</t>
+  </si>
+  <si>
+    <t>rengoku.jpg</t>
+  </si>
+  <si>
+    <t>uzui.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro blue.jpg</t>
+  </si>
+  <si>
+    <t>sanemi.jpg</t>
+  </si>
+  <si>
+    <t>zenitsu.jpg</t>
+  </si>
+  <si>
+    <t>giyu.jpg</t>
+  </si>
+  <si>
+    <t>obanai.jpg</t>
+  </si>
+  <si>
+    <t>inosuke.jpg</t>
+  </si>
+  <si>
+    <t>gyomei.jpg</t>
+  </si>
+  <si>
+    <t>nezuko kid.jpg</t>
+  </si>
+  <si>
+    <t>nezuko adult.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro green.jpg</t>
+  </si>
+  <si>
+    <t>Yonko Luffy</t>
+  </si>
+  <si>
+    <t>yonko luffy.jpg</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E187"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,7 +1663,7 @@
         <v>220</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -1635,7 +1680,7 @@
         <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -1652,7 +1697,7 @@
         <v>350</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1669,7 +1714,7 @@
         <v>180</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
@@ -1686,7 +1731,7 @@
         <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
@@ -1703,7 +1748,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -1720,7 +1765,7 @@
         <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -1737,7 +1782,7 @@
         <v>200</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
@@ -1745,7 +1790,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -1754,7 +1799,7 @@
         <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1762,7 +1807,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1771,7 +1816,7 @@
         <v>280</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1779,7 +1824,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -1788,7 +1833,7 @@
         <v>280</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -1796,7 +1841,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1805,7 +1850,7 @@
         <v>280</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1813,7 +1858,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -1822,7 +1867,7 @@
         <v>280</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -1830,7 +1875,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -1839,7 +1884,7 @@
         <v>280</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -1856,7 +1901,7 @@
         <v>200</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -1873,7 +1918,7 @@
         <v>200</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
@@ -1890,7 +1935,7 @@
         <v>200</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -1907,7 +1952,7 @@
         <v>200</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -1924,7 +1969,7 @@
         <v>200</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -1941,7 +1986,7 @@
         <v>200</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -1958,7 +2003,7 @@
         <v>200</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -1975,7 +2020,7 @@
         <v>200</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -1992,7 +2037,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -2009,7 +2054,7 @@
         <v>220</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -2026,7 +2071,7 @@
         <v>180</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
@@ -2043,7 +2088,7 @@
         <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2060,7 +2105,7 @@
         <v>180</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -2077,7 +2122,7 @@
         <v>180</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -2094,7 +2139,7 @@
         <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -2111,7 +2156,7 @@
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2128,7 +2173,7 @@
         <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2145,7 +2190,7 @@
         <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2162,7 +2207,7 @@
         <v>270</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2179,7 +2224,7 @@
         <v>270</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2196,7 +2241,7 @@
         <v>450</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2213,7 +2258,7 @@
         <v>380</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -2230,7 +2275,7 @@
         <v>800</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2247,7 +2292,7 @@
         <v>270</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2264,7 +2309,7 @@
         <v>270</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -2281,7 +2326,7 @@
         <v>270</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2298,7 +2343,7 @@
         <v>850</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2306,7 +2351,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B43" s="3">
         <v>2</v>
@@ -2315,7 +2360,7 @@
         <v>250</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2323,7 +2368,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
@@ -2332,7 +2377,7 @@
         <v>250</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2349,7 +2394,7 @@
         <v>250</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2366,7 +2411,7 @@
         <v>250</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2374,7 +2419,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
@@ -2383,7 +2428,7 @@
         <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -2391,7 +2436,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
@@ -2400,7 +2445,7 @@
         <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -2408,7 +2453,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -2417,7 +2462,7 @@
         <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -2425,7 +2470,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -2434,7 +2479,7 @@
         <v>360</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -2442,7 +2487,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -2451,7 +2496,7 @@
         <v>360</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -2459,7 +2504,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -2468,7 +2513,7 @@
         <v>200</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -2485,7 +2530,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>44</v>
@@ -2502,7 +2547,7 @@
         <v>150</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>44</v>
@@ -2519,7 +2564,7 @@
         <v>180</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>44</v>
@@ -2527,7 +2572,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
@@ -2536,7 +2581,7 @@
         <v>160</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>44</v>
@@ -2544,7 +2589,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B57" s="3">
         <v>2</v>
@@ -2553,7 +2598,7 @@
         <v>160</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>44</v>
@@ -2570,7 +2615,7 @@
         <v>300</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>44</v>
@@ -2587,7 +2632,7 @@
         <v>300</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>44</v>
@@ -2604,7 +2649,7 @@
         <v>350</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>44</v>
@@ -2621,7 +2666,7 @@
         <v>350</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>44</v>
@@ -2638,7 +2683,7 @@
         <v>500</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>44</v>
@@ -2655,7 +2700,7 @@
         <v>350</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>44</v>
@@ -2672,7 +2717,7 @@
         <v>350</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>44</v>
@@ -2689,7 +2734,7 @@
         <v>350</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>44</v>
@@ -2706,7 +2751,7 @@
         <v>500</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>44</v>
@@ -2723,7 +2768,7 @@
         <v>500</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>44</v>
@@ -2734,13 +2779,13 @@
         <v>57</v>
       </c>
       <c r="B68" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" s="3">
         <v>300</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>58</v>
@@ -2748,7 +2793,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
@@ -2757,7 +2802,7 @@
         <v>300</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>58</v>
@@ -2774,7 +2819,7 @@
         <v>300</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>58</v>
@@ -2791,7 +2836,7 @@
         <v>300</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>58</v>
@@ -2808,7 +2853,7 @@
         <v>300</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>58</v>
@@ -2825,7 +2870,7 @@
         <v>270</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>58</v>
@@ -2842,7 +2887,7 @@
         <v>270</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>58</v>
@@ -2859,7 +2904,7 @@
         <v>300</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>58</v>
@@ -2876,7 +2921,7 @@
         <v>300</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>58</v>
@@ -2893,7 +2938,7 @@
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>58</v>
@@ -2910,7 +2955,7 @@
         <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>58</v>
@@ -2927,7 +2972,7 @@
         <v>300</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>58</v>
@@ -2944,7 +2989,7 @@
         <v>300</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>58</v>
@@ -2952,7 +2997,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B81" s="3">
         <v>2</v>
@@ -2961,7 +3006,7 @@
         <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>58</v>
@@ -2978,7 +3023,7 @@
         <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>58</v>
@@ -2995,7 +3040,7 @@
         <v>300</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>58</v>
@@ -3012,7 +3057,7 @@
         <v>300</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>58</v>
@@ -3029,7 +3074,7 @@
         <v>300</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>58</v>
@@ -3046,7 +3091,7 @@
         <v>300</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>58</v>
@@ -3063,7 +3108,7 @@
         <v>300</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>58</v>
@@ -3080,7 +3125,7 @@
         <v>300</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>58</v>
@@ -3088,16 +3133,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>286</v>
+        <v>341</v>
       </c>
       <c r="B89" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>175</v>
+        <v>342</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>58</v>
@@ -3105,16 +3150,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B90" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C90" s="3">
         <v>350</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>58</v>
@@ -3122,16 +3167,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>77</v>
+        <v>286</v>
       </c>
       <c r="B91" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91" s="3">
         <v>350</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>58</v>
@@ -3139,16 +3184,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B92" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C92" s="3">
         <v>350</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>58</v>
@@ -3156,16 +3201,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" s="3">
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>58</v>
@@ -3173,16 +3218,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B94" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C94" s="3">
         <v>320</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>184</v>
+      <c r="D94" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>58</v>
@@ -3190,7 +3235,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B95" s="3">
         <v>1</v>
@@ -3199,7 +3244,7 @@
         <v>320</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>58</v>
@@ -3207,7 +3252,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B96" s="3">
         <v>1</v>
@@ -3216,7 +3261,7 @@
         <v>320</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>58</v>
@@ -3224,7 +3269,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B97" s="3">
         <v>1</v>
@@ -3233,7 +3278,7 @@
         <v>320</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>58</v>
@@ -3241,7 +3286,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
@@ -3250,7 +3295,7 @@
         <v>320</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>58</v>
@@ -3258,16 +3303,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B99" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C99" s="3">
         <v>320</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>58</v>
@@ -3275,16 +3320,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B100" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C100" s="3">
         <v>320</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>58</v>
@@ -3292,16 +3337,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B101" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="3">
         <v>320</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>58</v>
@@ -3309,7 +3354,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B102" s="3">
         <v>1</v>
@@ -3318,7 +3363,7 @@
         <v>320</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>58</v>
@@ -3326,16 +3371,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B103" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C103" s="3">
         <v>320</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>58</v>
@@ -3343,7 +3388,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B104" s="3">
         <v>2</v>
@@ -3352,7 +3397,7 @@
         <v>320</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>58</v>
@@ -3360,16 +3405,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B105" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" s="3">
         <v>320</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>58</v>
@@ -3377,16 +3422,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B106" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" s="3">
         <v>320</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>58</v>
@@ -3394,16 +3439,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B107" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C107" s="3">
         <v>320</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>58</v>
@@ -3411,16 +3456,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B108" s="3">
         <v>0</v>
       </c>
       <c r="C108" s="3">
-        <v>300</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>164</v>
+        <v>320</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>58</v>
@@ -3428,16 +3473,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>95</v>
+        <v>355</v>
       </c>
       <c r="B109" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C109" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>274</v>
+        <v>356</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>58</v>
@@ -3445,16 +3490,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B110" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C110" s="3">
         <v>300</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>58</v>
@@ -3462,7 +3507,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
@@ -3471,7 +3516,7 @@
         <v>300</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>58</v>
@@ -3479,7 +3524,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B112" s="3">
         <v>1</v>
@@ -3487,8 +3532,8 @@
       <c r="C112" s="3">
         <v>300</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>217</v>
+      <c r="D112" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>58</v>
@@ -3496,7 +3541,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
@@ -3505,7 +3550,7 @@
         <v>300</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>58</v>
@@ -3513,7 +3558,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B114" s="3">
         <v>1</v>
@@ -3522,7 +3567,7 @@
         <v>300</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>58</v>
@@ -3530,7 +3575,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B115" s="3">
         <v>1</v>
@@ -3539,7 +3584,7 @@
         <v>300</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>58</v>
@@ -3547,7 +3592,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B116" s="3">
         <v>1</v>
@@ -3556,7 +3601,7 @@
         <v>300</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>58</v>
@@ -3564,16 +3609,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B117" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C117" s="3">
         <v>300</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>58</v>
@@ -3581,16 +3626,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B118" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C118" s="3">
         <v>300</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>58</v>
@@ -3598,7 +3643,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B119" s="3">
         <v>1</v>
@@ -3606,8 +3651,8 @@
       <c r="C119" s="3">
         <v>300</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>276</v>
+      <c r="D119" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>58</v>
@@ -3615,16 +3660,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B120" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C120" s="3">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>58</v>
@@ -3632,16 +3677,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B121" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" s="3">
         <v>400</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>58</v>
@@ -3649,16 +3694,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B122" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122" s="3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>58</v>
@@ -3666,16 +3711,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B123" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C123" s="3">
         <v>300</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>58</v>
@@ -3683,16 +3728,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B124" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C124" s="3">
         <v>300</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>58</v>
@@ -3700,7 +3745,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B125" s="3">
         <v>1</v>
@@ -3709,7 +3754,7 @@
         <v>300</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>58</v>
@@ -3717,7 +3762,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
@@ -3726,7 +3771,7 @@
         <v>300</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>58</v>
@@ -3734,7 +3779,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -3743,7 +3788,7 @@
         <v>300</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>58</v>
@@ -3751,16 +3796,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B128" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C128" s="3">
         <v>300</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>58</v>
@@ -3768,16 +3813,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B129" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>58</v>
@@ -3785,16 +3830,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B130" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C130" s="3">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>58</v>
@@ -3802,7 +3847,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B131" s="3">
         <v>1</v>
@@ -3811,7 +3856,7 @@
         <v>300</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>58</v>
@@ -3819,41 +3864,41 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B132" s="3">
         <v>1</v>
       </c>
       <c r="C132" s="3">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>317</v>
+        <v>117</v>
       </c>
       <c r="B133" s="3">
         <v>1</v>
       </c>
       <c r="C133" s="3">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>337</v>
+        <v>276</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
@@ -3862,134 +3907,134 @@
         <v>280</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B135" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B136" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136" s="3">
         <v>260</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>120</v>
+        <v>319</v>
       </c>
       <c r="B137" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C137" s="3">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>164</v>
+        <v>339</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>321</v>
+        <v>119</v>
       </c>
       <c r="B138" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" s="3">
-        <v>280</v>
+        <v>500</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>341</v>
+        <v>163</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>121</v>
+        <v>320</v>
       </c>
       <c r="B139" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B140" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C140" s="3">
         <v>220</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B141" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C141" s="3">
         <v>220</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B142" s="3">
         <v>1</v>
@@ -3998,236 +4043,236 @@
         <v>220</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B143" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C143" s="3">
         <v>220</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B144" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C144" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>279</v>
+        <v>125</v>
       </c>
       <c r="B145" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C145" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>278</v>
+        <v>311</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B146" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C146" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B147" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C147" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="B148" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C148" s="3">
         <v>220</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>284</v>
+        <v>126</v>
       </c>
       <c r="B149" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C149" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>128</v>
+        <v>283</v>
       </c>
       <c r="B150" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C150" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B151" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C151" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>164</v>
+        <v>312</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B152" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C152" s="3">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>302</v>
+        <v>163</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B153" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C153" s="3">
         <v>350</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B154" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C154" s="3">
         <v>350</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B155" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C155" s="3">
         <v>350</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B156" s="3">
         <v>1</v>
@@ -4236,151 +4281,151 @@
         <v>350</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B157" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157" s="3">
         <v>350</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B158" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C158" s="3">
-        <v>220</v>
+        <v>350</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B159" s="3">
         <v>1</v>
       </c>
       <c r="C159" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>259</v>
+        <v>315</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B160" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C160" s="3">
-        <v>460</v>
+        <v>250</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B161" s="3">
         <v>0</v>
       </c>
       <c r="C161" s="3">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>260</v>
+        <v>163</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B162" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C162" s="3">
         <v>250</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B163" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C163" s="3">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>164</v>
+        <v>260</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B164" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C164" s="3">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B165" s="3">
         <v>3</v>
@@ -4389,32 +4434,32 @@
         <v>250</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>164</v>
+        <v>343</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B166" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C166" s="3">
         <v>250</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>164</v>
+        <v>344</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B167" s="3">
         <v>1</v>
@@ -4423,32 +4468,32 @@
         <v>250</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>164</v>
+        <v>345</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B168" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C168" s="3">
         <v>250</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>164</v>
+        <v>346</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B169" s="3">
         <v>2</v>
@@ -4457,168 +4502,168 @@
         <v>250</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>164</v>
+        <v>347</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B170" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C170" s="3">
         <v>250</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>164</v>
+        <v>348</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B171" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C171" s="3">
         <v>250</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>164</v>
+        <v>349</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B172" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C172" s="3">
         <v>250</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B173" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C173" s="3">
         <v>250</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>164</v>
+        <v>350</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B174" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C174" s="3">
         <v>250</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B175" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C175" s="3">
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>164</v>
+        <v>351</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B176" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C176" s="3">
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>164</v>
+        <v>352</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B177" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C177" s="3">
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>164</v>
+        <v>353</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B178" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C178" s="3">
         <v>250</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>164</v>
+        <v>354</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B179" s="3">
         <v>0</v>
@@ -4627,117 +4672,117 @@
         <v>250</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B180" s="5">
-        <v>7</v>
+        <v>158</v>
+      </c>
+      <c r="B180" s="3">
+        <v>0</v>
       </c>
       <c r="C180" s="3">
         <v>250</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E180" s="6" t="s">
-        <v>209</v>
+        <v>163</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>203</v>
+      <c r="A181" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="B181" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C181" s="3">
         <v>250</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>332</v>
+        <v>261</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B182" s="5">
         <v>1</v>
       </c>
-      <c r="C182" s="6">
-        <v>220</v>
+      <c r="C182" s="3">
+        <v>250</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>331</v>
+        <v>203</v>
       </c>
       <c r="B183" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" s="6">
         <v>220</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>164</v>
+        <v>332</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>205</v>
+        <v>330</v>
       </c>
       <c r="B184" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C184" s="6">
         <v>220</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>334</v>
+        <v>163</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B185" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C185" s="6">
         <v>220</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B186" s="5">
         <v>1</v>
@@ -4746,27 +4791,44 @@
         <v>220</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>206</v>
+      </c>
+      <c r="B187" s="5">
+        <v>1</v>
+      </c>
+      <c r="C187" s="6">
+        <v>220</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E187" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B187" s="5">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>207</v>
+      </c>
+      <c r="B188" s="5">
         <v>5</v>
       </c>
-      <c r="C187" s="6">
+      <c r="C188" s="6">
         <v>350</v>
       </c>
-      <c r="D187" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E187" s="6" t="s">
-        <v>209</v>
+      <c r="D188" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
socials icon updated and overall site update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7235DE-78E2-48C6-A325-1ACA58513FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A803ADA8-6AB1-4744-89C0-262839A2104B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1440" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="390" yWindow="1335" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1056,9 +1056,6 @@
     <t>Zoro Topless Green (WM)</t>
   </si>
   <si>
-    <t>zoro topless green WM.jpg</t>
-  </si>
-  <si>
     <t>rengoku.jpg</t>
   </si>
   <si>
@@ -1105,6 +1102,9 @@
   </si>
   <si>
     <t>jeager.jpg</t>
+  </si>
+  <si>
+    <t>zoro topless green WM.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3142,7 @@
         <v>300</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>340</v>
+        <v>356</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>58</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B109" s="3">
         <v>1</v>
@@ -3482,7 +3482,7 @@
         <v>320</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>58</v>
@@ -4434,7 +4434,7 @@
         <v>250</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>143</v>
@@ -4451,7 +4451,7 @@
         <v>250</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>143</v>
@@ -4468,7 +4468,7 @@
         <v>250</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>143</v>
@@ -4485,7 +4485,7 @@
         <v>250</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>143</v>
@@ -4502,7 +4502,7 @@
         <v>250</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>143</v>
@@ -4519,7 +4519,7 @@
         <v>250</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>143</v>
@@ -4536,7 +4536,7 @@
         <v>250</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>143</v>
@@ -4570,7 +4570,7 @@
         <v>250</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>143</v>
@@ -4604,7 +4604,7 @@
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>143</v>
@@ -4621,7 +4621,7 @@
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>143</v>
@@ -4638,7 +4638,7 @@
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>143</v>
@@ -4655,7 +4655,7 @@
         <v>250</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>143</v>
@@ -4791,7 +4791,7 @@
         <v>220</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>208</v>
@@ -4808,7 +4808,7 @@
         <v>220</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E187" s="6" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
added back to top button
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87A6A52-A3AD-426B-B9FB-728339FEFBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429BB806-EA00-46FC-8CB0-5D536B8A5685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="1335" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -1128,13 +1128,13 @@
     <t>pokemon sticker.jpg</t>
   </si>
   <si>
+    <t>Goku</t>
+  </si>
+  <si>
+    <t>DBZ</t>
+  </si>
+  <si>
     <t>manga cover sticker.jpg</t>
-  </si>
-  <si>
-    <t>Goku</t>
-  </si>
-  <si>
-    <t>DBZ</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1655,7 @@
   <dimension ref="A1:E193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A182" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4906,7 +4906,7 @@
         <v>250</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E191" s="6" t="s">
         <v>361</v>
@@ -4931,7 +4931,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B193" s="5">
         <v>0</v>
@@ -4943,7 +4943,7 @@
         <v>163</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display box and baseplate added
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429BB806-EA00-46FC-8CB0-5D536B8A5685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F2F82-D4B0-4E0D-A368-24D098CA7284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="1335" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="371">
   <si>
     <t>Product</t>
   </si>
@@ -1135,6 +1135,18 @@
   </si>
   <si>
     <t>manga cover sticker.jpg</t>
+  </si>
+  <si>
+    <t>display box.jpg</t>
+  </si>
+  <si>
+    <t>baseplate.jpg</t>
+  </si>
+  <si>
+    <t>Display Box (grey)</t>
+  </si>
+  <si>
+    <t>Baseplate</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1206,6 +1218,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1652,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A182" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+      <selection activeCell="G193" sqref="G193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4946,6 +4961,40 @@
         <v>365</v>
       </c>
     </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>369</v>
+      </c>
+      <c r="B194" s="5">
+        <v>4</v>
+      </c>
+      <c r="C194" s="7">
+        <v>800</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E194" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>370</v>
+      </c>
+      <c r="B195" s="5">
+        <v>13</v>
+      </c>
+      <c r="C195" s="7">
+        <v>200</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new category and products added
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288BCB09-AFAA-418C-9D0B-823B2DB4293A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBE2BC7-C85B-49F2-BFFE-576FB9740535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1335" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="2070" yWindow="1635" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="414">
   <si>
     <t>Product</t>
   </si>
@@ -702,12 +702,6 @@
     <t>Moonknight black.png</t>
   </si>
   <si>
-    <t>Black Adam hood.jpg</t>
-  </si>
-  <si>
-    <t>Black Adam bald.jpg</t>
-  </si>
-  <si>
     <t>Batman Affleck.jpg</t>
   </si>
   <si>
@@ -1246,6 +1240,42 @@
   </si>
   <si>
     <t>sleeping slow.jpg</t>
+  </si>
+  <si>
+    <t>pikaball.jpg</t>
+  </si>
+  <si>
+    <t>Cute Alien Cat Keyring</t>
+  </si>
+  <si>
+    <t>Cute Astro Bear Keyring</t>
+  </si>
+  <si>
+    <t>Cute Pink Cat Keyring</t>
+  </si>
+  <si>
+    <t>Labubu The Cute Monster Keyring</t>
+  </si>
+  <si>
+    <t>alien.jpg</t>
+  </si>
+  <si>
+    <t>astro.jpg</t>
+  </si>
+  <si>
+    <t>pink.jpg</t>
+  </si>
+  <si>
+    <t>labubu.jpg</t>
+  </si>
+  <si>
+    <t>adam hood.jpg</t>
+  </si>
+  <si>
+    <t>adam bald.jpg</t>
+  </si>
+  <si>
+    <t>Bleach</t>
   </si>
 </sst>
 </file>
@@ -1763,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D213" sqref="D213"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183:E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,7 +1919,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -1931,7 +1961,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -1940,7 +1970,7 @@
         <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1948,7 +1978,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1957,7 +1987,7 @@
         <v>280</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1965,7 +1995,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -1974,7 +2004,7 @@
         <v>280</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -1982,7 +2012,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1991,7 +2021,7 @@
         <v>280</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1999,7 +2029,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -2008,7 +2038,7 @@
         <v>280</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -2016,7 +2046,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2025,7 +2055,7 @@
         <v>280</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -2042,7 +2072,7 @@
         <v>220</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -2076,7 +2106,7 @@
         <v>220</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -2093,7 +2123,7 @@
         <v>220</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -2110,7 +2140,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -2127,7 +2157,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -2144,7 +2174,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -2178,7 +2208,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -2229,7 +2259,7 @@
         <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2297,7 +2327,7 @@
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2314,7 +2344,7 @@
         <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2331,7 +2361,7 @@
         <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2365,7 +2395,7 @@
         <v>270</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2382,7 +2412,7 @@
         <v>450</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2433,7 +2463,7 @@
         <v>270</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2467,7 +2497,7 @@
         <v>270</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2492,7 +2522,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B43" s="3">
         <v>2</v>
@@ -2509,7 +2539,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
@@ -2518,7 +2548,7 @@
         <v>250</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2535,7 +2565,7 @@
         <v>250</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2552,7 +2582,7 @@
         <v>250</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2560,7 +2590,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
@@ -2577,7 +2607,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
@@ -2594,7 +2624,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -2611,7 +2641,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -2620,7 +2650,7 @@
         <v>360</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -2628,7 +2658,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -2637,7 +2667,7 @@
         <v>360</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -2645,7 +2675,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -2654,7 +2684,7 @@
         <v>200</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -2671,7 +2701,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>44</v>
@@ -2713,16 +2743,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
       </c>
       <c r="C56" s="3">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>222</v>
+        <v>411</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>44</v>
@@ -2730,16 +2760,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" s="3">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>223</v>
+        <v>412</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>44</v>
@@ -2756,7 +2786,7 @@
         <v>300</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>44</v>
@@ -2773,7 +2803,7 @@
         <v>300</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>44</v>
@@ -2790,7 +2820,7 @@
         <v>350</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>44</v>
@@ -2807,7 +2837,7 @@
         <v>350</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>44</v>
@@ -2824,7 +2854,7 @@
         <v>500</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>44</v>
@@ -3087,7 +3117,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
@@ -3138,7 +3168,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B81" s="3">
         <v>2</v>
@@ -3147,7 +3177,7 @@
         <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>58</v>
@@ -3274,7 +3304,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B89" s="3">
         <v>1</v>
@@ -3283,7 +3313,7 @@
         <v>300</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>58</v>
@@ -3291,7 +3321,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B90" s="3">
         <v>2</v>
@@ -3308,7 +3338,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B91" s="3">
         <v>1</v>
@@ -3614,7 +3644,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B109" s="3">
         <v>1</v>
@@ -3623,7 +3653,7 @@
         <v>320</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>58</v>
@@ -3640,7 +3670,7 @@
         <v>300</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>58</v>
@@ -3657,7 +3687,7 @@
         <v>300</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>58</v>
@@ -3674,7 +3704,7 @@
         <v>300</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>58</v>
@@ -3810,7 +3840,7 @@
         <v>300</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>58</v>
@@ -3827,7 +3857,7 @@
         <v>400</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>58</v>
@@ -3844,7 +3874,7 @@
         <v>400</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>58</v>
@@ -3852,7 +3882,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B123" s="3">
         <v>1</v>
@@ -3861,7 +3891,7 @@
         <v>300</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>58</v>
@@ -3878,7 +3908,7 @@
         <v>300</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>58</v>
@@ -3895,7 +3925,7 @@
         <v>300</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>58</v>
@@ -3912,7 +3942,7 @@
         <v>300</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>58</v>
@@ -3929,7 +3959,7 @@
         <v>300</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>58</v>
@@ -3946,7 +3976,7 @@
         <v>300</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>58</v>
@@ -3963,7 +3993,7 @@
         <v>300</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>58</v>
@@ -3980,7 +4010,7 @@
         <v>500</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>58</v>
@@ -3997,7 +4027,7 @@
         <v>300</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>58</v>
@@ -4014,7 +4044,7 @@
         <v>300</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>58</v>
@@ -4031,7 +4061,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>116</v>
@@ -4039,7 +4069,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
@@ -4048,7 +4078,7 @@
         <v>280</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>116</v>
@@ -4056,7 +4086,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B135" s="3">
         <v>1</v>
@@ -4065,7 +4095,7 @@
         <v>280</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>116</v>
@@ -4073,7 +4103,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B136" s="3">
         <v>2</v>
@@ -4082,7 +4112,7 @@
         <v>260</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>116</v>
@@ -4090,7 +4120,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B137" s="3">
         <v>1</v>
@@ -4099,7 +4129,7 @@
         <v>260</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>116</v>
@@ -4124,7 +4154,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B139" s="3">
         <v>1</v>
@@ -4133,7 +4163,7 @@
         <v>280</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>116</v>
@@ -4150,7 +4180,7 @@
         <v>220</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>116</v>
@@ -4167,7 +4197,7 @@
         <v>220</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>116</v>
@@ -4184,7 +4214,7 @@
         <v>220</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>116</v>
@@ -4201,7 +4231,7 @@
         <v>220</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>116</v>
@@ -4218,7 +4248,7 @@
         <v>220</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>116</v>
@@ -4235,7 +4265,7 @@
         <v>250</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>116</v>
@@ -4243,7 +4273,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B146" s="3">
         <v>2</v>
@@ -4252,7 +4282,7 @@
         <v>220</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>116</v>
@@ -4260,7 +4290,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B147" s="3">
         <v>3</v>
@@ -4269,7 +4299,7 @@
         <v>250</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>116</v>
@@ -4277,7 +4307,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B148" s="3">
         <v>1</v>
@@ -4286,7 +4316,7 @@
         <v>220</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>116</v>
@@ -4303,7 +4333,7 @@
         <v>220</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>116</v>
@@ -4311,7 +4341,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B150" s="3">
         <v>2</v>
@@ -4320,7 +4350,7 @@
         <v>250</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>116</v>
@@ -4337,7 +4367,7 @@
         <v>220</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>116</v>
@@ -4371,7 +4401,7 @@
         <v>350</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>116</v>
@@ -4388,7 +4418,7 @@
         <v>350</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>116</v>
@@ -4405,7 +4435,7 @@
         <v>350</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>116</v>
@@ -4422,7 +4452,7 @@
         <v>350</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>116</v>
@@ -4439,7 +4469,7 @@
         <v>350</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>116</v>
@@ -4456,7 +4486,7 @@
         <v>350</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>116</v>
@@ -4473,7 +4503,7 @@
         <v>220</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>116</v>
@@ -4490,7 +4520,7 @@
         <v>250</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>135</v>
@@ -4524,7 +4554,7 @@
         <v>250</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>135</v>
@@ -4541,7 +4571,7 @@
         <v>250</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>135</v>
@@ -4575,7 +4605,7 @@
         <v>250</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>141</v>
@@ -4592,7 +4622,7 @@
         <v>250</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>141</v>
@@ -4609,7 +4639,7 @@
         <v>250</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>141</v>
@@ -4626,7 +4656,7 @@
         <v>250</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>141</v>
@@ -4643,7 +4673,7 @@
         <v>250</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>141</v>
@@ -4660,7 +4690,7 @@
         <v>250</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>141</v>
@@ -4677,7 +4707,7 @@
         <v>250</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>141</v>
@@ -4711,7 +4741,7 @@
         <v>250</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>141</v>
@@ -4745,7 +4775,7 @@
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>141</v>
@@ -4762,7 +4792,7 @@
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>141</v>
@@ -4779,7 +4809,7 @@
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>141</v>
@@ -4796,7 +4826,7 @@
         <v>250</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>141</v>
@@ -4847,7 +4877,7 @@
         <v>250</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E181" s="6" t="s">
         <v>206</v>
@@ -4864,7 +4894,7 @@
         <v>250</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>206</v>
@@ -4881,15 +4911,15 @@
         <v>220</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>206</v>
+        <v>413</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B184" s="5">
         <v>0</v>
@@ -4901,7 +4931,7 @@
         <v>161</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>206</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4915,10 +4945,10 @@
         <v>220</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>206</v>
+        <v>413</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4932,10 +4962,10 @@
         <v>220</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>206</v>
+        <v>413</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4949,10 +4979,10 @@
         <v>220</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>206</v>
+        <v>413</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4966,7 +4996,7 @@
         <v>350</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>206</v>
@@ -4974,7 +5004,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B189" s="5">
         <v>10</v>
@@ -4983,15 +5013,15 @@
         <v>250</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B190" s="5">
         <v>3</v>
@@ -5000,15 +5030,15 @@
         <v>250</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B191" s="5">
         <v>24</v>
@@ -5017,15 +5047,15 @@
         <v>250</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B192" s="5">
         <v>6</v>
@@ -5034,15 +5064,15 @@
         <v>150</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B193" s="5">
         <v>2</v>
@@ -5051,15 +5081,15 @@
         <v>150</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B194" s="5">
         <v>2</v>
@@ -5068,15 +5098,15 @@
         <v>150</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B195" s="5">
         <v>5</v>
@@ -5085,15 +5115,15 @@
         <v>550</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B196" s="5">
         <v>0</v>
@@ -5105,12 +5135,12 @@
         <v>161</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B197" s="5">
         <v>4</v>
@@ -5119,7 +5149,7 @@
         <v>800</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E197" s="6" t="s">
         <v>206</v>
@@ -5127,7 +5157,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B198" s="5">
         <v>13</v>
@@ -5136,7 +5166,7 @@
         <v>200</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E198" s="6" t="s">
         <v>206</v>
@@ -5144,7 +5174,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B199" s="5">
         <v>3</v>
@@ -5153,15 +5183,15 @@
         <v>150</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B200" s="5">
         <v>2</v>
@@ -5170,15 +5200,15 @@
         <v>150</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B201" s="5">
         <v>1</v>
@@ -5187,15 +5217,15 @@
         <v>150</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B202" s="5">
         <v>1</v>
@@ -5204,15 +5234,15 @@
         <v>150</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>161</v>
+        <v>402</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B203" s="5">
         <v>10</v>
@@ -5221,15 +5251,15 @@
         <v>30</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B204" s="5">
         <v>1</v>
@@ -5238,15 +5268,15 @@
         <v>550</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B205" s="5">
         <v>1</v>
@@ -5255,15 +5285,15 @@
         <v>550</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B206" s="5">
         <v>1</v>
@@ -5272,15 +5302,15 @@
         <v>550</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B207" s="5">
         <v>1</v>
@@ -5289,15 +5319,15 @@
         <v>550</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B208" s="5">
         <v>1</v>
@@ -5306,15 +5336,15 @@
         <v>550</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B209" s="5">
         <v>1</v>
@@ -5323,15 +5353,15 @@
         <v>550</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B210" s="5">
         <v>1</v>
@@ -5340,15 +5370,15 @@
         <v>550</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B211" s="5">
         <v>1</v>
@@ -5357,16 +5387,79 @@
         <v>550</v>
       </c>
       <c r="D211" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>403</v>
       </c>
-      <c r="E211" s="6" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B212" s="5"/>
-      <c r="C212" s="6"/>
-      <c r="E212" s="6"/>
+      <c r="B212" s="5">
+        <v>6</v>
+      </c>
+      <c r="C212" s="6">
+        <v>250</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="E212" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>404</v>
+      </c>
+      <c r="B213" s="5">
+        <v>1</v>
+      </c>
+      <c r="C213" s="6">
+        <v>250</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E213" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>405</v>
+      </c>
+      <c r="B214" s="5">
+        <v>4</v>
+      </c>
+      <c r="C214" s="6">
+        <v>250</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>406</v>
+      </c>
+      <c r="B215" s="5">
+        <v>1</v>
+      </c>
+      <c r="C215" s="6">
+        <v>250</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E215" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stock update cat keyring
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F40C2-0F0D-4352-A39E-50025C410A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC3AB-2397-47D3-87FE-D4773AF61C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="1635" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5458,7 +5458,7 @@
         <v>405</v>
       </c>
       <c r="B215" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C215" s="6">
         <v>250</v>

</xml_diff>

<commit_message>
new stock updated dc
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC3AB-2397-47D3-87FE-D4773AF61C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E70FD1-D00F-4DBA-857E-A72F7D6EEDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="1635" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="3240" yWindow="1260" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="431">
   <si>
     <t>Product</t>
   </si>
@@ -1285,6 +1285,48 @@
   </si>
   <si>
     <t>joker.jpg</t>
+  </si>
+  <si>
+    <t>Spot (Black)</t>
+  </si>
+  <si>
+    <t>spot black.jpg</t>
+  </si>
+  <si>
+    <t>spiderman2099 kdl.jpg</t>
+  </si>
+  <si>
+    <t>Spiderman 2099 v2</t>
+  </si>
+  <si>
+    <t>Prowler</t>
+  </si>
+  <si>
+    <t>prowler.jpg</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>wonder woman.jpg</t>
+  </si>
+  <si>
+    <t>General Zod</t>
+  </si>
+  <si>
+    <t>zod.jpg</t>
+  </si>
+  <si>
+    <t>The Flash</t>
+  </si>
+  <si>
+    <t>Cyborg</t>
+  </si>
+  <si>
+    <t>flash.jpg</t>
+  </si>
+  <si>
+    <t>cyborg.jpg</t>
   </si>
 </sst>
 </file>
@@ -1802,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,16 +2046,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>287</v>
+        <v>420</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
         <v>280</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>294</v>
+        <v>419</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -2021,7 +2063,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -2030,7 +2072,7 @@
         <v>280</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -2038,16 +2080,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>280</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -2055,7 +2097,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>290</v>
+        <v>417</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2064,7 +2106,7 @@
         <v>280</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>296</v>
+        <v>418</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -2072,16 +2114,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>289</v>
       </c>
       <c r="B16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -2089,16 +2131,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>290</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>161</v>
+        <v>296</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
@@ -2106,16 +2148,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>421</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
       </c>
       <c r="C18" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>260</v>
+        <v>422</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -2123,16 +2165,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>220</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -2140,16 +2182,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3">
         <v>220</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>262</v>
+        <v>161</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -2157,7 +2199,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -2166,7 +2208,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -2174,7 +2216,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -2183,7 +2225,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -2191,16 +2233,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
         <v>220</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>161</v>
+        <v>262</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -2208,16 +2250,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -2225,7 +2267,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -2234,7 +2276,7 @@
         <v>220</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>162</v>
+        <v>264</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -2242,16 +2284,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
@@ -2259,16 +2301,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2276,16 +2318,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -2293,16 +2335,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" s="3">
         <v>180</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -2310,16 +2352,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" s="3">
         <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -2327,16 +2369,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C31" s="3">
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2344,16 +2386,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="3">
         <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>229</v>
+        <v>161</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2361,16 +2403,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C33" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>230</v>
+        <v>161</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2378,16 +2420,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2395,16 +2437,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2412,16 +2454,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" s="3">
-        <v>450</v>
+        <v>270</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2429,16 +2471,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="3">
-        <v>380</v>
+        <v>270</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -2446,16 +2488,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C38" s="3">
-        <v>800</v>
+        <v>270</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2463,16 +2505,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="3">
-        <v>270</v>
+        <v>450</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2480,16 +2522,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C40" s="3">
-        <v>270</v>
+        <v>380</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -2497,16 +2539,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3">
-        <v>270</v>
+        <v>800</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2514,16 +2556,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="3">
-        <v>850</v>
+        <v>270</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>167</v>
+        <v>265</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2531,16 +2573,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>317</v>
+        <v>38</v>
       </c>
       <c r="B43" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2548,16 +2590,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>318</v>
+        <v>39</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
       </c>
       <c r="C44" s="3">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2565,16 +2607,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C45" s="3">
-        <v>250</v>
+        <v>850</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>234</v>
+        <v>167</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2582,7 +2624,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>317</v>
       </c>
       <c r="B46" s="3">
         <v>2</v>
@@ -2591,7 +2633,7 @@
         <v>250</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2599,16 +2641,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="3">
         <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>165</v>
+        <v>233</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -2616,16 +2658,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>319</v>
+        <v>41</v>
       </c>
       <c r="B48" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="3">
         <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -2633,16 +2675,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>321</v>
+        <v>42</v>
       </c>
       <c r="B49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" s="3">
         <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -2650,16 +2692,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B50" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" s="3">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>267</v>
+        <v>165</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -2667,16 +2709,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" s="3">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>268</v>
+        <v>221</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -2684,16 +2726,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="B52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -2701,67 +2743,67 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>322</v>
       </c>
       <c r="B53" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" s="3">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>43</v>
+        <v>323</v>
       </c>
       <c r="B54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="3">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>416</v>
+        <v>268</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>236</v>
       </c>
       <c r="B55" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C55" s="3">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>324</v>
+        <v>47</v>
       </c>
       <c r="B56" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C56" s="3">
         <v>180</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>411</v>
+        <v>238</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>44</v>
@@ -2769,16 +2811,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>325</v>
+        <v>425</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" s="3">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>44</v>
@@ -2786,16 +2828,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B58" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C58" s="3">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>239</v>
+        <v>416</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>44</v>
@@ -2803,16 +2845,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>45</v>
+        <v>423</v>
       </c>
       <c r="B59" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" s="3">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>240</v>
+        <v>424</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>44</v>
@@ -2820,16 +2862,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B60" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C60" s="3">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>222</v>
+        <v>161</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>44</v>
@@ -2837,16 +2879,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>50</v>
+        <v>427</v>
       </c>
       <c r="B61" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C61" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>223</v>
+        <v>429</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>44</v>
@@ -2854,16 +2896,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>51</v>
+        <v>428</v>
       </c>
       <c r="B62" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C62" s="3">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>224</v>
+        <v>430</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>44</v>
@@ -2871,16 +2913,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>52</v>
+        <v>324</v>
       </c>
       <c r="B63" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63" s="3">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>209</v>
+        <v>411</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>44</v>
@@ -2888,16 +2930,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>53</v>
+        <v>325</v>
       </c>
       <c r="B64" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" s="3">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>210</v>
+        <v>412</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>44</v>
@@ -2905,16 +2947,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B65" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C65" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>44</v>
@@ -2922,16 +2964,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B66" s="3">
         <v>0</v>
       </c>
       <c r="C66" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>44</v>
@@ -2939,16 +2981,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B67" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67" s="3">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>44</v>
@@ -2956,126 +2998,126 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B68" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C68" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="B69" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C69" s="3">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B70" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C70" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B71" s="3">
         <v>0</v>
       </c>
       <c r="C71" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B72" s="3">
         <v>1</v>
       </c>
       <c r="C72" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="C73" s="3">
-        <v>270</v>
+        <v>500</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B74" s="3">
         <v>0</v>
       </c>
       <c r="C74" s="3">
-        <v>270</v>
+        <v>500</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B75" s="3">
         <v>1</v>
@@ -3084,7 +3126,7 @@
         <v>300</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>58</v>
@@ -3092,16 +3134,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
       <c r="B76" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" s="3">
         <v>300</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>58</v>
@@ -3109,16 +3151,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B77" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="3">
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>58</v>
@@ -3126,16 +3168,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>374</v>
+        <v>60</v>
       </c>
       <c r="B78" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" s="3">
         <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>58</v>
@@ -3143,16 +3185,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79" s="3">
         <v>300</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>58</v>
@@ -3160,13 +3202,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B80" s="3">
         <v>0</v>
       </c>
       <c r="C80" s="3">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>161</v>
@@ -3177,16 +3219,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>283</v>
+        <v>63</v>
       </c>
       <c r="B81" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C81" s="3">
-        <v>350</v>
+        <v>270</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>284</v>
+        <v>169</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>58</v>
@@ -3194,16 +3236,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B82" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82" s="3">
         <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>58</v>
@@ -3211,7 +3253,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B83" s="3">
         <v>0</v>
@@ -3228,16 +3270,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B84" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C84" s="3">
         <v>300</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>58</v>
@@ -3245,16 +3287,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>72</v>
+        <v>374</v>
       </c>
       <c r="B85" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" s="3">
         <v>300</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>58</v>
@@ -3262,7 +3304,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B86" s="3">
         <v>0</v>
@@ -3271,7 +3313,7 @@
         <v>300</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>58</v>
@@ -3279,7 +3321,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B87" s="3">
         <v>0</v>
@@ -3296,16 +3338,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>75</v>
+        <v>283</v>
       </c>
       <c r="B88" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C88" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>177</v>
+        <v>284</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>58</v>
@@ -3313,16 +3355,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>335</v>
+        <v>69</v>
       </c>
       <c r="B89" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="3">
         <v>300</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>352</v>
+        <v>161</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>58</v>
@@ -3330,16 +3372,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>281</v>
+        <v>70</v>
       </c>
       <c r="B90" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C90" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>58</v>
@@ -3347,16 +3389,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>282</v>
+        <v>71</v>
       </c>
       <c r="B91" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>58</v>
@@ -3364,16 +3406,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B92" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C92" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>58</v>
@@ -3381,16 +3423,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B93" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>58</v>
@@ -3398,16 +3440,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B94" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C94" s="3">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>58</v>
@@ -3415,16 +3457,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B95" s="3">
         <v>1</v>
       </c>
       <c r="C95" s="3">
-        <v>320</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>181</v>
+        <v>300</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>58</v>
@@ -3432,16 +3474,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>80</v>
+        <v>335</v>
       </c>
       <c r="B96" s="3">
         <v>1</v>
       </c>
       <c r="C96" s="3">
-        <v>320</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>194</v>
+        <v>300</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>58</v>
@@ -3449,16 +3491,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>81</v>
+        <v>281</v>
       </c>
       <c r="B97" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C97" s="3">
-        <v>320</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>182</v>
+        <v>350</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>58</v>
@@ -3466,16 +3508,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>82</v>
+        <v>282</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
       </c>
       <c r="C98" s="3">
-        <v>320</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>183</v>
+        <v>350</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>58</v>
@@ -3483,16 +3525,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B99" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C99" s="3">
-        <v>320</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>184</v>
+        <v>350</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>58</v>
@@ -3500,16 +3542,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B100" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" s="3">
-        <v>320</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>185</v>
+        <v>350</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>58</v>
@@ -3517,16 +3559,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B101" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C101" s="3">
         <v>320</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>186</v>
+      <c r="D101" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>58</v>
@@ -3534,7 +3576,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B102" s="3">
         <v>1</v>
@@ -3543,7 +3585,7 @@
         <v>320</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>58</v>
@@ -3551,7 +3593,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
@@ -3560,7 +3602,7 @@
         <v>320</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>58</v>
@@ -3568,16 +3610,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B104" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" s="3">
         <v>320</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>58</v>
@@ -3585,16 +3627,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B105" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C105" s="3">
         <v>320</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>58</v>
@@ -3602,7 +3644,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B106" s="3">
         <v>1</v>
@@ -3611,7 +3653,7 @@
         <v>320</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>58</v>
@@ -3619,7 +3661,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B107" s="3">
         <v>2</v>
@@ -3628,7 +3670,7 @@
         <v>320</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>58</v>
@@ -3636,7 +3678,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B108" s="3">
         <v>0</v>
@@ -3645,7 +3687,7 @@
         <v>320</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>58</v>
@@ -3653,7 +3695,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>348</v>
+        <v>86</v>
       </c>
       <c r="B109" s="3">
         <v>1</v>
@@ -3661,8 +3703,8 @@
       <c r="C109" s="3">
         <v>320</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>349</v>
+      <c r="D109" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>58</v>
@@ -3670,16 +3712,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B110" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110" s="3">
-        <v>300</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>269</v>
+        <v>320</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>58</v>
@@ -3687,16 +3729,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B111" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C111" s="3">
-        <v>300</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>241</v>
+        <v>320</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>58</v>
@@ -3704,16 +3746,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B112" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C112" s="3">
-        <v>300</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>270</v>
+        <v>320</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>58</v>
@@ -3721,16 +3763,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
       </c>
       <c r="C113" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>58</v>
@@ -3738,16 +3780,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B114" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C114" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>58</v>
@@ -3755,16 +3797,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B115" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>58</v>
@@ -3772,16 +3814,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>99</v>
+        <v>348</v>
       </c>
       <c r="B116" s="3">
         <v>1</v>
       </c>
       <c r="C116" s="3">
-        <v>300</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>217</v>
+        <v>320</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>58</v>
@@ -3789,16 +3831,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B117" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C117" s="3">
         <v>300</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>218</v>
+      <c r="D117" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>58</v>
@@ -3806,16 +3848,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B118" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C118" s="3">
         <v>300</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>219</v>
+      <c r="D118" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>58</v>
@@ -3823,7 +3865,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B119" s="3">
         <v>1</v>
@@ -3831,8 +3873,8 @@
       <c r="C119" s="3">
         <v>300</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>220</v>
+      <c r="D119" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>58</v>
@@ -3840,7 +3882,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B120" s="3">
         <v>1</v>
@@ -3848,8 +3890,8 @@
       <c r="C120" s="3">
         <v>300</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>271</v>
+      <c r="D120" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>58</v>
@@ -3857,16 +3899,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B121" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C121" s="3">
-        <v>400</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>242</v>
+        <v>300</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>58</v>
@@ -3874,16 +3916,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B122" s="3">
         <v>1</v>
       </c>
       <c r="C122" s="3">
-        <v>400</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>243</v>
+        <v>300</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>58</v>
@@ -3891,7 +3933,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>375</v>
+        <v>99</v>
       </c>
       <c r="B123" s="3">
         <v>1</v>
@@ -3899,8 +3941,8 @@
       <c r="C123" s="3">
         <v>300</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>244</v>
+      <c r="D123" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>58</v>
@@ -3908,16 +3950,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B124" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C124" s="3">
         <v>300</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>245</v>
+      <c r="D124" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>58</v>
@@ -3925,16 +3967,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B125" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C125" s="3">
         <v>300</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>246</v>
+      <c r="D125" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>58</v>
@@ -3942,7 +3984,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
@@ -3950,8 +3992,8 @@
       <c r="C126" s="3">
         <v>300</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>247</v>
+      <c r="D126" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>58</v>
@@ -3959,7 +4001,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -3968,7 +4010,7 @@
         <v>300</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>58</v>
@@ -3976,16 +4018,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B128" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C128" s="3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>58</v>
@@ -3993,16 +4035,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B129" s="3">
         <v>1</v>
       </c>
       <c r="C129" s="3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>58</v>
@@ -4010,16 +4052,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>112</v>
+        <v>375</v>
       </c>
       <c r="B130" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C130" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>58</v>
@@ -4027,16 +4069,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B131" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C131" s="3">
         <v>300</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>58</v>
@@ -4044,7 +4086,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B132" s="3">
         <v>1</v>
@@ -4053,7 +4095,7 @@
         <v>300</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>58</v>
@@ -4061,135 +4103,135 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B133" s="3">
         <v>1</v>
       </c>
       <c r="C133" s="3">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>312</v>
+        <v>109</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
       </c>
       <c r="C134" s="3">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>330</v>
+        <v>248</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="B135" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135" s="3">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>331</v>
+        <v>249</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>314</v>
+        <v>111</v>
       </c>
       <c r="B136" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C136" s="3">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>332</v>
+        <v>250</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>315</v>
+        <v>112</v>
       </c>
       <c r="B137" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137" s="3">
-        <v>260</v>
+        <v>500</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>333</v>
+        <v>251</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B138" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C138" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>316</v>
+        <v>114</v>
       </c>
       <c r="B139" s="3">
         <v>1</v>
       </c>
       <c r="C139" s="3">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>334</v>
+        <v>253</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B140" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C140" s="3">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>116</v>
@@ -4197,16 +4239,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>119</v>
+        <v>312</v>
       </c>
       <c r="B141" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C141" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>116</v>
@@ -4214,16 +4256,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>120</v>
+        <v>313</v>
       </c>
       <c r="B142" s="3">
         <v>1</v>
       </c>
       <c r="C142" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>116</v>
@@ -4231,16 +4273,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>121</v>
+        <v>314</v>
       </c>
       <c r="B143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C143" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>116</v>
@@ -4248,16 +4290,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>122</v>
+        <v>315</v>
       </c>
       <c r="B144" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C144" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>116</v>
@@ -4265,16 +4307,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B145" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145" s="3">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>307</v>
+        <v>161</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>116</v>
@@ -4282,16 +4324,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="B146" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C146" s="3">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>273</v>
+        <v>334</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>116</v>
@@ -4299,16 +4341,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>275</v>
+        <v>118</v>
       </c>
       <c r="B147" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C147" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>116</v>
@@ -4316,16 +4358,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
       <c r="B148" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C148" s="3">
         <v>220</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>116</v>
@@ -4333,16 +4375,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B149" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C149" s="3">
         <v>220</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>116</v>
@@ -4350,16 +4392,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="B150" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C150" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>116</v>
@@ -4367,16 +4409,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B151" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C151" s="3">
         <v>220</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>116</v>
@@ -4384,16 +4426,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B152" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C152" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>161</v>
+        <v>307</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>116</v>
@@ -4401,16 +4443,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>127</v>
+        <v>274</v>
       </c>
       <c r="B153" s="3">
         <v>2</v>
       </c>
       <c r="C153" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>116</v>
@@ -4418,16 +4460,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>128</v>
+        <v>275</v>
       </c>
       <c r="B154" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C154" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>116</v>
@@ -4435,16 +4477,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>129</v>
+        <v>278</v>
       </c>
       <c r="B155" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C155" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>116</v>
@@ -4452,16 +4494,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B156" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C156" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>116</v>
@@ -4469,16 +4511,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>131</v>
+        <v>279</v>
       </c>
       <c r="B157" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C157" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>116</v>
@@ -4486,16 +4528,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B158" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C158" s="3">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>116</v>
@@ -4503,16 +4545,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B159" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="3">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>311</v>
+        <v>161</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>116</v>
@@ -4520,126 +4562,126 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B160" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C160" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B161" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C161" s="3">
-        <v>460</v>
+        <v>350</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>161</v>
+        <v>298</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B162" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C162" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B163" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C163" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B164" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C164" s="3">
-        <v>240</v>
+        <v>350</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>161</v>
+        <v>301</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B165" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C165" s="3">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B166" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C166" s="3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B167" s="3">
         <v>1</v>
@@ -4648,92 +4690,92 @@
         <v>250</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>338</v>
+        <v>254</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B168" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C168" s="3">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>339</v>
+        <v>161</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B169" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C169" s="3">
         <v>250</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>340</v>
+        <v>255</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B170" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C170" s="3">
         <v>250</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>341</v>
+        <v>256</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B171" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" s="3">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>342</v>
+        <v>161</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B172" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C172" s="3">
         <v>250</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>161</v>
+        <v>336</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>141</v>
@@ -4741,16 +4783,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B173" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C173" s="3">
         <v>250</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>141</v>
@@ -4758,16 +4800,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B174" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C174" s="3">
         <v>250</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>161</v>
+        <v>338</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>141</v>
@@ -4775,7 +4817,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B175" s="3">
         <v>1</v>
@@ -4784,7 +4826,7 @@
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>141</v>
@@ -4792,7 +4834,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B176" s="3">
         <v>2</v>
@@ -4801,7 +4843,7 @@
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>141</v>
@@ -4809,16 +4851,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B177" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C177" s="3">
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>141</v>
@@ -4826,16 +4868,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B178" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178" s="3">
         <v>250</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>141</v>
@@ -4843,7 +4885,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B179" s="3">
         <v>0</v>
@@ -4860,16 +4902,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B180" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C180" s="3">
         <v>250</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>161</v>
+        <v>343</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>141</v>
@@ -4877,135 +4919,135 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B181" s="5">
-        <v>6</v>
+        <v>150</v>
+      </c>
+      <c r="B181" s="3">
+        <v>0</v>
       </c>
       <c r="C181" s="3">
         <v>250</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E181" s="6" t="s">
-        <v>206</v>
+        <v>161</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>200</v>
-      </c>
-      <c r="B182" s="5">
+      <c r="A182" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B182" s="3">
         <v>1</v>
       </c>
       <c r="C182" s="3">
         <v>250</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E182" s="6" t="s">
-        <v>206</v>
+        <v>344</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>201</v>
-      </c>
-      <c r="B183" s="5">
-        <v>1</v>
-      </c>
-      <c r="C183" s="6">
-        <v>220</v>
+      <c r="A183" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B183" s="3">
+        <v>2</v>
+      </c>
+      <c r="C183" s="3">
+        <v>250</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E183" s="6" t="s">
-        <v>413</v>
+        <v>345</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>326</v>
-      </c>
-      <c r="B184" s="5">
+      <c r="A184" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B184" s="3">
+        <v>1</v>
+      </c>
+      <c r="C184" s="3">
+        <v>250</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B185" s="3">
+        <v>2</v>
+      </c>
+      <c r="C185" s="3">
+        <v>250</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B186" s="3">
         <v>0</v>
       </c>
-      <c r="C184" s="6">
-        <v>220</v>
-      </c>
-      <c r="D184" s="2" t="s">
+      <c r="C186" s="3">
+        <v>250</v>
+      </c>
+      <c r="D186" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E184" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>202</v>
-      </c>
-      <c r="B185" s="5">
-        <v>2</v>
-      </c>
-      <c r="C185" s="6">
-        <v>220</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E185" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>203</v>
-      </c>
-      <c r="B186" s="5">
-        <v>1</v>
-      </c>
-      <c r="C186" s="6">
-        <v>220</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E186" s="6" t="s">
-        <v>413</v>
+      <c r="E186" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>204</v>
-      </c>
-      <c r="B187" s="5">
-        <v>1</v>
-      </c>
-      <c r="C187" s="6">
-        <v>220</v>
+      <c r="A187" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B187" s="3">
+        <v>0</v>
+      </c>
+      <c r="C187" s="3">
+        <v>250</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E187" s="6" t="s">
-        <v>413</v>
+        <v>161</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>205</v>
+      <c r="A188" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="B188" s="5">
-        <v>5</v>
-      </c>
-      <c r="C188" s="6">
-        <v>350</v>
+        <v>6</v>
+      </c>
+      <c r="C188" s="3">
+        <v>250</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>206</v>
@@ -5013,135 +5055,135 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>353</v>
+        <v>200</v>
       </c>
       <c r="B189" s="5">
-        <v>10</v>
-      </c>
-      <c r="C189" s="6">
+        <v>1</v>
+      </c>
+      <c r="C189" s="3">
         <v>250</v>
       </c>
-      <c r="D189" s="4" t="s">
-        <v>357</v>
+      <c r="D189" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>356</v>
+        <v>206</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>354</v>
+        <v>201</v>
       </c>
       <c r="B190" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C190" s="6">
-        <v>250</v>
-      </c>
-      <c r="D190" s="4" t="s">
-        <v>358</v>
+        <v>220</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
       <c r="B191" s="5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C191" s="6">
-        <v>250</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>361</v>
+        <v>220</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>373</v>
+        <v>202</v>
       </c>
       <c r="B192" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C192" s="6">
-        <v>150</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>366</v>
+        <v>220</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>371</v>
+        <v>203</v>
       </c>
       <c r="B193" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C193" s="6">
-        <v>150</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>369</v>
+        <v>220</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>372</v>
+        <v>204</v>
       </c>
       <c r="B194" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C194" s="6">
-        <v>150</v>
-      </c>
-      <c r="D194" s="4" t="s">
-        <v>370</v>
+        <v>220</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>368</v>
+        <v>205</v>
       </c>
       <c r="B195" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C195" s="6">
-        <v>550</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>367</v>
+        <v>350</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>356</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>414</v>
+        <v>353</v>
       </c>
       <c r="B196" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C196" s="6">
-        <v>650</v>
+        <v>250</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>415</v>
+        <v>357</v>
       </c>
       <c r="E196" s="6" t="s">
         <v>356</v>
@@ -5149,75 +5191,75 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B197" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C197" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>161</v>
+        <v>358</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B198" s="5">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C198" s="6">
-        <v>800</v>
+        <v>250</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>206</v>
+        <v>356</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="B199" s="5">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C199" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>206</v>
+        <v>356</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B200" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C200" s="6">
         <v>150</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B201" s="5">
         <v>2</v>
@@ -5226,109 +5268,109 @@
         <v>150</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B202" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C202" s="6">
-        <v>150</v>
+        <v>550</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
       <c r="B203" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C203" s="6">
-        <v>150</v>
+        <v>650</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="B204" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C204" s="6">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>386</v>
+        <v>161</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="B205" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C205" s="6">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>387</v>
+        <v>362</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>381</v>
+        <v>206</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="B206" s="5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C206" s="6">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>381</v>
+        <v>206</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B207" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C207" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="E207" s="6" t="s">
         <v>381</v>
@@ -5336,16 +5378,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B208" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C208" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="E208" s="6" t="s">
         <v>381</v>
@@ -5353,16 +5395,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B209" s="5">
         <v>1</v>
       </c>
       <c r="C209" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="E209" s="6" t="s">
         <v>381</v>
@@ -5370,16 +5412,16 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B210" s="5">
         <v>1</v>
       </c>
       <c r="C210" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="E210" s="6" t="s">
         <v>381</v>
@@ -5387,16 +5429,16 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="B211" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C211" s="6">
-        <v>550</v>
+        <v>30</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="E211" s="6" t="s">
         <v>381</v>
@@ -5404,7 +5446,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B212" s="5">
         <v>1</v>
@@ -5413,7 +5455,7 @@
         <v>550</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="E212" s="6" t="s">
         <v>381</v>
@@ -5421,69 +5463,188 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="B213" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C213" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>206</v>
+        <v>381</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B214" s="5">
         <v>1</v>
       </c>
       <c r="C214" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>206</v>
+        <v>381</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B215" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C215" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>206</v>
+        <v>381</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>392</v>
+      </c>
+      <c r="B216" s="5">
+        <v>1</v>
+      </c>
+      <c r="C216" s="6">
+        <v>550</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E216" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>393</v>
+      </c>
+      <c r="B217" s="5">
+        <v>1</v>
+      </c>
+      <c r="C217" s="6">
+        <v>550</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E217" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>395</v>
+      </c>
+      <c r="B218" s="5">
+        <v>1</v>
+      </c>
+      <c r="C218" s="6">
+        <v>550</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="E218" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>394</v>
+      </c>
+      <c r="B219" s="5">
+        <v>1</v>
+      </c>
+      <c r="C219" s="6">
+        <v>550</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E219" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>403</v>
+      </c>
+      <c r="B220" s="5">
+        <v>6</v>
+      </c>
+      <c r="C220" s="6">
+        <v>250</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="E220" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>404</v>
+      </c>
+      <c r="B221" s="5">
+        <v>1</v>
+      </c>
+      <c r="C221" s="6">
+        <v>250</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E221" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>405</v>
+      </c>
+      <c r="B222" s="5">
+        <v>2</v>
+      </c>
+      <c r="C222" s="6">
+        <v>250</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E222" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>406</v>
       </c>
-      <c r="B216" s="5">
-        <v>1</v>
-      </c>
-      <c r="C216" s="6">
+      <c r="B223" s="5">
+        <v>1</v>
+      </c>
+      <c r="C223" s="6">
         <v>250</v>
       </c>
-      <c r="D216" s="4" t="s">
+      <c r="D223" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="E216" s="6" t="s">
+      <c r="E223" s="6" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dbz + jjk new image update, not stock
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8E6E6F-CB51-4D27-A95C-1E4275DE1772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDFEA3C-BD56-4FF3-A925-24B2287FA6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1455" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="3075" yWindow="1800" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="565">
   <si>
     <t>Product</t>
   </si>
@@ -450,9 +450,6 @@
     <t>Gojo</t>
   </si>
   <si>
-    <t>Sukuna</t>
-  </si>
-  <si>
     <t>Mahito</t>
   </si>
   <si>
@@ -1113,9 +1110,6 @@
     <t>pokemon sticker.jpg</t>
   </si>
   <si>
-    <t>Goku</t>
-  </si>
-  <si>
     <t>DBZ</t>
   </si>
   <si>
@@ -1581,18 +1575,6 @@
     <t>Makora</t>
   </si>
   <si>
-    <t>Sukuna (Multihands)</t>
-  </si>
-  <si>
-    <t>Sukuna (Fushiguro)</t>
-  </si>
-  <si>
-    <t>Gojo 0.5</t>
-  </si>
-  <si>
-    <t>Gojo (Purple Hollow)</t>
-  </si>
-  <si>
     <t>Fushiguro Megumi</t>
   </si>
   <si>
@@ -1608,7 +1590,145 @@
     <t>Yuta</t>
   </si>
   <si>
-    <t>Sukuna (heart)</t>
+    <t>Ryomen Sukuna (True Form)</t>
+  </si>
+  <si>
+    <t>Ryomen Sukuna (Megumi Form)</t>
+  </si>
+  <si>
+    <t>Satoru Gojo (Final Arc)</t>
+  </si>
+  <si>
+    <t>Satoru Gojo (Strongest Form)</t>
+  </si>
+  <si>
+    <t>Ryomen Sukuna (Itadori Form)</t>
+  </si>
+  <si>
+    <t>Itadori Yuji</t>
+  </si>
+  <si>
+    <t>makora.jpg</t>
+  </si>
+  <si>
+    <t>sukuna mult.jpg</t>
+  </si>
+  <si>
+    <t>sukuna fushi.jpg</t>
+  </si>
+  <si>
+    <t>gojo half.jpg</t>
+  </si>
+  <si>
+    <t>gojo purple.jpg</t>
+  </si>
+  <si>
+    <t>megumi.jpg</t>
+  </si>
+  <si>
+    <t>toji.jpg</t>
+  </si>
+  <si>
+    <t>yuki.jpg</t>
+  </si>
+  <si>
+    <t>maki.jpg</t>
+  </si>
+  <si>
+    <t>yuta.jpg</t>
+  </si>
+  <si>
+    <t>sukuna heart.jpg</t>
+  </si>
+  <si>
+    <t>Goku SS4</t>
+  </si>
+  <si>
+    <t>Goku SSG</t>
+  </si>
+  <si>
+    <t>Goku Ultra Instinct</t>
+  </si>
+  <si>
+    <t>Vegeta SSG</t>
+  </si>
+  <si>
+    <t>Son Gohan</t>
+  </si>
+  <si>
+    <t>Jiren Final form</t>
+  </si>
+  <si>
+    <t>Jiren</t>
+  </si>
+  <si>
+    <t>Goku SS2</t>
+  </si>
+  <si>
+    <t>Frieza</t>
+  </si>
+  <si>
+    <t>Birusu</t>
+  </si>
+  <si>
+    <t>Vegeta</t>
+  </si>
+  <si>
+    <t>Hitto</t>
+  </si>
+  <si>
+    <t>Zamasu</t>
+  </si>
+  <si>
+    <t>Majin Buu</t>
+  </si>
+  <si>
+    <t>Piccolo</t>
+  </si>
+  <si>
+    <t>goku ss4.jpg</t>
+  </si>
+  <si>
+    <t>goku ssg.jpg</t>
+  </si>
+  <si>
+    <t>goku ultra instinct.jpg</t>
+  </si>
+  <si>
+    <t>vegeta ssg.jpg</t>
+  </si>
+  <si>
+    <t>son gohan.jpg</t>
+  </si>
+  <si>
+    <t>jiren final form.jpg</t>
+  </si>
+  <si>
+    <t>jiren.jpg</t>
+  </si>
+  <si>
+    <t>goku ss2.jpg</t>
+  </si>
+  <si>
+    <t>frieza.jpg</t>
+  </si>
+  <si>
+    <t>birusu.jpg</t>
+  </si>
+  <si>
+    <t>vegeta.jpg</t>
+  </si>
+  <si>
+    <t>piccolo.jpg</t>
+  </si>
+  <si>
+    <t>majin buu.jpg</t>
+  </si>
+  <si>
+    <t>hitto.jpg</t>
+  </si>
+  <si>
+    <t>zamasu.jpg</t>
   </si>
 </sst>
 </file>
@@ -2130,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E275"/>
+  <dimension ref="A1:E289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204:E215"/>
+    <sheetView tabSelected="1" topLeftCell="A243" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B255" sqref="B255:B269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2291,7 @@
         <v>220</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -2188,7 +2308,7 @@
         <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -2205,7 +2325,7 @@
         <v>350</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -2222,7 +2342,7 @@
         <v>180</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
@@ -2239,7 +2359,7 @@
         <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
@@ -2256,7 +2376,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -2273,7 +2393,7 @@
         <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -2290,7 +2410,7 @@
         <v>200</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
@@ -2298,7 +2418,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -2307,7 +2427,7 @@
         <v>250</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -2315,7 +2435,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -2324,7 +2444,7 @@
         <v>250</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -2332,7 +2452,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -2341,7 +2461,7 @@
         <v>250</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -2349,7 +2469,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -2358,7 +2478,7 @@
         <v>250</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -2366,7 +2486,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -2375,7 +2495,7 @@
         <v>250</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -2383,7 +2503,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2392,7 +2512,7 @@
         <v>250</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -2400,7 +2520,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -2409,7 +2529,7 @@
         <v>250</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -2417,7 +2537,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -2426,7 +2546,7 @@
         <v>250</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
@@ -2434,7 +2554,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
@@ -2443,7 +2563,7 @@
         <v>250</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -2460,7 +2580,7 @@
         <v>220</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -2477,7 +2597,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
@@ -2494,7 +2614,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -2511,7 +2631,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -2528,7 +2648,7 @@
         <v>220</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -2545,7 +2665,7 @@
         <v>220</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -2562,7 +2682,7 @@
         <v>220</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -2579,7 +2699,7 @@
         <v>220</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
@@ -2596,7 +2716,7 @@
         <v>200</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2613,7 +2733,7 @@
         <v>220</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -2630,7 +2750,7 @@
         <v>180</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -2647,7 +2767,7 @@
         <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -2664,7 +2784,7 @@
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -2681,7 +2801,7 @@
         <v>180</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -2698,7 +2818,7 @@
         <v>180</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -2715,7 +2835,7 @@
         <v>180</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2732,7 +2852,7 @@
         <v>180</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2749,7 +2869,7 @@
         <v>270</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2766,7 +2886,7 @@
         <v>270</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -2783,7 +2903,7 @@
         <v>270</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2800,7 +2920,7 @@
         <v>450</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2817,7 +2937,7 @@
         <v>380</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -2834,7 +2954,7 @@
         <v>800</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -2851,7 +2971,7 @@
         <v>270</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -2868,7 +2988,7 @@
         <v>270</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -2885,7 +3005,7 @@
         <v>270</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -2893,7 +3013,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
@@ -2902,7 +3022,7 @@
         <v>250</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -2919,7 +3039,7 @@
         <v>850</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -2927,7 +3047,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
@@ -2936,7 +3056,7 @@
         <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -2944,7 +3064,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B48" s="3">
         <v>2</v>
@@ -2953,7 +3073,7 @@
         <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -2970,7 +3090,7 @@
         <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -2987,7 +3107,7 @@
         <v>250</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -2995,7 +3115,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -3004,7 +3124,7 @@
         <v>250</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -3012,7 +3132,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -3021,7 +3141,7 @@
         <v>250</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -3029,7 +3149,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
@@ -3038,7 +3158,7 @@
         <v>250</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>6</v>
@@ -3046,7 +3166,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B54" s="3">
         <v>2</v>
@@ -3055,7 +3175,7 @@
         <v>360</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>6</v>
@@ -3063,7 +3183,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
@@ -3072,7 +3192,7 @@
         <v>360</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>6</v>
@@ -3080,7 +3200,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B56" s="3">
         <v>2</v>
@@ -3089,7 +3209,7 @@
         <v>200</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>6</v>
@@ -3097,7 +3217,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B57" s="3">
         <v>4</v>
@@ -3106,7 +3226,7 @@
         <v>260</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>6</v>
@@ -3114,7 +3234,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B58" s="3">
         <v>2</v>
@@ -3123,7 +3243,7 @@
         <v>260</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>6</v>
@@ -3131,7 +3251,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B59" s="3">
         <v>2</v>
@@ -3140,7 +3260,7 @@
         <v>260</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>6</v>
@@ -3148,7 +3268,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B60" s="3">
         <v>4</v>
@@ -3157,7 +3277,7 @@
         <v>260</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>6</v>
@@ -3165,7 +3285,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B61" s="3">
         <v>1</v>
@@ -3174,7 +3294,7 @@
         <v>220</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>6</v>
@@ -3182,7 +3302,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B62" s="3">
         <v>0</v>
@@ -3191,7 +3311,7 @@
         <v>250</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>6</v>
@@ -3199,7 +3319,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B63" s="3">
         <v>5</v>
@@ -3208,7 +3328,7 @@
         <v>250</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
@@ -3216,7 +3336,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B64" s="3">
         <v>1</v>
@@ -3225,7 +3345,7 @@
         <v>250</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
@@ -3233,7 +3353,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B65" s="3">
         <v>2</v>
@@ -3242,7 +3362,7 @@
         <v>250</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>6</v>
@@ -3250,7 +3370,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
@@ -3259,7 +3379,7 @@
         <v>250</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>6</v>
@@ -3267,7 +3387,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B67" s="3">
         <v>3</v>
@@ -3276,7 +3396,7 @@
         <v>220</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>6</v>
@@ -3293,7 +3413,7 @@
         <v>180</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>44</v>
@@ -3301,7 +3421,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
@@ -3310,7 +3430,7 @@
         <v>250</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>44</v>
@@ -3327,7 +3447,7 @@
         <v>250</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>44</v>
@@ -3335,7 +3455,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B71" s="3">
         <v>1</v>
@@ -3344,7 +3464,7 @@
         <v>250</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>44</v>
@@ -3361,7 +3481,7 @@
         <v>180</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>44</v>
@@ -3369,7 +3489,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B73" s="3">
         <v>1</v>
@@ -3378,7 +3498,7 @@
         <v>250</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>44</v>
@@ -3386,7 +3506,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
@@ -3395,7 +3515,7 @@
         <v>250</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>44</v>
@@ -3403,7 +3523,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B75" s="3">
         <v>1</v>
@@ -3412,7 +3532,7 @@
         <v>180</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>44</v>
@@ -3420,7 +3540,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B76" s="3">
         <v>1</v>
@@ -3429,7 +3549,7 @@
         <v>180</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>44</v>
@@ -3446,7 +3566,7 @@
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>44</v>
@@ -3463,7 +3583,7 @@
         <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>44</v>
@@ -3480,7 +3600,7 @@
         <v>350</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>44</v>
@@ -3497,7 +3617,7 @@
         <v>350</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>44</v>
@@ -3514,7 +3634,7 @@
         <v>500</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>44</v>
@@ -3522,7 +3642,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B82" s="3">
         <v>4</v>
@@ -3531,7 +3651,7 @@
         <v>220</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>44</v>
@@ -3539,7 +3659,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B83" s="3">
         <v>2</v>
@@ -3548,7 +3668,7 @@
         <v>220</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>44</v>
@@ -3556,7 +3676,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B84" s="6">
         <v>1</v>
@@ -3565,7 +3685,7 @@
         <v>200</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>44</v>
@@ -3573,7 +3693,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B85" s="3">
         <v>2</v>
@@ -3582,7 +3702,7 @@
         <v>220</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>44</v>
@@ -3590,7 +3710,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B86" s="3">
         <v>1</v>
@@ -3599,7 +3719,7 @@
         <v>250</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>44</v>
@@ -3607,7 +3727,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B87" s="3">
         <v>1</v>
@@ -3616,7 +3736,7 @@
         <v>250</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>44</v>
@@ -3624,7 +3744,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B88" s="3">
         <v>3</v>
@@ -3633,7 +3753,7 @@
         <v>220</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>44</v>
@@ -3650,7 +3770,7 @@
         <v>350</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>44</v>
@@ -3667,7 +3787,7 @@
         <v>350</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>44</v>
@@ -3684,7 +3804,7 @@
         <v>350</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>44</v>
@@ -3701,7 +3821,7 @@
         <v>500</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>44</v>
@@ -3718,7 +3838,7 @@
         <v>500</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>44</v>
@@ -3735,7 +3855,7 @@
         <v>300</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>58</v>
@@ -3743,7 +3863,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" s="3">
         <v>2</v>
@@ -3752,7 +3872,7 @@
         <v>300</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>58</v>
@@ -3769,7 +3889,7 @@
         <v>300</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>58</v>
@@ -3786,7 +3906,7 @@
         <v>300</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>58</v>
@@ -3803,7 +3923,7 @@
         <v>300</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>58</v>
@@ -3820,7 +3940,7 @@
         <v>270</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>58</v>
@@ -3837,7 +3957,7 @@
         <v>270</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>58</v>
@@ -3854,7 +3974,7 @@
         <v>300</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>58</v>
@@ -3871,7 +3991,7 @@
         <v>300</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>58</v>
@@ -3888,7 +4008,7 @@
         <v>300</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>58</v>
@@ -3896,7 +4016,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B104" s="3">
         <v>1</v>
@@ -3905,7 +4025,7 @@
         <v>300</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>58</v>
@@ -3922,7 +4042,7 @@
         <v>300</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>58</v>
@@ -3939,7 +4059,7 @@
         <v>300</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>58</v>
@@ -3947,7 +4067,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B107" s="3">
         <v>2</v>
@@ -3956,7 +4076,7 @@
         <v>350</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>58</v>
@@ -3973,7 +4093,7 @@
         <v>300</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>58</v>
@@ -3990,7 +4110,7 @@
         <v>300</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>58</v>
@@ -4007,7 +4127,7 @@
         <v>300</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>58</v>
@@ -4024,7 +4144,7 @@
         <v>300</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>58</v>
@@ -4041,7 +4161,7 @@
         <v>300</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>58</v>
@@ -4058,7 +4178,7 @@
         <v>300</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>58</v>
@@ -4075,7 +4195,7 @@
         <v>300</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>58</v>
@@ -4083,7 +4203,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B115" s="3">
         <v>1</v>
@@ -4092,7 +4212,7 @@
         <v>300</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>58</v>
@@ -4100,7 +4220,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B116" s="3">
         <v>2</v>
@@ -4109,7 +4229,7 @@
         <v>350</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>58</v>
@@ -4117,7 +4237,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B117" s="3">
         <v>1</v>
@@ -4126,7 +4246,7 @@
         <v>350</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>58</v>
@@ -4143,7 +4263,7 @@
         <v>350</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>58</v>
@@ -4160,7 +4280,7 @@
         <v>350</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>58</v>
@@ -4177,7 +4297,7 @@
         <v>320</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>58</v>
@@ -4194,7 +4314,7 @@
         <v>320</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>58</v>
@@ -4211,7 +4331,7 @@
         <v>320</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>58</v>
@@ -4228,7 +4348,7 @@
         <v>320</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>58</v>
@@ -4245,7 +4365,7 @@
         <v>320</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>58</v>
@@ -4262,7 +4382,7 @@
         <v>320</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>58</v>
@@ -4279,7 +4399,7 @@
         <v>320</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>58</v>
@@ -4296,7 +4416,7 @@
         <v>320</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>58</v>
@@ -4313,7 +4433,7 @@
         <v>320</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>58</v>
@@ -4330,7 +4450,7 @@
         <v>320</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>58</v>
@@ -4347,7 +4467,7 @@
         <v>320</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>58</v>
@@ -4364,7 +4484,7 @@
         <v>320</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>58</v>
@@ -4381,7 +4501,7 @@
         <v>320</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>58</v>
@@ -4398,7 +4518,7 @@
         <v>320</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>58</v>
@@ -4415,7 +4535,7 @@
         <v>320</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>58</v>
@@ -4423,7 +4543,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B135" s="3">
         <v>1</v>
@@ -4432,7 +4552,7 @@
         <v>320</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>58</v>
@@ -4449,7 +4569,7 @@
         <v>300</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>58</v>
@@ -4466,7 +4586,7 @@
         <v>300</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>58</v>
@@ -4483,7 +4603,7 @@
         <v>300</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>58</v>
@@ -4500,7 +4620,7 @@
         <v>300</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>58</v>
@@ -4517,7 +4637,7 @@
         <v>300</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>58</v>
@@ -4534,7 +4654,7 @@
         <v>300</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>58</v>
@@ -4551,7 +4671,7 @@
         <v>300</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>58</v>
@@ -4568,7 +4688,7 @@
         <v>300</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>58</v>
@@ -4585,7 +4705,7 @@
         <v>300</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>58</v>
@@ -4602,7 +4722,7 @@
         <v>300</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>58</v>
@@ -4619,7 +4739,7 @@
         <v>300</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>58</v>
@@ -4636,7 +4756,7 @@
         <v>400</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>58</v>
@@ -4653,7 +4773,7 @@
         <v>400</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>58</v>
@@ -4661,7 +4781,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B149" s="3">
         <v>3</v>
@@ -4670,7 +4790,7 @@
         <v>300</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>58</v>
@@ -4687,7 +4807,7 @@
         <v>300</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>58</v>
@@ -4704,7 +4824,7 @@
         <v>300</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>58</v>
@@ -4721,7 +4841,7 @@
         <v>300</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>58</v>
@@ -4738,7 +4858,7 @@
         <v>300</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>58</v>
@@ -4755,7 +4875,7 @@
         <v>300</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>58</v>
@@ -4772,7 +4892,7 @@
         <v>300</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>58</v>
@@ -4789,7 +4909,7 @@
         <v>500</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>58</v>
@@ -4797,7 +4917,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B157" s="3">
         <v>1</v>
@@ -4806,7 +4926,7 @@
         <v>280</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>58</v>
@@ -4814,7 +4934,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
@@ -4823,7 +4943,7 @@
         <v>280</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>58</v>
@@ -4831,7 +4951,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B159" s="3">
         <v>1</v>
@@ -4840,7 +4960,7 @@
         <v>280</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>58</v>
@@ -4857,7 +4977,7 @@
         <v>300</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>58</v>
@@ -4874,7 +4994,7 @@
         <v>300</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>58</v>
@@ -4891,7 +5011,7 @@
         <v>250</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>116</v>
@@ -4899,7 +5019,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B163" s="3">
         <v>1</v>
@@ -4908,7 +5028,7 @@
         <v>280</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>116</v>
@@ -4916,7 +5036,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B164" s="3">
         <v>1</v>
@@ -4925,7 +5045,7 @@
         <v>280</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>116</v>
@@ -4933,7 +5053,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B165" s="3">
         <v>2</v>
@@ -4942,7 +5062,7 @@
         <v>260</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>116</v>
@@ -4950,7 +5070,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B166" s="3">
         <v>1</v>
@@ -4959,7 +5079,7 @@
         <v>260</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>116</v>
@@ -4976,7 +5096,7 @@
         <v>500</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>116</v>
@@ -4984,7 +5104,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B168" s="3">
         <v>1</v>
@@ -4993,7 +5113,7 @@
         <v>280</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>116</v>
@@ -5010,7 +5130,7 @@
         <v>220</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>116</v>
@@ -5027,7 +5147,7 @@
         <v>220</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>116</v>
@@ -5044,7 +5164,7 @@
         <v>220</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>116</v>
@@ -5061,7 +5181,7 @@
         <v>220</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>116</v>
@@ -5078,7 +5198,7 @@
         <v>220</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>116</v>
@@ -5095,7 +5215,7 @@
         <v>250</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>116</v>
@@ -5103,7 +5223,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B175" s="3">
         <v>2</v>
@@ -5112,7 +5232,7 @@
         <v>220</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>116</v>
@@ -5120,7 +5240,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B176" s="3">
         <v>3</v>
@@ -5129,7 +5249,7 @@
         <v>250</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>116</v>
@@ -5137,7 +5257,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B177" s="3">
         <v>1</v>
@@ -5146,7 +5266,7 @@
         <v>220</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>116</v>
@@ -5163,7 +5283,7 @@
         <v>220</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>116</v>
@@ -5171,7 +5291,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B179" s="3">
         <v>2</v>
@@ -5180,7 +5300,7 @@
         <v>250</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>116</v>
@@ -5197,7 +5317,7 @@
         <v>220</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>116</v>
@@ -5214,7 +5334,7 @@
         <v>220</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>116</v>
@@ -5231,7 +5351,7 @@
         <v>350</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>116</v>
@@ -5248,7 +5368,7 @@
         <v>350</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>116</v>
@@ -5265,7 +5385,7 @@
         <v>350</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>116</v>
@@ -5282,7 +5402,7 @@
         <v>350</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>116</v>
@@ -5299,7 +5419,7 @@
         <v>350</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>116</v>
@@ -5316,7 +5436,7 @@
         <v>350</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>116</v>
@@ -5333,7 +5453,7 @@
         <v>220</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>116</v>
@@ -5341,7 +5461,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B189" s="3">
         <v>1</v>
@@ -5350,7 +5470,7 @@
         <v>220</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>116</v>
@@ -5358,7 +5478,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B190" s="3">
         <v>1</v>
@@ -5367,7 +5487,7 @@
         <v>220</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>116</v>
@@ -5375,7 +5495,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B191" s="3">
         <v>1</v>
@@ -5384,7 +5504,7 @@
         <v>220</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>116</v>
@@ -5392,7 +5512,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B192" s="3">
         <v>1</v>
@@ -5401,7 +5521,7 @@
         <v>250</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>116</v>
@@ -5409,7 +5529,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B193" s="3">
         <v>2</v>
@@ -5418,7 +5538,7 @@
         <v>250</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>116</v>
@@ -5435,7 +5555,7 @@
         <v>220</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>116</v>
@@ -5443,7 +5563,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B195" s="3">
         <v>1</v>
@@ -5452,7 +5572,7 @@
         <v>220</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>116</v>
@@ -5460,7 +5580,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B196" s="3">
         <v>1</v>
@@ -5469,7 +5589,7 @@
         <v>250</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>116</v>
@@ -5477,7 +5597,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B197" s="3">
         <v>1</v>
@@ -5486,7 +5606,7 @@
         <v>250</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>116</v>
@@ -5494,7 +5614,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B198" s="3">
         <v>1</v>
@@ -5503,7 +5623,7 @@
         <v>250</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>116</v>
@@ -5511,7 +5631,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B199" s="3">
         <v>1</v>
@@ -5520,7 +5640,7 @@
         <v>250</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>116</v>
@@ -5537,7 +5657,7 @@
         <v>250</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>135</v>
@@ -5554,7 +5674,7 @@
         <v>460</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>135</v>
@@ -5571,7 +5691,7 @@
         <v>250</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>135</v>
@@ -5579,7 +5699,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>138</v>
+        <v>523</v>
       </c>
       <c r="B203" s="3">
         <v>4</v>
@@ -5588,7 +5708,7 @@
         <v>250</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>135</v>
@@ -5596,7 +5716,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B204" s="3">
         <v>0</v>
@@ -5605,7 +5725,7 @@
         <v>240</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>135</v>
@@ -5613,7 +5733,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B205" s="3">
         <v>0</v>
@@ -5622,7 +5742,7 @@
         <v>400</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>161</v>
+        <v>524</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>135</v>
@@ -5630,7 +5750,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="B206" s="3">
         <v>0</v>
@@ -5639,7 +5759,7 @@
         <v>400</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>161</v>
+        <v>525</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>135</v>
@@ -5647,7 +5767,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B207" s="3">
         <v>0</v>
@@ -5656,7 +5776,7 @@
         <v>350</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>161</v>
+        <v>526</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>135</v>
@@ -5664,7 +5784,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B208" s="3">
         <v>0</v>
@@ -5673,7 +5793,7 @@
         <v>400</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>161</v>
+        <v>527</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>135</v>
@@ -5681,7 +5801,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B209" s="3">
         <v>0</v>
@@ -5690,7 +5810,7 @@
         <v>350</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>161</v>
+        <v>528</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>135</v>
@@ -5698,7 +5818,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B210" s="3">
         <v>0</v>
@@ -5707,7 +5827,7 @@
         <v>350</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>161</v>
+        <v>529</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>135</v>
@@ -5715,7 +5835,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B211" s="3">
         <v>0</v>
@@ -5724,7 +5844,7 @@
         <v>400</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>161</v>
+        <v>530</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>135</v>
@@ -5732,7 +5852,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="B212" s="3">
         <v>0</v>
@@ -5741,7 +5861,7 @@
         <v>350</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>161</v>
+        <v>531</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>135</v>
@@ -5749,7 +5869,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B213" s="3">
         <v>0</v>
@@ -5758,7 +5878,7 @@
         <v>350</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>161</v>
+        <v>532</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>135</v>
@@ -5766,7 +5886,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="B214" s="3">
         <v>0</v>
@@ -5775,7 +5895,7 @@
         <v>350</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>161</v>
+        <v>533</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>135</v>
@@ -5783,7 +5903,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B215" s="3">
         <v>0</v>
@@ -5792,7 +5912,7 @@
         <v>350</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>161</v>
+        <v>534</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>135</v>
@@ -5800,7 +5920,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B216" s="3">
         <v>3</v>
@@ -5809,15 +5929,15 @@
         <v>250</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B217" s="3">
         <v>3</v>
@@ -5826,15 +5946,15 @@
         <v>250</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B218" s="3">
         <v>1</v>
@@ -5843,15 +5963,15 @@
         <v>250</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B219" s="3">
         <v>1</v>
@@ -5860,15 +5980,15 @@
         <v>250</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B220" s="3">
         <v>2</v>
@@ -5877,15 +5997,15 @@
         <v>250</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B221" s="3">
         <v>2</v>
@@ -5894,15 +6014,15 @@
         <v>250</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B222" s="3">
         <v>1</v>
@@ -5911,15 +6031,15 @@
         <v>250</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B223" s="3">
         <v>0</v>
@@ -5928,15 +6048,15 @@
         <v>250</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B224" s="3">
         <v>2</v>
@@ -5945,15 +6065,15 @@
         <v>250</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B225" s="3">
         <v>0</v>
@@ -5962,15 +6082,15 @@
         <v>250</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B226" s="3">
         <v>1</v>
@@ -5979,15 +6099,15 @@
         <v>250</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B227" s="3">
         <v>2</v>
@@ -5996,15 +6116,15 @@
         <v>250</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B228" s="3">
         <v>1</v>
@@ -6013,15 +6133,15 @@
         <v>250</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B229" s="3">
         <v>2</v>
@@ -6030,15 +6150,15 @@
         <v>250</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B230" s="3">
         <v>0</v>
@@ -6047,15 +6167,15 @@
         <v>250</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B231" s="3">
         <v>0</v>
@@ -6064,15 +6184,15 @@
         <v>250</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B232" s="3">
         <v>4</v>
@@ -6081,15 +6201,15 @@
         <v>250</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B233" s="3">
         <v>2</v>
@@ -6098,15 +6218,15 @@
         <v>250</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B234" s="3">
         <v>1</v>
@@ -6115,15 +6235,15 @@
         <v>220</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B235" s="3">
         <v>1</v>
@@ -6132,15 +6252,15 @@
         <v>220</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B236" s="3">
         <v>1</v>
@@ -6149,15 +6269,15 @@
         <v>220</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B237" s="3">
         <v>2</v>
@@ -6166,15 +6286,15 @@
         <v>220</v>
       </c>
       <c r="D237" s="8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B238" s="3">
         <v>1</v>
@@ -6183,15 +6303,15 @@
         <v>160</v>
       </c>
       <c r="D238" s="8" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B239" s="5">
         <v>6</v>
@@ -6200,15 +6320,15 @@
         <v>250</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B240" s="5">
         <v>1</v>
@@ -6217,15 +6337,15 @@
         <v>250</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B241" s="5">
         <v>1</v>
@@ -6234,15 +6354,15 @@
         <v>220</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B242" s="5">
         <v>0</v>
@@ -6251,15 +6371,15 @@
         <v>220</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B243" s="5">
         <v>2</v>
@@ -6268,15 +6388,15 @@
         <v>220</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B244" s="5">
         <v>1</v>
@@ -6285,15 +6405,15 @@
         <v>220</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B245" s="5">
         <v>1</v>
@@ -6302,15 +6422,15 @@
         <v>220</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B246" s="5">
         <v>5</v>
@@ -6319,15 +6439,15 @@
         <v>350</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E246" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B247" s="5">
         <v>10</v>
@@ -6336,15 +6456,15 @@
         <v>250</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B248" s="5">
         <v>1</v>
@@ -6353,15 +6473,15 @@
         <v>250</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E248" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B249" s="5">
         <v>24</v>
@@ -6370,15 +6490,15 @@
         <v>250</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B250" s="5">
         <v>6</v>
@@ -6387,15 +6507,15 @@
         <v>150</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B251" s="5">
         <v>2</v>
@@ -6404,15 +6524,15 @@
         <v>150</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E251" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B252" s="5">
         <v>2</v>
@@ -6421,15 +6541,15 @@
         <v>150</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E252" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B253" s="5">
         <v>2</v>
@@ -6438,15 +6558,15 @@
         <v>550</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E253" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B254" s="5">
         <v>2</v>
@@ -6455,15 +6575,15 @@
         <v>650</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E254" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>359</v>
+        <v>535</v>
       </c>
       <c r="B255" s="5">
         <v>0</v>
@@ -6472,350 +6592,588 @@
         <v>300</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>161</v>
+        <v>550</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>363</v>
+        <v>536</v>
       </c>
       <c r="B256" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C256" s="6">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>361</v>
+        <v>551</v>
       </c>
       <c r="E256" s="6" t="s">
-        <v>206</v>
+        <v>358</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>364</v>
+        <v>537</v>
       </c>
       <c r="B257" s="5">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C257" s="6">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>362</v>
+        <v>552</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>206</v>
+        <v>358</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>375</v>
+        <v>538</v>
       </c>
       <c r="B258" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C258" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>382</v>
+        <v>553</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>376</v>
+        <v>539</v>
       </c>
       <c r="B259" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C259" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>383</v>
+        <v>554</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>377</v>
+        <v>540</v>
       </c>
       <c r="B260" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C260" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>384</v>
+        <v>555</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>378</v>
+        <v>541</v>
       </c>
       <c r="B261" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C261" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>401</v>
+        <v>556</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>379</v>
+        <v>542</v>
       </c>
       <c r="B262" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C262" s="6">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>385</v>
+        <v>557</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>381</v>
+        <v>543</v>
       </c>
       <c r="B263" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C263" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>386</v>
+        <v>558</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>387</v>
+        <v>544</v>
       </c>
       <c r="B264" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C264" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>388</v>
+        <v>559</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>389</v>
+        <v>545</v>
       </c>
       <c r="B265" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C265" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>395</v>
+        <v>560</v>
       </c>
       <c r="E265" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>390</v>
+        <v>549</v>
       </c>
       <c r="B266" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C266" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>396</v>
+        <v>561</v>
       </c>
       <c r="E266" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>391</v>
+        <v>548</v>
       </c>
       <c r="B267" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C267" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>397</v>
+        <v>562</v>
       </c>
       <c r="E267" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>392</v>
+        <v>546</v>
       </c>
       <c r="B268" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C268" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>398</v>
+        <v>563</v>
       </c>
       <c r="E268" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>394</v>
+        <v>547</v>
       </c>
       <c r="B269" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C269" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>399</v>
+        <v>564</v>
       </c>
       <c r="E269" s="6" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>393</v>
+        <v>361</v>
       </c>
       <c r="B270" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C270" s="6">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>380</v>
+        <v>205</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="B271" s="5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C271" s="6">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>406</v>
+        <v>360</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>403</v>
+        <v>373</v>
       </c>
       <c r="B272" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C272" s="6">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="E272" s="6" t="s">
-        <v>206</v>
+        <v>378</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>404</v>
+        <v>374</v>
       </c>
       <c r="B273" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C273" s="6">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="E273" s="6" t="s">
-        <v>206</v>
+        <v>378</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="B274" s="5">
         <v>1</v>
       </c>
       <c r="C274" s="6">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="E274" s="6" t="s">
-        <v>206</v>
+        <v>378</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>513</v>
+        <v>376</v>
       </c>
       <c r="B275" s="5">
+        <v>1</v>
+      </c>
+      <c r="C275" s="6">
+        <v>150</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E275" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>377</v>
+      </c>
+      <c r="B276" s="5">
+        <v>10</v>
+      </c>
+      <c r="C276" s="6">
+        <v>30</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E276" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>379</v>
+      </c>
+      <c r="B277" s="5">
+        <v>1</v>
+      </c>
+      <c r="C277" s="6">
+        <v>550</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E277" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>385</v>
+      </c>
+      <c r="B278" s="5">
+        <v>1</v>
+      </c>
+      <c r="C278" s="6">
+        <v>550</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E278" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>387</v>
+      </c>
+      <c r="B279" s="5">
+        <v>1</v>
+      </c>
+      <c r="C279" s="6">
+        <v>550</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E279" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>388</v>
+      </c>
+      <c r="B280" s="5">
+        <v>1</v>
+      </c>
+      <c r="C280" s="6">
+        <v>550</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E280" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>389</v>
+      </c>
+      <c r="B281" s="5">
+        <v>1</v>
+      </c>
+      <c r="C281" s="6">
+        <v>550</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E281" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>390</v>
+      </c>
+      <c r="B282" s="5">
+        <v>1</v>
+      </c>
+      <c r="C282" s="6">
+        <v>550</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E282" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>392</v>
+      </c>
+      <c r="B283" s="5">
+        <v>1</v>
+      </c>
+      <c r="C283" s="6">
+        <v>550</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E283" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>391</v>
+      </c>
+      <c r="B284" s="5">
+        <v>1</v>
+      </c>
+      <c r="C284" s="6">
+        <v>550</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E284" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>400</v>
+      </c>
+      <c r="B285" s="5">
+        <v>2</v>
+      </c>
+      <c r="C285" s="6">
+        <v>250</v>
+      </c>
+      <c r="D285" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E285" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>401</v>
+      </c>
+      <c r="B286" s="5">
+        <v>1</v>
+      </c>
+      <c r="C286" s="6">
+        <v>250</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E286" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>402</v>
+      </c>
+      <c r="B287" s="5">
+        <v>0</v>
+      </c>
+      <c r="C287" s="6">
+        <v>250</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E287" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>403</v>
+      </c>
+      <c r="B288" s="5">
+        <v>1</v>
+      </c>
+      <c r="C288" s="6">
+        <v>250</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="E288" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>511</v>
+      </c>
+      <c r="B289" s="5">
         <v>4</v>
       </c>
-      <c r="C275" s="6">
+      <c r="C289" s="6">
         <v>220</v>
       </c>
-      <c r="D275" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="E275" s="6" t="s">
-        <v>206</v>
+      <c r="D289" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="E289" s="6" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock update [kunai, jjk, dbz]
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76346AA-EDF6-4587-8FB7-1F52C8E66C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE794A2-F617-4067-81BC-BB0297240F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="2730" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="2505" yWindow="2220" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="571">
   <si>
     <t>Product</t>
   </si>
@@ -1735,6 +1735,18 @@
   </si>
   <si>
     <t>Spiderman [Symbiote Suit]</t>
+  </si>
+  <si>
+    <t>Hiraishin Kunai [Metal]</t>
+  </si>
+  <si>
+    <t>Kunai [Metal]</t>
+  </si>
+  <si>
+    <t>kunai.jpg</t>
+  </si>
+  <si>
+    <t>minato kunai.jpg</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1811,6 +1823,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2256,10 +2271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E290"/>
+  <dimension ref="A1:E292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D292" sqref="D292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5759,7 +5774,7 @@
         <v>486</v>
       </c>
       <c r="B206" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C206" s="3">
         <v>400</v>
@@ -5776,7 +5791,7 @@
         <v>556</v>
       </c>
       <c r="B207" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C207" s="3">
         <v>400</v>
@@ -5793,7 +5808,7 @@
         <v>557</v>
       </c>
       <c r="B208" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C208" s="3">
         <v>350</v>
@@ -5810,7 +5825,7 @@
         <v>558</v>
       </c>
       <c r="B209" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C209" s="3">
         <v>400</v>
@@ -5827,7 +5842,7 @@
         <v>559</v>
       </c>
       <c r="B210" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C210" s="3">
         <v>350</v>
@@ -5844,7 +5859,7 @@
         <v>487</v>
       </c>
       <c r="B211" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C211" s="3">
         <v>350</v>
@@ -5861,7 +5876,7 @@
         <v>488</v>
       </c>
       <c r="B212" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C212" s="3">
         <v>400</v>
@@ -5878,7 +5893,7 @@
         <v>489</v>
       </c>
       <c r="B213" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C213" s="3">
         <v>350</v>
@@ -5895,7 +5910,7 @@
         <v>490</v>
       </c>
       <c r="B214" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C214" s="3">
         <v>350</v>
@@ -5929,7 +5944,7 @@
         <v>560</v>
       </c>
       <c r="B216" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C216" s="3">
         <v>350</v>
@@ -6609,7 +6624,7 @@
         <v>504</v>
       </c>
       <c r="B256" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C256" s="6">
         <v>300</v>
@@ -6626,7 +6641,7 @@
         <v>505</v>
       </c>
       <c r="B257" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C257" s="6">
         <v>300</v>
@@ -6643,7 +6658,7 @@
         <v>506</v>
       </c>
       <c r="B258" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C258" s="6">
         <v>300</v>
@@ -6660,7 +6675,7 @@
         <v>507</v>
       </c>
       <c r="B259" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C259" s="6">
         <v>300</v>
@@ -6677,7 +6692,7 @@
         <v>508</v>
       </c>
       <c r="B260" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C260" s="6">
         <v>300</v>
@@ -6694,7 +6709,7 @@
         <v>509</v>
       </c>
       <c r="B261" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C261" s="6">
         <v>300</v>
@@ -6711,7 +6726,7 @@
         <v>510</v>
       </c>
       <c r="B262" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C262" s="6">
         <v>300</v>
@@ -6728,7 +6743,7 @@
         <v>511</v>
       </c>
       <c r="B263" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C263" s="6">
         <v>300</v>
@@ -6745,7 +6760,7 @@
         <v>512</v>
       </c>
       <c r="B264" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C264" s="6">
         <v>300</v>
@@ -6762,7 +6777,7 @@
         <v>513</v>
       </c>
       <c r="B265" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C265" s="6">
         <v>300</v>
@@ -6779,7 +6794,7 @@
         <v>514</v>
       </c>
       <c r="B266" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C266" s="6">
         <v>300</v>
@@ -6796,7 +6811,7 @@
         <v>518</v>
       </c>
       <c r="B267" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C267" s="6">
         <v>300</v>
@@ -6813,7 +6828,7 @@
         <v>517</v>
       </c>
       <c r="B268" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C268" s="6">
         <v>300</v>
@@ -7196,6 +7211,40 @@
         <v>484</v>
       </c>
       <c r="E290" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>568</v>
+      </c>
+      <c r="B291" s="5">
+        <v>2</v>
+      </c>
+      <c r="C291" s="9">
+        <v>1200</v>
+      </c>
+      <c r="D291" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="E291" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>567</v>
+      </c>
+      <c r="B292" s="5">
+        <v>2</v>
+      </c>
+      <c r="C292" s="9">
+        <v>1200</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="E292" s="6" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
STAR WARS NEW ADDED
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE794A2-F617-4067-81BC-BB0297240F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF4F431-C2E3-4964-81AC-EF9D3F91639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="2220" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="587">
   <si>
     <t>Product</t>
   </si>
@@ -1747,6 +1747,54 @@
   </si>
   <si>
     <t>minato kunai.jpg</t>
+  </si>
+  <si>
+    <t>Darth Vader v2</t>
+  </si>
+  <si>
+    <t>Darth Vader Hologram</t>
+  </si>
+  <si>
+    <t>Mandalorian v2</t>
+  </si>
+  <si>
+    <t>Inferno Squad Agent</t>
+  </si>
+  <si>
+    <t>Luke Skywalker Hood</t>
+  </si>
+  <si>
+    <t>C-3P0</t>
+  </si>
+  <si>
+    <t>General Grievous</t>
+  </si>
+  <si>
+    <t>Obi-wan Kenobi</t>
+  </si>
+  <si>
+    <t>darth v2.jpg</t>
+  </si>
+  <si>
+    <t>darth holo.jpg</t>
+  </si>
+  <si>
+    <t>manda2.jpg</t>
+  </si>
+  <si>
+    <t>inferno.jpg</t>
+  </si>
+  <si>
+    <t>luke2.jpg</t>
+  </si>
+  <si>
+    <t>c3p0.jpg</t>
+  </si>
+  <si>
+    <t>grievous.jpg</t>
+  </si>
+  <si>
+    <t>obiwan.jpg</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1823,9 +1871,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2271,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E292"/>
+  <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D292" sqref="D292"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D248" sqref="D248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,7 +3898,7 @@
         <v>46</v>
       </c>
       <c r="B93" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" s="3">
         <v>500</v>
@@ -4465,7 +4510,7 @@
         <v>76</v>
       </c>
       <c r="B129" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129" s="3">
         <v>320</v>
@@ -4788,7 +4833,7 @@
         <v>94</v>
       </c>
       <c r="B148" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C148" s="3">
         <v>400</v>
@@ -6348,425 +6393,425 @@
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B240" s="5">
-        <v>5</v>
+      <c r="A240" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="B240" s="3">
+        <v>1</v>
       </c>
       <c r="C240" s="3">
         <v>250</v>
       </c>
-      <c r="D240" s="2" t="s">
-        <v>244</v>
+      <c r="D240" s="8" t="s">
+        <v>579</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>193</v>
+        <v>455</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>187</v>
-      </c>
-      <c r="B241" s="5">
+      <c r="A241" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="B241" s="3">
         <v>1</v>
       </c>
       <c r="C241" s="3">
         <v>250</v>
       </c>
-      <c r="D241" s="2" t="s">
-        <v>311</v>
+      <c r="D241" s="8" t="s">
+        <v>580</v>
       </c>
       <c r="E241" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="B242" s="3">
+        <v>1</v>
+      </c>
+      <c r="C242" s="3">
+        <v>220</v>
+      </c>
+      <c r="D242" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="E242" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="B243" s="3">
+        <v>1</v>
+      </c>
+      <c r="C243" s="3">
+        <v>220</v>
+      </c>
+      <c r="D243" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="E243" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B244" s="3">
+        <v>1</v>
+      </c>
+      <c r="C244" s="3">
+        <v>220</v>
+      </c>
+      <c r="D244" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="E244" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="B245" s="3">
+        <v>1</v>
+      </c>
+      <c r="C245" s="3">
+        <v>250</v>
+      </c>
+      <c r="D245" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="E245" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B246" s="3">
+        <v>1</v>
+      </c>
+      <c r="C246" s="3">
+        <v>250</v>
+      </c>
+      <c r="D246" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="E246" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="B247" s="3">
+        <v>1</v>
+      </c>
+      <c r="C247" s="3">
+        <v>220</v>
+      </c>
+      <c r="D247" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="E247" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B248" s="5">
+        <v>5</v>
+      </c>
+      <c r="C248" s="3">
+        <v>250</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E248" s="6" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>188</v>
-      </c>
-      <c r="B242" s="5">
-        <v>1</v>
-      </c>
-      <c r="C242" s="6">
-        <v>220</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E242" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>310</v>
-      </c>
-      <c r="B243" s="5">
-        <v>0</v>
-      </c>
-      <c r="C243" s="6">
-        <v>220</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E243" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>189</v>
-      </c>
-      <c r="B244" s="5">
-        <v>2</v>
-      </c>
-      <c r="C244" s="6">
-        <v>220</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E244" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>190</v>
-      </c>
-      <c r="B245" s="5">
-        <v>1</v>
-      </c>
-      <c r="C245" s="6">
-        <v>220</v>
-      </c>
-      <c r="D245" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E245" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>191</v>
-      </c>
-      <c r="B246" s="5">
-        <v>1</v>
-      </c>
-      <c r="C246" s="6">
-        <v>220</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E246" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>192</v>
-      </c>
-      <c r="B247" s="5">
-        <v>5</v>
-      </c>
-      <c r="C247" s="6">
-        <v>350</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E247" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>337</v>
-      </c>
-      <c r="B248" s="5">
-        <v>10</v>
-      </c>
-      <c r="C248" s="6">
-        <v>250</v>
-      </c>
-      <c r="D248" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="E248" s="6" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>338</v>
+        <v>187</v>
       </c>
       <c r="B249" s="5">
         <v>1</v>
       </c>
-      <c r="C249" s="6">
+      <c r="C249" s="3">
         <v>250</v>
       </c>
-      <c r="D249" s="4" t="s">
-        <v>342</v>
+      <c r="D249" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>413</v>
+        <v>193</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>339</v>
+        <v>188</v>
       </c>
       <c r="B250" s="5">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C250" s="6">
-        <v>250</v>
-      </c>
-      <c r="D250" s="4" t="s">
-        <v>414</v>
+        <v>220</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>355</v>
+        <v>310</v>
       </c>
       <c r="B251" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C251" s="6">
-        <v>150</v>
-      </c>
-      <c r="D251" s="4" t="s">
-        <v>348</v>
+        <v>220</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="E251" s="6" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>353</v>
+        <v>189</v>
       </c>
       <c r="B252" s="5">
         <v>2</v>
       </c>
       <c r="C252" s="6">
-        <v>150</v>
-      </c>
-      <c r="D252" s="4" t="s">
-        <v>351</v>
+        <v>220</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="E252" s="6" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>354</v>
+        <v>190</v>
       </c>
       <c r="B253" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C253" s="6">
-        <v>150</v>
-      </c>
-      <c r="D253" s="4" t="s">
-        <v>352</v>
+        <v>220</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="E253" s="6" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>350</v>
+        <v>191</v>
       </c>
       <c r="B254" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C254" s="6">
-        <v>550</v>
-      </c>
-      <c r="D254" s="4" t="s">
-        <v>349</v>
+        <v>220</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="E254" s="6" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>396</v>
+        <v>192</v>
       </c>
       <c r="B255" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C255" s="6">
-        <v>650</v>
-      </c>
-      <c r="D255" s="4" t="s">
-        <v>397</v>
+        <v>350</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>340</v>
+        <v>193</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>504</v>
+        <v>337</v>
       </c>
       <c r="B256" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C256" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>519</v>
+        <v>341</v>
       </c>
       <c r="E256" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>505</v>
+        <v>338</v>
       </c>
       <c r="B257" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C257" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>520</v>
+        <v>342</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>343</v>
+        <v>413</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>506</v>
+        <v>339</v>
       </c>
       <c r="B258" s="5">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C258" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>521</v>
+        <v>414</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>507</v>
+        <v>355</v>
       </c>
       <c r="B259" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C259" s="6">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>522</v>
+        <v>348</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>508</v>
+        <v>353</v>
       </c>
       <c r="B260" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C260" s="6">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>523</v>
+        <v>351</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>509</v>
+        <v>354</v>
       </c>
       <c r="B261" s="5">
         <v>2</v>
       </c>
       <c r="C261" s="6">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>524</v>
+        <v>352</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>510</v>
+        <v>350</v>
       </c>
       <c r="B262" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C262" s="6">
-        <v>300</v>
+        <v>550</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>525</v>
+        <v>349</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>511</v>
+        <v>396</v>
       </c>
       <c r="B263" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C263" s="6">
-        <v>300</v>
+        <v>650</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>526</v>
+        <v>397</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="B264" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C264" s="6">
         <v>300</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E264" s="6" t="s">
         <v>343</v>
@@ -6774,16 +6819,16 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B265" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C265" s="6">
         <v>300</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="E265" s="6" t="s">
         <v>343</v>
@@ -6791,7 +6836,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B266" s="5">
         <v>3</v>
@@ -6800,7 +6845,7 @@
         <v>300</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E266" s="6" t="s">
         <v>343</v>
@@ -6808,16 +6853,16 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="B267" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C267" s="6">
         <v>300</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="E267" s="6" t="s">
         <v>343</v>
@@ -6825,7 +6870,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="B268" s="5">
         <v>1</v>
@@ -6834,7 +6879,7 @@
         <v>300</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="E268" s="6" t="s">
         <v>343</v>
@@ -6842,16 +6887,16 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B269" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C269" s="6">
         <v>300</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="E269" s="6" t="s">
         <v>343</v>
@@ -6859,16 +6904,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="B270" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C270" s="6">
         <v>300</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="E270" s="6" t="s">
         <v>343</v>
@@ -6876,186 +6921,186 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>346</v>
+        <v>511</v>
       </c>
       <c r="B271" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C271" s="6">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>344</v>
+        <v>526</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>347</v>
+        <v>512</v>
       </c>
       <c r="B272" s="5">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C272" s="6">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>345</v>
+        <v>527</v>
       </c>
       <c r="E272" s="6" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>358</v>
+        <v>513</v>
       </c>
       <c r="B273" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C273" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>365</v>
+        <v>528</v>
       </c>
       <c r="E273" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>359</v>
+        <v>514</v>
       </c>
       <c r="B274" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C274" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>366</v>
+        <v>529</v>
       </c>
       <c r="E274" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>360</v>
+        <v>518</v>
       </c>
       <c r="B275" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C275" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>367</v>
+        <v>530</v>
       </c>
       <c r="E275" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>361</v>
+        <v>517</v>
       </c>
       <c r="B276" s="5">
         <v>1</v>
       </c>
       <c r="C276" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>384</v>
+        <v>531</v>
       </c>
       <c r="E276" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>362</v>
+        <v>515</v>
       </c>
       <c r="B277" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C277" s="6">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>368</v>
+        <v>532</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>364</v>
+        <v>516</v>
       </c>
       <c r="B278" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C278" s="6">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="D278" s="4" t="s">
-        <v>369</v>
+        <v>533</v>
       </c>
       <c r="E278" s="6" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="B279" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C279" s="6">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="E279" s="6" t="s">
-        <v>363</v>
+        <v>193</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="B280" s="5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C280" s="6">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="D280" s="4" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="E280" s="6" t="s">
-        <v>363</v>
+        <v>193</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="B281" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C281" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="E281" s="6" t="s">
         <v>363</v>
@@ -7063,16 +7108,16 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="B282" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C282" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="E282" s="6" t="s">
         <v>363</v>
@@ -7080,16 +7125,16 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="B283" s="5">
         <v>1</v>
       </c>
       <c r="C283" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="E283" s="6" t="s">
         <v>363</v>
@@ -7097,16 +7142,16 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="B284" s="5">
         <v>1</v>
       </c>
       <c r="C284" s="6">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E284" s="6" t="s">
         <v>363</v>
@@ -7114,16 +7159,16 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B285" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C285" s="6">
-        <v>550</v>
+        <v>30</v>
       </c>
       <c r="D285" s="4" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="E285" s="6" t="s">
         <v>363</v>
@@ -7131,120 +7176,256 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="B286" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C286" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="E286" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B287" s="5">
         <v>1</v>
       </c>
       <c r="C287" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D287" s="4" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="E287" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="B288" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C288" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="E288" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="B289" s="5">
         <v>1</v>
       </c>
       <c r="C289" s="6">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="E289" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>485</v>
+        <v>374</v>
       </c>
       <c r="B290" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C290" s="6">
-        <v>220</v>
+        <v>550</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>484</v>
+        <v>380</v>
       </c>
       <c r="E290" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>568</v>
+        <v>375</v>
       </c>
       <c r="B291" s="5">
-        <v>2</v>
-      </c>
-      <c r="C291" s="9">
-        <v>1200</v>
+        <v>1</v>
+      </c>
+      <c r="C291" s="6">
+        <v>550</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>569</v>
+        <v>381</v>
       </c>
       <c r="E291" s="6" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
+        <v>377</v>
+      </c>
+      <c r="B292" s="5">
+        <v>1</v>
+      </c>
+      <c r="C292" s="6">
+        <v>550</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E292" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>376</v>
+      </c>
+      <c r="B293" s="5">
+        <v>1</v>
+      </c>
+      <c r="C293" s="6">
+        <v>550</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E293" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>385</v>
+      </c>
+      <c r="B294" s="5">
+        <v>2</v>
+      </c>
+      <c r="C294" s="6">
+        <v>250</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E294" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>386</v>
+      </c>
+      <c r="B295" s="5">
+        <v>1</v>
+      </c>
+      <c r="C295" s="6">
+        <v>250</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E295" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>387</v>
+      </c>
+      <c r="B296" s="5">
+        <v>0</v>
+      </c>
+      <c r="C296" s="6">
+        <v>250</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E296" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>388</v>
+      </c>
+      <c r="B297" s="5">
+        <v>1</v>
+      </c>
+      <c r="C297" s="6">
+        <v>250</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E297" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>485</v>
+      </c>
+      <c r="B298" s="5">
+        <v>4</v>
+      </c>
+      <c r="C298" s="6">
+        <v>220</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="E298" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>568</v>
+      </c>
+      <c r="B299" s="5">
+        <v>2</v>
+      </c>
+      <c r="C299" s="6">
+        <v>1200</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="E299" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
         <v>567</v>
       </c>
-      <c r="B292" s="5">
+      <c r="B300" s="5">
         <v>2</v>
       </c>
-      <c r="C292" s="9">
+      <c r="C300" s="6">
         <v>1200</v>
       </c>
-      <c r="D292" s="4" t="s">
+      <c r="D300" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="E292" s="6" t="s">
+      <c r="E300" s="6" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update stock data in spreadsheet
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F087A992-D532-4D5A-BA29-4C6C38E0173C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB3B94C-C87C-48FB-8824-9B25C542AADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="2625" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="1140" yWindow="2595" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,9 +519,6 @@
     <t>Zoro rizz purple.jpg</t>
   </si>
   <si>
-    <t>Zoro Wano</t>
-  </si>
-  <si>
     <t>Zoro Wano.jpg</t>
   </si>
   <si>
@@ -1795,6 +1792,9 @@
   </si>
   <si>
     <t>obiwan.jpg</t>
+  </si>
+  <si>
+    <t>Zoro [Wano]</t>
   </si>
 </sst>
 </file>
@@ -2318,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B296" sqref="B296"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -2442,7 +2442,7 @@
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -2493,7 +2493,7 @@
         <v>250</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -2510,7 +2510,7 @@
         <v>250</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -2527,7 +2527,7 @@
         <v>250</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -2544,7 +2544,7 @@
         <v>250</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -2561,7 +2561,7 @@
         <v>250</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2578,7 +2578,7 @@
         <v>250</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -2595,7 +2595,7 @@
         <v>250</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -2612,7 +2612,7 @@
         <v>250</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
@@ -2629,7 +2629,7 @@
         <v>250</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -2646,7 +2646,7 @@
         <v>220</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -2680,7 +2680,7 @@
         <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
@@ -2697,7 +2697,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -2714,7 +2714,7 @@
         <v>220</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -2731,7 +2731,7 @@
         <v>220</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -2748,7 +2748,7 @@
         <v>220</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -2782,7 +2782,7 @@
         <v>200</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -2833,7 +2833,7 @@
         <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
@@ -2901,7 +2901,7 @@
         <v>180</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -2918,7 +2918,7 @@
         <v>180</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B36" s="3">
         <v>0</v>
@@ -2935,7 +2935,7 @@
         <v>270</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B38" s="3">
         <v>2</v>
@@ -2969,7 +2969,7 @@
         <v>270</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -2986,7 +2986,7 @@
         <v>450</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -2997,7 +2997,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="3">
         <v>380</v>
@@ -3037,7 +3037,7 @@
         <v>270</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -3071,7 +3071,7 @@
         <v>270</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -3079,7 +3079,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
@@ -3088,7 +3088,7 @@
         <v>250</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
@@ -3122,7 +3122,7 @@
         <v>250</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B48" s="3">
         <v>2</v>
@@ -3139,7 +3139,7 @@
         <v>250</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -3156,7 +3156,7 @@
         <v>250</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -3173,7 +3173,7 @@
         <v>250</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -3207,7 +3207,7 @@
         <v>250</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
@@ -3224,7 +3224,7 @@
         <v>250</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>6</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B54" s="3">
         <v>2</v>
@@ -3241,7 +3241,7 @@
         <v>360</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>6</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
@@ -3258,7 +3258,7 @@
         <v>360</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>6</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B56" s="3">
         <v>2</v>
@@ -3275,7 +3275,7 @@
         <v>200</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>6</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B57" s="3">
         <v>4</v>
@@ -3292,7 +3292,7 @@
         <v>260</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>6</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B58" s="3">
         <v>2</v>
@@ -3309,7 +3309,7 @@
         <v>260</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>6</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B59" s="3">
         <v>2</v>
@@ -3326,7 +3326,7 @@
         <v>260</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>6</v>
@@ -3334,7 +3334,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B60" s="3">
         <v>4</v>
@@ -3343,7 +3343,7 @@
         <v>260</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>6</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B61" s="3">
         <v>1</v>
@@ -3360,7 +3360,7 @@
         <v>220</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>6</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B62" s="3">
         <v>0</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B63" s="3">
         <v>5</v>
@@ -3394,7 +3394,7 @@
         <v>250</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B64" s="3">
         <v>1</v>
@@ -3411,7 +3411,7 @@
         <v>250</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
@@ -3419,7 +3419,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B65" s="3">
         <v>2</v>
@@ -3428,7 +3428,7 @@
         <v>250</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>6</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
@@ -3445,7 +3445,7 @@
         <v>250</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>6</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B67" s="3">
         <v>3</v>
@@ -3462,7 +3462,7 @@
         <v>220</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>6</v>
@@ -3473,13 +3473,13 @@
         <v>38</v>
       </c>
       <c r="B68" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" s="3">
         <v>180</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>35</v>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
@@ -3496,7 +3496,7 @@
         <v>250</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>35</v>
@@ -3513,7 +3513,7 @@
         <v>250</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>35</v>
@@ -3521,7 +3521,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B71" s="3">
         <v>1</v>
@@ -3530,7 +3530,7 @@
         <v>250</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>35</v>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B73" s="3">
         <v>1</v>
@@ -3564,7 +3564,7 @@
         <v>250</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>35</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
@@ -3581,7 +3581,7 @@
         <v>250</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>35</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B75" s="3">
         <v>1</v>
@@ -3598,7 +3598,7 @@
         <v>180</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>35</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B76" s="3">
         <v>1</v>
@@ -3615,7 +3615,7 @@
         <v>180</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>35</v>
@@ -3632,7 +3632,7 @@
         <v>300</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>35</v>
@@ -3649,7 +3649,7 @@
         <v>300</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>35</v>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B79" s="3">
         <v>1</v>
@@ -3666,7 +3666,7 @@
         <v>1000</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>35</v>
@@ -3683,7 +3683,7 @@
         <v>350</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>35</v>
@@ -3700,7 +3700,7 @@
         <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>35</v>
@@ -3717,7 +3717,7 @@
         <v>500</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>35</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B83" s="3">
         <v>3</v>
@@ -3734,7 +3734,7 @@
         <v>220</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>35</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B84" s="3">
         <v>1</v>
@@ -3751,7 +3751,7 @@
         <v>220</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>35</v>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B85" s="6">
         <v>1</v>
@@ -3768,7 +3768,7 @@
         <v>200</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>35</v>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B86" s="3">
         <v>2</v>
@@ -3785,7 +3785,7 @@
         <v>220</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>35</v>
@@ -3793,7 +3793,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B87" s="3">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>250</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>35</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B88" s="3">
         <v>0</v>
@@ -3819,7 +3819,7 @@
         <v>250</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>35</v>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B89" s="3">
         <v>3</v>
@@ -3836,7 +3836,7 @@
         <v>220</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>35</v>
@@ -3853,7 +3853,7 @@
         <v>350</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>35</v>
@@ -3870,7 +3870,7 @@
         <v>350</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>35</v>
@@ -3887,7 +3887,7 @@
         <v>350</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>35</v>
@@ -3904,7 +3904,7 @@
         <v>500</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>35</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B94" s="3">
         <v>3</v>
@@ -3921,7 +3921,7 @@
         <v>500</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>35</v>
@@ -3938,7 +3938,7 @@
         <v>300</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>48</v>
@@ -3946,16 +3946,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>161</v>
+        <v>586</v>
       </c>
       <c r="B96" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C96" s="3">
         <v>300</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>48</v>
@@ -3972,7 +3972,7 @@
         <v>300</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>48</v>
@@ -4091,7 +4091,7 @@
         <v>300</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>48</v>
@@ -4099,7 +4099,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B105" s="3">
         <v>1</v>
@@ -4108,7 +4108,7 @@
         <v>300</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>48</v>
@@ -4125,7 +4125,7 @@
         <v>300</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>48</v>
@@ -4150,16 +4150,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B108" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C108" s="3">
         <v>350</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>48</v>
@@ -4278,7 +4278,7 @@
         <v>300</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>48</v>
@@ -4286,16 +4286,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B116" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116" s="3">
         <v>300</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>48</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B117" s="3">
         <v>2</v>
@@ -4320,10 +4320,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B118" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118" s="3">
         <v>350</v>
@@ -4346,7 +4346,7 @@
         <v>350</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>48</v>
@@ -4363,7 +4363,7 @@
         <v>350</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>48</v>
@@ -4380,7 +4380,7 @@
         <v>320</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>48</v>
@@ -4397,7 +4397,7 @@
         <v>320</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>48</v>
@@ -4414,7 +4414,7 @@
         <v>320</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>48</v>
@@ -4425,13 +4425,13 @@
         <v>71</v>
       </c>
       <c r="B124" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124" s="3">
         <v>320</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>48</v>
@@ -4448,7 +4448,7 @@
         <v>320</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>48</v>
@@ -4465,7 +4465,7 @@
         <v>320</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>48</v>
@@ -4482,7 +4482,7 @@
         <v>320</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>48</v>
@@ -4499,7 +4499,7 @@
         <v>320</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>48</v>
@@ -4516,7 +4516,7 @@
         <v>320</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>48</v>
@@ -4533,7 +4533,7 @@
         <v>320</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>48</v>
@@ -4550,7 +4550,7 @@
         <v>320</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>48</v>
@@ -4561,13 +4561,13 @@
         <v>79</v>
       </c>
       <c r="B132" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132" s="3">
         <v>320</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>48</v>
@@ -4584,7 +4584,7 @@
         <v>320</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>48</v>
@@ -4601,7 +4601,7 @@
         <v>320</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>48</v>
@@ -4618,7 +4618,7 @@
         <v>320</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>48</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B136" s="3">
         <v>1</v>
@@ -4635,7 +4635,7 @@
         <v>320</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>48</v>
@@ -4652,7 +4652,7 @@
         <v>300</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>48</v>
@@ -4669,7 +4669,7 @@
         <v>300</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>48</v>
@@ -4686,7 +4686,7 @@
         <v>300</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>48</v>
@@ -4703,7 +4703,7 @@
         <v>300</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>48</v>
@@ -4720,7 +4720,7 @@
         <v>300</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>48</v>
@@ -4737,7 +4737,7 @@
         <v>300</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>48</v>
@@ -4754,7 +4754,7 @@
         <v>300</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>48</v>
@@ -4771,7 +4771,7 @@
         <v>300</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>48</v>
@@ -4788,7 +4788,7 @@
         <v>300</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>48</v>
@@ -4805,7 +4805,7 @@
         <v>300</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>48</v>
@@ -4822,7 +4822,7 @@
         <v>300</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>48</v>
@@ -4833,13 +4833,13 @@
         <v>94</v>
       </c>
       <c r="B148" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" s="3">
         <v>400</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>48</v>
@@ -4856,7 +4856,7 @@
         <v>400</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>48</v>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B150" s="3">
         <v>3</v>
@@ -4873,7 +4873,7 @@
         <v>300</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>48</v>
@@ -4890,7 +4890,7 @@
         <v>300</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>48</v>
@@ -4907,7 +4907,7 @@
         <v>300</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>48</v>
@@ -4918,13 +4918,13 @@
         <v>98</v>
       </c>
       <c r="B153" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" s="3">
         <v>300</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>48</v>
@@ -4941,7 +4941,7 @@
         <v>300</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>48</v>
@@ -4958,7 +4958,7 @@
         <v>300</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>48</v>
@@ -4975,7 +4975,7 @@
         <v>300</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>48</v>
@@ -4992,7 +4992,7 @@
         <v>500</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>48</v>
@@ -5000,7 +5000,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
@@ -5009,7 +5009,7 @@
         <v>280</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>48</v>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B159" s="3">
         <v>1</v>
@@ -5026,7 +5026,7 @@
         <v>280</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>48</v>
@@ -5034,7 +5034,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B160" s="3">
         <v>1</v>
@@ -5043,7 +5043,7 @@
         <v>280</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>48</v>
@@ -5060,7 +5060,7 @@
         <v>300</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>48</v>
@@ -5077,7 +5077,7 @@
         <v>300</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>48</v>
@@ -5094,7 +5094,7 @@
         <v>250</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>106</v>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B164" s="3">
         <v>1</v>
@@ -5111,7 +5111,7 @@
         <v>280</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>106</v>
@@ -5119,7 +5119,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B165" s="3">
         <v>1</v>
@@ -5128,7 +5128,7 @@
         <v>280</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>106</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B166" s="3">
         <v>2</v>
@@ -5145,7 +5145,7 @@
         <v>260</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>106</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B167" s="3">
         <v>1</v>
@@ -5162,7 +5162,7 @@
         <v>260</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>106</v>
@@ -5187,7 +5187,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B169" s="3">
         <v>1</v>
@@ -5196,7 +5196,7 @@
         <v>280</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>106</v>
@@ -5213,7 +5213,7 @@
         <v>220</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>106</v>
@@ -5230,7 +5230,7 @@
         <v>220</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>106</v>
@@ -5247,7 +5247,7 @@
         <v>220</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>106</v>
@@ -5264,7 +5264,7 @@
         <v>220</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>106</v>
@@ -5281,7 +5281,7 @@
         <v>220</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>106</v>
@@ -5298,7 +5298,7 @@
         <v>250</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>106</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B176" s="3">
         <v>2</v>
@@ -5315,7 +5315,7 @@
         <v>220</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>106</v>
@@ -5323,7 +5323,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B177" s="3">
         <v>3</v>
@@ -5332,7 +5332,7 @@
         <v>250</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>106</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B178" s="3">
         <v>0</v>
@@ -5349,7 +5349,7 @@
         <v>220</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>106</v>
@@ -5366,7 +5366,7 @@
         <v>220</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>106</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B180" s="3">
         <v>2</v>
@@ -5383,7 +5383,7 @@
         <v>250</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>106</v>
@@ -5400,7 +5400,7 @@
         <v>220</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>106</v>
@@ -5417,7 +5417,7 @@
         <v>220</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>106</v>
@@ -5434,7 +5434,7 @@
         <v>350</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>106</v>
@@ -5451,7 +5451,7 @@
         <v>350</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>106</v>
@@ -5468,7 +5468,7 @@
         <v>350</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>106</v>
@@ -5479,13 +5479,13 @@
         <v>120</v>
       </c>
       <c r="B186" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" s="3">
         <v>350</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>106</v>
@@ -5502,7 +5502,7 @@
         <v>350</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>106</v>
@@ -5519,7 +5519,7 @@
         <v>350</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>106</v>
@@ -5536,7 +5536,7 @@
         <v>220</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>106</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B190" s="3">
         <v>1</v>
@@ -5553,7 +5553,7 @@
         <v>220</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>106</v>
@@ -5561,7 +5561,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B191" s="3">
         <v>1</v>
@@ -5570,7 +5570,7 @@
         <v>220</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>106</v>
@@ -5578,7 +5578,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B192" s="3">
         <v>1</v>
@@ -5587,7 +5587,7 @@
         <v>220</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>106</v>
@@ -5595,7 +5595,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B193" s="3">
         <v>1</v>
@@ -5604,7 +5604,7 @@
         <v>250</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>106</v>
@@ -5612,16 +5612,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B194" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C194" s="3">
         <v>250</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>106</v>
@@ -5638,7 +5638,7 @@
         <v>220</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>106</v>
@@ -5646,16 +5646,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B196" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" s="3">
         <v>220</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>106</v>
@@ -5663,7 +5663,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B197" s="3">
         <v>1</v>
@@ -5672,7 +5672,7 @@
         <v>250</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>106</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B198" s="3">
         <v>1</v>
@@ -5689,7 +5689,7 @@
         <v>250</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>106</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B199" s="3">
         <v>0</v>
@@ -5706,7 +5706,7 @@
         <v>250</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>106</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B200" s="3">
         <v>1</v>
@@ -5723,7 +5723,7 @@
         <v>250</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>106</v>
@@ -5740,7 +5740,7 @@
         <v>250</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>125</v>
@@ -5774,7 +5774,7 @@
         <v>250</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>125</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B204" s="3">
         <v>4</v>
@@ -5791,7 +5791,7 @@
         <v>250</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>125</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B206" s="3">
         <v>1</v>
@@ -5825,7 +5825,7 @@
         <v>400</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>125</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B207" s="3">
         <v>1</v>
@@ -5842,7 +5842,7 @@
         <v>400</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>125</v>
@@ -5850,7 +5850,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B208" s="3">
         <v>2</v>
@@ -5859,7 +5859,7 @@
         <v>350</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>125</v>
@@ -5867,7 +5867,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B209" s="3">
         <v>1</v>
@@ -5876,7 +5876,7 @@
         <v>400</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>125</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B210" s="3">
         <v>1</v>
@@ -5893,7 +5893,7 @@
         <v>350</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>125</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B211" s="3">
         <v>2</v>
@@ -5910,7 +5910,7 @@
         <v>350</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>125</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B212" s="3">
         <v>1</v>
@@ -5927,7 +5927,7 @@
         <v>400</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>125</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B213" s="3">
         <v>1</v>
@@ -5944,7 +5944,7 @@
         <v>350</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>125</v>
@@ -5952,7 +5952,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B214" s="3">
         <v>2</v>
@@ -5961,7 +5961,7 @@
         <v>350</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>125</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B215" s="3">
         <v>0</v>
@@ -5978,7 +5978,7 @@
         <v>350</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>125</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B216" s="3">
         <v>2</v>
@@ -5995,7 +5995,7 @@
         <v>350</v>
       </c>
       <c r="D216" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>125</v>
@@ -6012,7 +6012,7 @@
         <v>250</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>130</v>
@@ -6029,7 +6029,7 @@
         <v>250</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>130</v>
@@ -6037,7 +6037,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B219" s="3">
         <v>1</v>
@@ -6046,7 +6046,7 @@
         <v>250</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>130</v>
@@ -6063,7 +6063,7 @@
         <v>250</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>130</v>
@@ -6080,7 +6080,7 @@
         <v>250</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>130</v>
@@ -6097,7 +6097,7 @@
         <v>250</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>130</v>
@@ -6114,7 +6114,7 @@
         <v>250</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>130</v>
@@ -6148,7 +6148,7 @@
         <v>250</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>130</v>
@@ -6182,7 +6182,7 @@
         <v>250</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>130</v>
@@ -6199,7 +6199,7 @@
         <v>250</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>130</v>
@@ -6216,7 +6216,7 @@
         <v>250</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>130</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B230" s="3">
         <v>2</v>
@@ -6233,7 +6233,7 @@
         <v>250</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>130</v>
@@ -6275,7 +6275,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B233" s="3">
         <v>4</v>
@@ -6284,15 +6284,15 @@
         <v>250</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B234" s="3">
         <v>2</v>
@@ -6301,15 +6301,15 @@
         <v>250</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B235" s="3">
         <v>1</v>
@@ -6318,15 +6318,15 @@
         <v>220</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B236" s="3">
         <v>1</v>
@@ -6335,15 +6335,15 @@
         <v>220</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B237" s="3">
         <v>1</v>
@@ -6352,15 +6352,15 @@
         <v>220</v>
       </c>
       <c r="D237" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B238" s="3">
         <v>2</v>
@@ -6369,15 +6369,15 @@
         <v>220</v>
       </c>
       <c r="D238" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B239" s="3">
         <v>1</v>
@@ -6386,15 +6386,15 @@
         <v>160</v>
       </c>
       <c r="D239" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B240" s="3">
         <v>1</v>
@@ -6403,15 +6403,15 @@
         <v>250</v>
       </c>
       <c r="D240" s="8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B241" s="3">
         <v>1</v>
@@ -6420,15 +6420,15 @@
         <v>250</v>
       </c>
       <c r="D241" s="8" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B242" s="3">
         <v>1</v>
@@ -6437,15 +6437,15 @@
         <v>220</v>
       </c>
       <c r="D242" s="8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B243" s="3">
         <v>1</v>
@@ -6454,15 +6454,15 @@
         <v>220</v>
       </c>
       <c r="D243" s="8" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B244" s="3">
         <v>1</v>
@@ -6471,15 +6471,15 @@
         <v>220</v>
       </c>
       <c r="D244" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B245" s="3">
         <v>1</v>
@@ -6488,15 +6488,15 @@
         <v>250</v>
       </c>
       <c r="D245" s="8" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B246" s="3">
         <v>1</v>
@@ -6505,15 +6505,15 @@
         <v>250</v>
       </c>
       <c r="D246" s="8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E246" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B247" s="3">
         <v>1</v>
@@ -6522,15 +6522,15 @@
         <v>220</v>
       </c>
       <c r="D247" s="8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B248" s="5">
         <v>5</v>
@@ -6539,15 +6539,15 @@
         <v>250</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E248" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B249" s="5">
         <v>1</v>
@@ -6556,15 +6556,15 @@
         <v>250</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B250" s="5">
         <v>1</v>
@@ -6573,15 +6573,15 @@
         <v>220</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B251" s="5">
         <v>0</v>
@@ -6593,12 +6593,12 @@
         <v>148</v>
       </c>
       <c r="E251" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B252" s="5">
         <v>2</v>
@@ -6607,15 +6607,15 @@
         <v>220</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E252" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B253" s="5">
         <v>1</v>
@@ -6624,15 +6624,15 @@
         <v>220</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E253" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B254" s="5">
         <v>1</v>
@@ -6641,32 +6641,32 @@
         <v>220</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E254" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B255" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C255" s="6">
         <v>350</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B256" s="5">
         <v>10</v>
@@ -6675,15 +6675,15 @@
         <v>250</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E256" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B257" s="5">
         <v>1</v>
@@ -6692,15 +6692,15 @@
         <v>250</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B258" s="5">
         <v>24</v>
@@ -6709,15 +6709,15 @@
         <v>250</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B259" s="5">
         <v>6</v>
@@ -6726,15 +6726,15 @@
         <v>150</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B260" s="5">
         <v>2</v>
@@ -6743,15 +6743,15 @@
         <v>150</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B261" s="5">
         <v>2</v>
@@ -6760,15 +6760,15 @@
         <v>150</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B262" s="5">
         <v>2</v>
@@ -6777,15 +6777,15 @@
         <v>550</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B263" s="5">
         <v>2</v>
@@ -6794,32 +6794,32 @@
         <v>650</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B264" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C264" s="6">
         <v>300</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B265" s="5">
         <v>2</v>
@@ -6828,32 +6828,32 @@
         <v>300</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E265" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B266" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C266" s="6">
         <v>300</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E266" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B267" s="5">
         <v>2</v>
@@ -6862,15 +6862,15 @@
         <v>300</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E267" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B268" s="5">
         <v>1</v>
@@ -6879,15 +6879,15 @@
         <v>300</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E268" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B269" s="5">
         <v>2</v>
@@ -6896,15 +6896,15 @@
         <v>300</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E269" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B270" s="5">
         <v>1</v>
@@ -6913,15 +6913,15 @@
         <v>300</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B271" s="5">
         <v>1</v>
@@ -6930,15 +6930,15 @@
         <v>300</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B272" s="5">
         <v>1</v>
@@ -6947,66 +6947,66 @@
         <v>300</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E272" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B273" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C273" s="6">
         <v>300</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E273" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B274" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C274" s="6">
         <v>300</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E274" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B275" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C275" s="6">
         <v>300</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E275" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B276" s="5">
         <v>1</v>
@@ -7015,15 +7015,15 @@
         <v>300</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E276" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B277" s="5">
         <v>0</v>
@@ -7032,15 +7032,15 @@
         <v>300</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B278" s="5">
         <v>0</v>
@@ -7049,15 +7049,15 @@
         <v>300</v>
       </c>
       <c r="D278" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E278" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B279" s="5">
         <v>4</v>
@@ -7066,15 +7066,15 @@
         <v>800</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E279" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B280" s="5">
         <v>13</v>
@@ -7083,15 +7083,15 @@
         <v>200</v>
       </c>
       <c r="D280" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E280" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B281" s="5">
         <v>3</v>
@@ -7100,15 +7100,15 @@
         <v>150</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E281" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B282" s="5">
         <v>2</v>
@@ -7117,15 +7117,15 @@
         <v>150</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E282" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B283" s="5">
         <v>1</v>
@@ -7134,15 +7134,15 @@
         <v>150</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E283" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B284" s="5">
         <v>1</v>
@@ -7151,15 +7151,15 @@
         <v>150</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E284" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B285" s="5">
         <v>10</v>
@@ -7168,15 +7168,15 @@
         <v>30</v>
       </c>
       <c r="D285" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E285" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B286" s="5">
         <v>1</v>
@@ -7185,15 +7185,15 @@
         <v>550</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E286" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B287" s="5">
         <v>1</v>
@@ -7202,15 +7202,15 @@
         <v>550</v>
       </c>
       <c r="D287" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E287" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B288" s="5">
         <v>1</v>
@@ -7219,15 +7219,15 @@
         <v>550</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E288" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B289" s="5">
         <v>1</v>
@@ -7236,15 +7236,15 @@
         <v>550</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E289" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B290" s="5">
         <v>1</v>
@@ -7253,15 +7253,15 @@
         <v>550</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E290" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B291" s="5">
         <v>1</v>
@@ -7270,15 +7270,15 @@
         <v>550</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E291" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B292" s="5">
         <v>1</v>
@@ -7287,15 +7287,15 @@
         <v>550</v>
       </c>
       <c r="D292" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E292" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B293" s="5">
         <v>1</v>
@@ -7304,15 +7304,15 @@
         <v>550</v>
       </c>
       <c r="D293" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E293" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B294" s="5">
         <v>1</v>
@@ -7321,15 +7321,15 @@
         <v>250</v>
       </c>
       <c r="D294" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E294" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B295" s="5">
         <v>0</v>
@@ -7338,15 +7338,15 @@
         <v>250</v>
       </c>
       <c r="D295" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E295" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B296" s="5">
         <v>0</v>
@@ -7355,15 +7355,15 @@
         <v>250</v>
       </c>
       <c r="D296" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E296" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B297" s="5">
         <v>1</v>
@@ -7372,15 +7372,15 @@
         <v>250</v>
       </c>
       <c r="D297" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E297" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B298" s="5">
         <v>4</v>
@@ -7389,15 +7389,15 @@
         <v>220</v>
       </c>
       <c r="D298" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E298" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B299" s="5">
         <v>2</v>
@@ -7406,15 +7406,15 @@
         <v>1200</v>
       </c>
       <c r="D299" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E299" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B300" s="5">
         <v>2</v>
@@ -7423,10 +7423,10 @@
         <v>1200</v>
       </c>
       <c r="D300" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E300" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
itachi crow img fix
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9FF1BA-DFFF-40EA-96C7-DD14487DEE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0572A5C-9E4C-40B4-A11F-E4075005FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1815" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:E395"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A233" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D235" sqref="D235"/>
+      <selection activeCell="D241" sqref="D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
itachi img fix p3
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603C06D-F617-4FE4-A21D-1923AF3FD42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F56E26-EC90-4A4F-A4B6-4F9FBAFADD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1815" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -2370,13 +2370,13 @@
     <t>aot cosplay.jpg</t>
   </si>
   <si>
-    <t>itachi crow.jpg</t>
-  </si>
-  <si>
     <t>Batcave</t>
   </si>
   <si>
     <t>batcave.jpg</t>
+  </si>
+  <si>
+    <t>itachi rein.jpg</t>
   </si>
 </sst>
 </file>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B97" s="3">
         <v>5</v>
@@ -4585,7 +4585,7 @@
         <v>400</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>35</v>
@@ -7033,7 +7033,7 @@
         <v>250</v>
       </c>
       <c r="D241" s="8" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
stock update  8 sept
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CEA583-8DA5-4B88-9C7C-F2864BE66695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E599CC14-0028-4317-82B3-0C56A244011E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2445" yWindow="885" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -2518,7 +2518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -2556,9 +2556,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3006,8 +3003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D403" sqref="D403"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,7 +3138,7 @@
         <v>598</v>
       </c>
       <c r="B8" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="11">
         <v>650</v>
@@ -4110,7 +4107,7 @@
         <v>291</v>
       </c>
       <c r="B65" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="3">
         <v>250</v>
@@ -4127,7 +4124,7 @@
         <v>533</v>
       </c>
       <c r="B66" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="3">
         <v>250</v>
@@ -4484,7 +4481,7 @@
         <v>752</v>
       </c>
       <c r="B87" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" s="14">
         <v>270</v>
@@ -4671,7 +4668,7 @@
         <v>37</v>
       </c>
       <c r="B98" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="3">
         <v>300</v>
@@ -4705,7 +4702,7 @@
         <v>519</v>
       </c>
       <c r="B100" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" s="3">
         <v>1000</v>
@@ -4773,7 +4770,7 @@
         <v>423</v>
       </c>
       <c r="B104" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" s="3">
         <v>220</v>
@@ -4960,7 +4957,7 @@
         <v>422</v>
       </c>
       <c r="B115" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" s="3">
         <v>220</v>
@@ -7833,7 +7830,7 @@
         <v>542</v>
       </c>
       <c r="B284" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C284" s="3">
         <v>350</v>
@@ -7850,7 +7847,7 @@
         <v>543</v>
       </c>
       <c r="B285" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C285" s="3">
         <v>400</v>
@@ -8343,7 +8340,7 @@
         <v>435</v>
       </c>
       <c r="B314" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C314" s="3">
         <v>250</v>
@@ -8513,7 +8510,7 @@
         <v>559</v>
       </c>
       <c r="B324" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C324" s="3">
         <v>220</v>
@@ -8649,7 +8646,7 @@
         <v>742</v>
       </c>
       <c r="B332" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C332" s="3">
         <v>50</v>
@@ -9739,7 +9736,7 @@
       <c r="B396" s="5">
         <v>1</v>
       </c>
-      <c r="C396" s="16">
+      <c r="C396" s="6">
         <v>250</v>
       </c>
       <c r="D396" s="4" t="s">
@@ -9756,7 +9753,7 @@
       <c r="B397" s="5">
         <v>1</v>
       </c>
-      <c r="C397" s="16">
+      <c r="C397" s="6">
         <v>250</v>
       </c>
       <c r="D397" s="4" t="s">
@@ -9773,7 +9770,7 @@
       <c r="B398" s="5">
         <v>1</v>
       </c>
-      <c r="C398" s="16">
+      <c r="C398" s="6">
         <v>250</v>
       </c>
       <c r="D398" s="4" t="s">
@@ -9790,7 +9787,7 @@
       <c r="B399" s="5">
         <v>1</v>
       </c>
-      <c r="C399" s="16">
+      <c r="C399" s="6">
         <v>250</v>
       </c>
       <c r="D399" s="4" t="s">
@@ -9807,7 +9804,7 @@
       <c r="B400" s="5">
         <v>1</v>
       </c>
-      <c r="C400" s="16">
+      <c r="C400" s="6">
         <v>250</v>
       </c>
       <c r="D400" s="4" t="s">
@@ -9824,7 +9821,7 @@
       <c r="B401" s="5">
         <v>1</v>
       </c>
-      <c r="C401" s="16">
+      <c r="C401" s="6">
         <v>250</v>
       </c>
       <c r="D401" s="4" t="s">
@@ -9841,7 +9838,7 @@
       <c r="B402" s="5">
         <v>1</v>
       </c>
-      <c r="C402" s="16">
+      <c r="C402" s="6">
         <v>250</v>
       </c>
       <c r="D402" s="4" t="s">
@@ -9858,7 +9855,7 @@
       <c r="B403" s="5">
         <v>1</v>
       </c>
-      <c r="C403" s="16">
+      <c r="C403" s="6">
         <v>250</v>
       </c>
       <c r="D403" s="4" t="s">
@@ -9875,7 +9872,7 @@
       <c r="B404" s="5">
         <v>1</v>
       </c>
-      <c r="C404" s="16">
+      <c r="C404" s="6">
         <v>250</v>
       </c>
       <c r="D404" s="4" t="s">
@@ -9892,7 +9889,7 @@
       <c r="B405" s="5">
         <v>1</v>
       </c>
-      <c r="C405" s="16">
+      <c r="C405" s="6">
         <v>250</v>
       </c>
       <c r="D405" s="4" t="s">
@@ -9909,7 +9906,7 @@
       <c r="B406" s="5">
         <v>1</v>
       </c>
-      <c r="C406" s="16">
+      <c r="C406" s="6">
         <v>250</v>
       </c>
       <c r="D406" s="4" t="s">
@@ -9926,7 +9923,7 @@
       <c r="B407" s="5">
         <v>1</v>
       </c>
-      <c r="C407" s="16">
+      <c r="C407" s="6">
         <v>250</v>
       </c>
       <c r="D407" s="4" t="s">

</xml_diff>

<commit_message>
removed print invoice button+stock update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D085B-C63F-4F32-844C-50F638981D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6A4DA8-D3F0-4E94-997C-2AE3C51EE057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2445" yWindow="885" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -3003,8 +3003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3716,7 +3716,7 @@
         <v>22</v>
       </c>
       <c r="B42" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="3">
         <v>180</v>
@@ -3750,7 +3750,7 @@
         <v>523</v>
       </c>
       <c r="B44" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="3">
         <v>180</v>
@@ -3801,7 +3801,7 @@
         <v>24</v>
       </c>
       <c r="B47" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="3">
         <v>180</v>
@@ -4022,7 +4022,7 @@
         <v>289</v>
       </c>
       <c r="B60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="3">
         <v>250</v>

</xml_diff>

<commit_message>
removed SMTP ports, replaced with sheets update stock update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0434A8D4-5A4C-4ADE-BB02-F70888556525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641BDF06-4D51-490D-925B-B1C889CC1D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1470" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="4470" yWindow="1575" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3069,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B409" sqref="B409"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5975,7 +5975,7 @@
         <v>68</v>
       </c>
       <c r="B171" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" s="3">
         <v>320</v>
@@ -5992,7 +5992,7 @@
         <v>69</v>
       </c>
       <c r="B172" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C172" s="3">
         <v>320</v>
@@ -7352,7 +7352,7 @@
         <v>114</v>
       </c>
       <c r="B252" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C252" s="3">
         <v>350</v>
@@ -7760,7 +7760,7 @@
         <v>719</v>
       </c>
       <c r="B276" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C276" s="3">
         <v>250</v>
@@ -7845,7 +7845,7 @@
         <v>780</v>
       </c>
       <c r="B281" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C281" s="3">
         <v>250</v>
@@ -8015,7 +8015,7 @@
         <v>543</v>
       </c>
       <c r="B291" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C291" s="3">
         <v>400</v>

</xml_diff>

<commit_message>
stock update, andrew 0 bat dio 6
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2127BC-621D-4AB8-9934-8F2BA32498EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF9C57-2649-4885-BAC4-1DDC818CB8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="1560" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -1257,9 +1257,6 @@
     <t>Thor endgame MCU</t>
   </si>
   <si>
-    <t>Loki TVA Varient</t>
-  </si>
-  <si>
     <t>Ironman Pulse Hands</t>
   </si>
   <si>
@@ -2515,6 +2512,9 @@
   </si>
   <si>
     <t>okarun white.jpg</t>
+  </si>
+  <si>
+    <t>Loki TVA Agent</t>
   </si>
 </sst>
 </file>
@@ -3069,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B320" sqref="B320"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -3108,7 +3108,7 @@
         <v>250</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -3125,7 +3125,7 @@
         <v>250</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -3142,7 +3142,7 @@
         <v>250</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -3159,7 +3159,7 @@
         <v>250</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -3176,7 +3176,7 @@
         <v>250</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -3193,7 +3193,7 @@
         <v>250</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -3210,7 +3210,7 @@
         <v>300</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>186</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -3227,7 +3227,7 @@
         <v>300</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>186</v>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
@@ -3244,7 +3244,7 @@
         <v>300</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>186</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -3261,7 +3261,7 @@
         <v>300</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>186</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -3278,7 +3278,7 @@
         <v>300</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>186</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B13" s="10">
         <v>4</v>
@@ -3295,7 +3295,7 @@
         <v>650</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>186</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B14" s="10">
         <v>5</v>
@@ -3312,7 +3312,7 @@
         <v>280</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>6</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -3380,7 +3380,7 @@
         <v>550</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -3490,16 +3490,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>250</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>614</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>250</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>615</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -3524,16 +3524,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>250</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>616</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>250</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>617</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
@@ -3652,7 +3652,7 @@
         <v>250</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
@@ -3669,7 +3669,7 @@
         <v>250</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -3873,7 +3873,7 @@
         <v>180</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -3890,7 +3890,7 @@
         <v>180</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -3907,7 +3907,7 @@
         <v>180</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B50" s="3">
         <v>0</v>
@@ -3924,7 +3924,7 @@
         <v>180</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
@@ -3941,7 +3941,7 @@
         <v>180</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -3949,7 +3949,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -3958,7 +3958,7 @@
         <v>180</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -3975,7 +3975,7 @@
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>6</v>
@@ -3983,7 +3983,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B54" s="3">
         <v>2</v>
@@ -3992,7 +3992,7 @@
         <v>180</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>6</v>
@@ -4000,7 +4000,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B55" s="3">
         <v>0</v>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B56" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="3">
         <v>270</v>
@@ -4034,7 +4034,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B57" s="3">
         <v>0</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B64" s="3">
         <v>0</v>
@@ -4162,7 +4162,7 @@
         <v>250</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B72" s="3">
         <v>0</v>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B76" s="3">
         <v>4</v>
@@ -4366,7 +4366,7 @@
         <v>260</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>6</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>407</v>
+        <v>826</v>
       </c>
       <c r="B77" s="3">
         <v>2</v>
@@ -4383,7 +4383,7 @@
         <v>260</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>6</v>
@@ -4400,7 +4400,7 @@
         <v>260</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>6</v>
@@ -4417,7 +4417,7 @@
         <v>260</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>6</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B80" s="3">
         <v>1</v>
@@ -4434,7 +4434,7 @@
         <v>220</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>6</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B81" s="3">
         <v>0</v>
@@ -4468,7 +4468,7 @@
         <v>250</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>6</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B83" s="3">
         <v>1</v>
@@ -4485,7 +4485,7 @@
         <v>250</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>6</v>
@@ -4502,7 +4502,7 @@
         <v>250</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>6</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B85" s="3">
         <v>1</v>
@@ -4519,7 +4519,7 @@
         <v>250</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>6</v>
@@ -4536,7 +4536,7 @@
         <v>220</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>6</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B87" s="3">
         <v>1</v>
@@ -4553,7 +4553,7 @@
         <v>350</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>6</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
@@ -4570,7 +4570,7 @@
         <v>350</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>6</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B89" s="3">
         <v>1</v>
@@ -4587,7 +4587,7 @@
         <v>350</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>6</v>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B90" s="3">
         <v>1</v>
@@ -4604,7 +4604,7 @@
         <v>350</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>6</v>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B91" s="3">
         <v>1</v>
@@ -4621,7 +4621,7 @@
         <v>350</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>6</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B92" s="3">
         <v>1</v>
@@ -4638,7 +4638,7 @@
         <v>350</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>6</v>
@@ -4646,7 +4646,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B93" s="14">
         <v>0</v>
@@ -4655,7 +4655,7 @@
         <v>270</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>35</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B103" s="3">
         <v>5</v>
@@ -4825,7 +4825,7 @@
         <v>400</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>35</v>
@@ -4867,16 +4867,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B106" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C106" s="3">
         <v>1000</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>35</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B110" s="3">
         <v>0</v>
@@ -4944,7 +4944,7 @@
         <v>220</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>35</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B111" s="3">
         <v>0</v>
@@ -4961,7 +4961,7 @@
         <v>220</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>35</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B112" s="6">
         <v>0</v>
@@ -4978,7 +4978,7 @@
         <v>200</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>35</v>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B113" s="6">
         <v>0</v>
@@ -4995,7 +4995,7 @@
         <v>250</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>35</v>
@@ -5003,7 +5003,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B114" s="6">
         <v>2</v>
@@ -5012,7 +5012,7 @@
         <v>220</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>35</v>
@@ -5020,7 +5020,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B115" s="6">
         <v>2</v>
@@ -5029,7 +5029,7 @@
         <v>220</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>35</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B116" s="6">
         <v>1</v>
@@ -5046,7 +5046,7 @@
         <v>220</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>35</v>
@@ -5054,7 +5054,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B117" s="6">
         <v>3</v>
@@ -5063,7 +5063,7 @@
         <v>220</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>35</v>
@@ -5071,7 +5071,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B118" s="3">
         <v>0</v>
@@ -5080,7 +5080,7 @@
         <v>220</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>35</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B119" s="3">
         <v>0</v>
@@ -5097,7 +5097,7 @@
         <v>250</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>35</v>
@@ -5105,7 +5105,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B120" s="3">
         <v>0</v>
@@ -5114,7 +5114,7 @@
         <v>250</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>35</v>
@@ -5122,7 +5122,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B121" s="3">
         <v>0</v>
@@ -5131,7 +5131,7 @@
         <v>220</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>35</v>
@@ -5207,7 +5207,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B126" s="3">
         <v>5</v>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B127" s="3">
         <v>2</v>
@@ -5233,7 +5233,7 @@
         <v>250</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>35</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B128" s="3">
         <v>1</v>
@@ -5250,7 +5250,7 @@
         <v>250</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>35</v>
@@ -5258,7 +5258,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B129" s="3">
         <v>1</v>
@@ -5267,7 +5267,7 @@
         <v>250</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>35</v>
@@ -5275,7 +5275,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B130" s="3">
         <v>1</v>
@@ -5284,7 +5284,7 @@
         <v>250</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>35</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B131" s="3">
         <v>0</v>
@@ -5301,7 +5301,7 @@
         <v>270</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>35</v>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B132" s="3">
         <v>2</v>
@@ -5318,7 +5318,7 @@
         <v>250</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>35</v>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B134" s="3">
         <v>1</v>
@@ -5352,7 +5352,7 @@
         <v>350</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>48</v>
@@ -5360,7 +5360,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B135" s="3">
         <v>2</v>
@@ -5411,7 +5411,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B138" s="3">
         <v>0</v>
@@ -5420,7 +5420,7 @@
         <v>400</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>48</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B139" s="3">
         <v>0</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B141" s="3">
         <v>2</v>
@@ -5471,7 +5471,7 @@
         <v>300</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>48</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B144" s="3">
         <v>2</v>
@@ -5522,7 +5522,7 @@
         <v>320</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>48</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B145" s="3">
         <v>1</v>
@@ -5539,7 +5539,7 @@
         <v>320</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>48</v>
@@ -5547,7 +5547,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B146" s="3">
         <v>1</v>
@@ -5556,7 +5556,7 @@
         <v>350</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>48</v>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B147" s="3">
         <v>2</v>
@@ -5573,7 +5573,7 @@
         <v>350</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>48</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B148" s="3">
         <v>2</v>
@@ -5590,7 +5590,7 @@
         <v>300</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>48</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B153" s="3">
         <v>0</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B154" s="3">
         <v>1</v>
@@ -5819,7 +5819,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B162" s="3">
         <v>1</v>
@@ -5828,7 +5828,7 @@
         <v>300</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>48</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B163" s="3">
         <v>1</v>
@@ -5845,7 +5845,7 @@
         <v>300</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>48</v>
@@ -6261,7 +6261,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B188" s="3">
         <v>2</v>
@@ -6270,7 +6270,7 @@
         <v>300</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>48</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B193" s="3">
         <v>1</v>
@@ -6355,7 +6355,7 @@
         <v>300</v>
       </c>
       <c r="D193" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>48</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B203" s="3">
         <v>1</v>
@@ -6525,7 +6525,7 @@
         <v>300</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>48</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B204" s="3">
         <v>1</v>
@@ -6542,7 +6542,7 @@
         <v>300</v>
       </c>
       <c r="D204" s="8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>48</v>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B205" s="3">
         <v>1</v>
@@ -6559,7 +6559,7 @@
         <v>300</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>48</v>
@@ -6567,7 +6567,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B206" s="3">
         <v>1</v>
@@ -6576,7 +6576,7 @@
         <v>300</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>48</v>
@@ -6584,7 +6584,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B207" s="3">
         <v>1</v>
@@ -6593,7 +6593,7 @@
         <v>300</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>48</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B208" s="3">
         <v>1</v>
@@ -6610,7 +6610,7 @@
         <v>300</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>48</v>
@@ -6618,7 +6618,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B209" s="3">
         <v>1</v>
@@ -6627,7 +6627,7 @@
         <v>300</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>48</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B215" s="3">
         <v>1</v>
@@ -6729,7 +6729,7 @@
         <v>280</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>48</v>
@@ -6737,7 +6737,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B216" s="3">
         <v>1</v>
@@ -6746,7 +6746,7 @@
         <v>280</v>
       </c>
       <c r="D216" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>48</v>
@@ -6754,7 +6754,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B217" s="3">
         <v>1</v>
@@ -6763,7 +6763,7 @@
         <v>280</v>
       </c>
       <c r="D217" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>48</v>
@@ -6839,7 +6839,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B222" s="3">
         <v>0</v>
@@ -6890,7 +6890,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B225" s="3">
         <v>2</v>
@@ -6899,7 +6899,7 @@
         <v>250</v>
       </c>
       <c r="D225" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>104</v>
@@ -6907,7 +6907,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B226" s="3">
         <v>0</v>
@@ -6916,7 +6916,7 @@
         <v>250</v>
       </c>
       <c r="D226" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>104</v>
@@ -6924,7 +6924,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B227" s="3">
         <v>1</v>
@@ -6933,7 +6933,7 @@
         <v>250</v>
       </c>
       <c r="D227" s="8" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>104</v>
@@ -6941,7 +6941,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B228" s="3">
         <v>2</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B229" s="3">
         <v>1</v>
@@ -6967,7 +6967,7 @@
         <v>250</v>
       </c>
       <c r="D229" s="8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>104</v>
@@ -6975,7 +6975,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B230" s="3">
         <v>2</v>
@@ -6984,7 +6984,7 @@
         <v>250</v>
       </c>
       <c r="D230" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>104</v>
@@ -6992,7 +6992,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B231" s="3">
         <v>1</v>
@@ -7001,7 +7001,7 @@
         <v>250</v>
       </c>
       <c r="D231" s="8" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>104</v>
@@ -7009,7 +7009,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B232" s="3">
         <v>0</v>
@@ -7018,7 +7018,7 @@
         <v>260</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>104</v>
@@ -7026,7 +7026,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B233" s="3">
         <v>1</v>
@@ -7035,7 +7035,7 @@
         <v>250</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>104</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B234" s="3">
         <v>1</v>
@@ -7052,7 +7052,7 @@
         <v>250</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>104</v>
@@ -7060,7 +7060,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B235" s="3">
         <v>1</v>
@@ -7069,7 +7069,7 @@
         <v>250</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>104</v>
@@ -7077,7 +7077,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B236" s="3">
         <v>1</v>
@@ -7086,7 +7086,7 @@
         <v>260</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>104</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B243" s="3">
         <v>1</v>
@@ -7273,7 +7273,7 @@
         <v>250</v>
       </c>
       <c r="D247" s="8" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>104</v>
@@ -7298,7 +7298,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B249" s="3">
         <v>4</v>
@@ -7315,7 +7315,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B250" s="3">
         <v>3</v>
@@ -7341,7 +7341,7 @@
         <v>250</v>
       </c>
       <c r="D251" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E251" s="3" t="s">
         <v>104</v>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B258" s="3">
         <v>1</v>
@@ -7460,7 +7460,7 @@
         <v>800</v>
       </c>
       <c r="D258" s="8" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E258" s="3" t="s">
         <v>104</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B259" s="3">
         <v>1</v>
@@ -7477,7 +7477,7 @@
         <v>800</v>
       </c>
       <c r="D259" s="8" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E259" s="3" t="s">
         <v>104</v>
@@ -7485,7 +7485,7 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B260" s="3">
         <v>1</v>
@@ -7494,7 +7494,7 @@
         <v>800</v>
       </c>
       <c r="D260" s="8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E260" s="3" t="s">
         <v>104</v>
@@ -7502,7 +7502,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B261" s="3">
         <v>1</v>
@@ -7511,7 +7511,7 @@
         <v>800</v>
       </c>
       <c r="D261" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E261" s="3" t="s">
         <v>104</v>
@@ -7519,7 +7519,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B262" s="3">
         <v>1</v>
@@ -7528,7 +7528,7 @@
         <v>800</v>
       </c>
       <c r="D262" s="8" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E262" s="3" t="s">
         <v>104</v>
@@ -7536,7 +7536,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B263" s="3">
         <v>0</v>
@@ -7545,7 +7545,7 @@
         <v>800</v>
       </c>
       <c r="D263" s="8" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E263" s="3" t="s">
         <v>104</v>
@@ -7562,7 +7562,7 @@
         <v>250</v>
       </c>
       <c r="D264" s="8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E264" s="3" t="s">
         <v>104</v>
@@ -7570,7 +7570,7 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B265" s="3">
         <v>0</v>
@@ -7579,7 +7579,7 @@
         <v>250</v>
       </c>
       <c r="D265" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E265" s="3" t="s">
         <v>104</v>
@@ -7587,7 +7587,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B266" s="3">
         <v>0</v>
@@ -7596,7 +7596,7 @@
         <v>250</v>
       </c>
       <c r="D266" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E266" s="3" t="s">
         <v>104</v>
@@ -7604,7 +7604,7 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B267" s="3">
         <v>0</v>
@@ -7613,7 +7613,7 @@
         <v>250</v>
       </c>
       <c r="D267" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E267" s="3" t="s">
         <v>104</v>
@@ -7621,7 +7621,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B268" s="3">
         <v>1</v>
@@ -7630,7 +7630,7 @@
         <v>250</v>
       </c>
       <c r="D268" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E268" s="3" t="s">
         <v>104</v>
@@ -7638,7 +7638,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B269" s="3">
         <v>0</v>
@@ -7647,7 +7647,7 @@
         <v>250</v>
       </c>
       <c r="D269" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E269" s="3" t="s">
         <v>104</v>
@@ -7664,7 +7664,7 @@
         <v>250</v>
       </c>
       <c r="D270" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E270" s="3" t="s">
         <v>104</v>
@@ -7672,7 +7672,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B271" s="3">
         <v>0</v>
@@ -7681,7 +7681,7 @@
         <v>250</v>
       </c>
       <c r="D271" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E271" s="3" t="s">
         <v>104</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B272" s="3">
         <v>0</v>
@@ -7698,7 +7698,7 @@
         <v>250</v>
       </c>
       <c r="D272" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E272" s="3" t="s">
         <v>104</v>
@@ -7706,7 +7706,7 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B273" s="3">
         <v>1</v>
@@ -7715,7 +7715,7 @@
         <v>250</v>
       </c>
       <c r="D273" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E273" s="3" t="s">
         <v>104</v>
@@ -7723,7 +7723,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B274" s="3">
         <v>0</v>
@@ -7732,7 +7732,7 @@
         <v>250</v>
       </c>
       <c r="D274" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E274" s="3" t="s">
         <v>104</v>
@@ -7740,7 +7740,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B275" s="3">
         <v>1</v>
@@ -7749,7 +7749,7 @@
         <v>250</v>
       </c>
       <c r="D275" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E275" s="3" t="s">
         <v>104</v>
@@ -7757,7 +7757,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B276" s="3">
         <v>0</v>
@@ -7766,7 +7766,7 @@
         <v>250</v>
       </c>
       <c r="D276" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E276" s="3" t="s">
         <v>104</v>
@@ -7774,7 +7774,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B277" s="3">
         <v>1</v>
@@ -7783,7 +7783,7 @@
         <v>250</v>
       </c>
       <c r="D277" s="8" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E277" s="3" t="s">
         <v>104</v>
@@ -7791,7 +7791,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B278" s="3">
         <v>2</v>
@@ -7800,7 +7800,7 @@
         <v>250</v>
       </c>
       <c r="D278" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E278" s="3" t="s">
         <v>104</v>
@@ -7808,7 +7808,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B279" s="3">
         <v>2</v>
@@ -7817,7 +7817,7 @@
         <v>250</v>
       </c>
       <c r="D279" s="8" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E279" s="3" t="s">
         <v>104</v>
@@ -7825,7 +7825,7 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B280" s="3">
         <v>2</v>
@@ -7834,7 +7834,7 @@
         <v>250</v>
       </c>
       <c r="D280" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E280" s="3" t="s">
         <v>104</v>
@@ -7842,7 +7842,7 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B281" s="3">
         <v>1</v>
@@ -7851,7 +7851,7 @@
         <v>250</v>
       </c>
       <c r="D281" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E281" s="3" t="s">
         <v>104</v>
@@ -7859,7 +7859,7 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B282" s="3">
         <v>2</v>
@@ -7868,7 +7868,7 @@
         <v>250</v>
       </c>
       <c r="D282" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E282" s="3" t="s">
         <v>104</v>
@@ -7927,7 +7927,7 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B286" s="3">
         <v>4</v>
@@ -7961,7 +7961,7 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B288" s="3">
         <v>2</v>
@@ -7970,7 +7970,7 @@
         <v>400</v>
       </c>
       <c r="D288" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E288" s="3" t="s">
         <v>122</v>
@@ -7978,7 +7978,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B289" s="3">
         <v>1</v>
@@ -7987,7 +7987,7 @@
         <v>400</v>
       </c>
       <c r="D289" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E289" s="3" t="s">
         <v>122</v>
@@ -7995,7 +7995,7 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B290" s="3">
         <v>2</v>
@@ -8004,7 +8004,7 @@
         <v>350</v>
       </c>
       <c r="D290" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E290" s="3" t="s">
         <v>122</v>
@@ -8012,7 +8012,7 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B291" s="3">
         <v>2</v>
@@ -8021,7 +8021,7 @@
         <v>400</v>
       </c>
       <c r="D291" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E291" s="3" t="s">
         <v>122</v>
@@ -8029,7 +8029,7 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B292" s="3">
         <v>1</v>
@@ -8038,7 +8038,7 @@
         <v>350</v>
       </c>
       <c r="D292" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E292" s="3" t="s">
         <v>122</v>
@@ -8046,7 +8046,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B293" s="3">
         <v>4</v>
@@ -8055,7 +8055,7 @@
         <v>350</v>
       </c>
       <c r="D293" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E293" s="3" t="s">
         <v>122</v>
@@ -8063,7 +8063,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B294" s="3">
         <v>4</v>
@@ -8072,7 +8072,7 @@
         <v>400</v>
       </c>
       <c r="D294" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E294" s="3" t="s">
         <v>122</v>
@@ -8080,7 +8080,7 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B295" s="3">
         <v>1</v>
@@ -8089,7 +8089,7 @@
         <v>350</v>
       </c>
       <c r="D295" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E295" s="3" t="s">
         <v>122</v>
@@ -8097,7 +8097,7 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B296" s="3">
         <v>2</v>
@@ -8106,7 +8106,7 @@
         <v>350</v>
       </c>
       <c r="D296" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E296" s="3" t="s">
         <v>122</v>
@@ -8114,7 +8114,7 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B297" s="3">
         <v>2</v>
@@ -8123,7 +8123,7 @@
         <v>350</v>
       </c>
       <c r="D297" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E297" s="3" t="s">
         <v>122</v>
@@ -8131,7 +8131,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B298" s="3">
         <v>2</v>
@@ -8140,7 +8140,7 @@
         <v>350</v>
       </c>
       <c r="D298" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E298" s="3" t="s">
         <v>122</v>
@@ -8148,7 +8148,7 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B299" s="3">
         <v>1</v>
@@ -8157,7 +8157,7 @@
         <v>250</v>
       </c>
       <c r="D299" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E299" s="3" t="s">
         <v>122</v>
@@ -8165,7 +8165,7 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B300" s="3">
         <v>1</v>
@@ -8174,7 +8174,7 @@
         <v>250</v>
       </c>
       <c r="D300" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E300" s="3" t="s">
         <v>122</v>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B301" s="3">
         <v>1</v>
@@ -8191,7 +8191,7 @@
         <v>250</v>
       </c>
       <c r="D301" s="8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E301" s="3" t="s">
         <v>122</v>
@@ -8199,7 +8199,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B302" s="3">
         <v>2</v>
@@ -8208,7 +8208,7 @@
         <v>250</v>
       </c>
       <c r="D302" s="8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E302" s="3" t="s">
         <v>122</v>
@@ -8216,7 +8216,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B303" s="3">
         <v>1</v>
@@ -8225,7 +8225,7 @@
         <v>250</v>
       </c>
       <c r="D303" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E303" s="3" t="s">
         <v>122</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B306" s="3">
         <v>0</v>
@@ -8420,7 +8420,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B315" s="3">
         <v>0</v>
@@ -8437,7 +8437,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B316" s="3">
         <v>1</v>
@@ -8454,7 +8454,7 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B317" s="3">
         <v>0</v>
@@ -8505,7 +8505,7 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B320" s="3">
         <v>0</v>
@@ -8514,15 +8514,15 @@
         <v>250</v>
       </c>
       <c r="D320" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E320" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B321" s="3">
         <v>0</v>
@@ -8531,15 +8531,15 @@
         <v>250</v>
       </c>
       <c r="D321" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E321" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B322" s="3">
         <v>0</v>
@@ -8548,15 +8548,15 @@
         <v>220</v>
       </c>
       <c r="D322" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E322" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B323" s="3">
         <v>0</v>
@@ -8565,15 +8565,15 @@
         <v>220</v>
       </c>
       <c r="D323" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E323" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B324" s="3">
         <v>1</v>
@@ -8582,15 +8582,15 @@
         <v>220</v>
       </c>
       <c r="D324" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E324" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B325" s="3">
         <v>2</v>
@@ -8599,15 +8599,15 @@
         <v>220</v>
       </c>
       <c r="D325" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E325" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B326" s="3">
         <v>1</v>
@@ -8616,15 +8616,15 @@
         <v>160</v>
       </c>
       <c r="D326" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E326" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B327" s="3">
         <v>0</v>
@@ -8633,15 +8633,15 @@
         <v>250</v>
       </c>
       <c r="D327" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E327" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B328" s="3">
         <v>1</v>
@@ -8650,15 +8650,15 @@
         <v>250</v>
       </c>
       <c r="D328" s="8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E328" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B329" s="3">
         <v>0</v>
@@ -8667,15 +8667,15 @@
         <v>220</v>
       </c>
       <c r="D329" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E329" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B330" s="3">
         <v>0</v>
@@ -8684,15 +8684,15 @@
         <v>220</v>
       </c>
       <c r="D330" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E330" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B331" s="3">
         <v>0</v>
@@ -8701,15 +8701,15 @@
         <v>220</v>
       </c>
       <c r="D331" s="8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E331" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B332" s="3">
         <v>0</v>
@@ -8718,15 +8718,15 @@
         <v>250</v>
       </c>
       <c r="D332" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E332" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B333" s="3">
         <v>2</v>
@@ -8735,15 +8735,15 @@
         <v>250</v>
       </c>
       <c r="D333" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E333" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B334" s="3">
         <v>0</v>
@@ -8752,15 +8752,15 @@
         <v>220</v>
       </c>
       <c r="D334" s="8" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E334" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="7" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B335" s="3">
         <v>2</v>
@@ -8769,15 +8769,15 @@
         <v>250</v>
       </c>
       <c r="D335" s="8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E335" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B336" s="3">
         <v>2</v>
@@ -8786,15 +8786,15 @@
         <v>250</v>
       </c>
       <c r="D336" s="8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E336" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B337" s="3">
         <v>2</v>
@@ -8803,15 +8803,15 @@
         <v>250</v>
       </c>
       <c r="D337" s="8" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E337" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B338" s="3">
         <v>0</v>
@@ -8820,10 +8820,10 @@
         <v>50</v>
       </c>
       <c r="D338" s="8" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E338" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -8947,7 +8947,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B346" s="5">
         <v>3</v>
@@ -8956,7 +8956,7 @@
         <v>320</v>
       </c>
       <c r="D346" s="8" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E346" s="6" t="s">
         <v>382</v>
@@ -8964,7 +8964,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B347" s="5">
         <v>2</v>
@@ -8973,7 +8973,7 @@
         <v>320</v>
       </c>
       <c r="D347" s="8" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E347" s="6" t="s">
         <v>382</v>
@@ -8981,7 +8981,7 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B348" s="5">
         <v>3</v>
@@ -8990,7 +8990,7 @@
         <v>320</v>
       </c>
       <c r="D348" s="8" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E348" s="6" t="s">
         <v>382</v>
@@ -8998,7 +8998,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B349" s="5">
         <v>2</v>
@@ -9007,7 +9007,7 @@
         <v>320</v>
       </c>
       <c r="D349" s="8" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E349" s="6" t="s">
         <v>382</v>
@@ -9015,7 +9015,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B350" s="5">
         <v>0</v>
@@ -9024,7 +9024,7 @@
         <v>320</v>
       </c>
       <c r="D350" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E350" s="6" t="s">
         <v>382</v>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B360" s="5">
         <v>1</v>
@@ -9194,7 +9194,7 @@
         <v>300</v>
       </c>
       <c r="D360" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E360" s="6" t="s">
         <v>330</v>
@@ -9202,7 +9202,7 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B361" s="5">
         <v>1</v>
@@ -9211,7 +9211,7 @@
         <v>300</v>
       </c>
       <c r="D361" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E361" s="6" t="s">
         <v>330</v>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B362" s="5">
         <v>1</v>
@@ -9228,7 +9228,7 @@
         <v>300</v>
       </c>
       <c r="D362" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E362" s="6" t="s">
         <v>330</v>
@@ -9236,7 +9236,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B363" s="5">
         <v>1</v>
@@ -9245,7 +9245,7 @@
         <v>300</v>
       </c>
       <c r="D363" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E363" s="6" t="s">
         <v>330</v>
@@ -9253,7 +9253,7 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B364" s="5">
         <v>0</v>
@@ -9262,7 +9262,7 @@
         <v>300</v>
       </c>
       <c r="D364" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E364" s="6" t="s">
         <v>330</v>
@@ -9270,7 +9270,7 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B365" s="5">
         <v>2</v>
@@ -9279,7 +9279,7 @@
         <v>300</v>
       </c>
       <c r="D365" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E365" s="6" t="s">
         <v>330</v>
@@ -9287,7 +9287,7 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B366" s="5">
         <v>1</v>
@@ -9296,7 +9296,7 @@
         <v>300</v>
       </c>
       <c r="D366" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E366" s="6" t="s">
         <v>330</v>
@@ -9304,7 +9304,7 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B367" s="5">
         <v>0</v>
@@ -9313,7 +9313,7 @@
         <v>300</v>
       </c>
       <c r="D367" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E367" s="6" t="s">
         <v>330</v>
@@ -9321,7 +9321,7 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B368" s="5">
         <v>1</v>
@@ -9330,7 +9330,7 @@
         <v>300</v>
       </c>
       <c r="D368" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E368" s="6" t="s">
         <v>330</v>
@@ -9338,7 +9338,7 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B369" s="5">
         <v>0</v>
@@ -9347,7 +9347,7 @@
         <v>300</v>
       </c>
       <c r="D369" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E369" s="6" t="s">
         <v>330</v>
@@ -9355,7 +9355,7 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B370" s="5">
         <v>2</v>
@@ -9364,7 +9364,7 @@
         <v>300</v>
       </c>
       <c r="D370" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E370" s="6" t="s">
         <v>330</v>
@@ -9372,7 +9372,7 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B371" s="5">
         <v>2</v>
@@ -9381,7 +9381,7 @@
         <v>300</v>
       </c>
       <c r="D371" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E371" s="6" t="s">
         <v>330</v>
@@ -9389,7 +9389,7 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B372" s="5">
         <v>1</v>
@@ -9398,7 +9398,7 @@
         <v>300</v>
       </c>
       <c r="D372" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E372" s="6" t="s">
         <v>330</v>
@@ -9406,7 +9406,7 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B373" s="5">
         <v>0</v>
@@ -9415,7 +9415,7 @@
         <v>300</v>
       </c>
       <c r="D373" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E373" s="6" t="s">
         <v>330</v>
@@ -9423,7 +9423,7 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B374" s="5">
         <v>0</v>
@@ -9432,7 +9432,7 @@
         <v>300</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E374" s="6" t="s">
         <v>330</v>
@@ -9440,7 +9440,7 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B375" s="5">
         <v>1</v>
@@ -9449,7 +9449,7 @@
         <v>320</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E375" s="6" t="s">
         <v>330</v>
@@ -9457,7 +9457,7 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B376" s="5">
         <v>3</v>
@@ -9466,7 +9466,7 @@
         <v>320</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E376" s="6" t="s">
         <v>330</v>
@@ -9474,7 +9474,7 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B377" s="5">
         <v>2</v>
@@ -9483,7 +9483,7 @@
         <v>320</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E377" s="6" t="s">
         <v>330</v>
@@ -9491,7 +9491,7 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B378" s="5">
         <v>2</v>
@@ -9500,7 +9500,7 @@
         <v>320</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E378" s="6" t="s">
         <v>330</v>
@@ -9508,7 +9508,7 @@
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B379" s="5">
         <v>3</v>
@@ -9517,7 +9517,7 @@
         <v>320</v>
       </c>
       <c r="D379" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E379" s="6" t="s">
         <v>330</v>
@@ -9525,7 +9525,7 @@
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B380" s="5">
         <v>1</v>
@@ -9534,7 +9534,7 @@
         <v>300</v>
       </c>
       <c r="D380" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E380" s="6" t="s">
         <v>330</v>
@@ -9542,7 +9542,7 @@
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B381" s="5">
         <v>3</v>
@@ -9551,7 +9551,7 @@
         <v>320</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E381" s="6" t="s">
         <v>330</v>
@@ -9559,7 +9559,7 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B382" s="5">
         <v>1</v>
@@ -9568,7 +9568,7 @@
         <v>320</v>
       </c>
       <c r="D382" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E382" s="6" t="s">
         <v>330</v>
@@ -9576,7 +9576,7 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B383" s="5">
         <v>2</v>
@@ -9585,7 +9585,7 @@
         <v>300</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E383" s="6" t="s">
         <v>330</v>
@@ -9916,7 +9916,7 @@
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B403" s="5">
         <v>4</v>
@@ -9925,7 +9925,7 @@
         <v>220</v>
       </c>
       <c r="D403" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E403" s="6" t="s">
         <v>186</v>
@@ -9933,7 +9933,7 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B404" s="5">
         <v>1</v>
@@ -9942,7 +9942,7 @@
         <v>1200</v>
       </c>
       <c r="D404" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E404" s="6" t="s">
         <v>186</v>
@@ -9950,7 +9950,7 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B405" s="5">
         <v>2</v>
@@ -9959,7 +9959,7 @@
         <v>1200</v>
       </c>
       <c r="D405" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E405" s="6" t="s">
         <v>186</v>
@@ -9967,7 +9967,7 @@
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B406" s="5">
         <v>2</v>
@@ -9976,7 +9976,7 @@
         <v>1000</v>
       </c>
       <c r="D406" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E406" s="6" t="s">
         <v>186</v>
@@ -9984,7 +9984,7 @@
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B407" s="5">
         <v>1</v>
@@ -9993,7 +9993,7 @@
         <v>250</v>
       </c>
       <c r="D407" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E407" s="6" t="s">
         <v>186</v>
@@ -10001,7 +10001,7 @@
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B408" s="5">
         <v>1</v>
@@ -10010,7 +10010,7 @@
         <v>250</v>
       </c>
       <c r="D408" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E408" s="6" t="s">
         <v>186</v>
@@ -10018,7 +10018,7 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B409" s="5">
         <v>2</v>
@@ -10027,7 +10027,7 @@
         <v>250</v>
       </c>
       <c r="D409" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E409" s="6" t="s">
         <v>186</v>
@@ -10035,7 +10035,7 @@
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B410" s="5">
         <v>0</v>
@@ -10044,7 +10044,7 @@
         <v>250</v>
       </c>
       <c r="D410" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E410" s="6" t="s">
         <v>186</v>
@@ -10052,7 +10052,7 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B411" s="5">
         <v>1</v>
@@ -10061,7 +10061,7 @@
         <v>250</v>
       </c>
       <c r="D411" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E411" s="6" t="s">
         <v>186</v>
@@ -10069,7 +10069,7 @@
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B412" s="5">
         <v>2</v>
@@ -10078,7 +10078,7 @@
         <v>250</v>
       </c>
       <c r="D412" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E412" s="6" t="s">
         <v>186</v>
@@ -10086,7 +10086,7 @@
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B413" s="5">
         <v>2</v>
@@ -10095,7 +10095,7 @@
         <v>250</v>
       </c>
       <c r="D413" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E413" s="6" t="s">
         <v>186</v>
@@ -10103,7 +10103,7 @@
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B414" s="5">
         <v>1</v>
@@ -10112,7 +10112,7 @@
         <v>250</v>
       </c>
       <c r="D414" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E414" s="6" t="s">
         <v>186</v>
@@ -10120,7 +10120,7 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B415" s="5">
         <v>1</v>
@@ -10129,7 +10129,7 @@
         <v>250</v>
       </c>
       <c r="D415" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E415" s="6" t="s">
         <v>186</v>
@@ -10137,7 +10137,7 @@
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B416" s="5">
         <v>1</v>
@@ -10146,7 +10146,7 @@
         <v>250</v>
       </c>
       <c r="D416" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E416" s="6" t="s">
         <v>186</v>
@@ -10154,7 +10154,7 @@
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B417" s="5">
         <v>2</v>
@@ -10163,7 +10163,7 @@
         <v>250</v>
       </c>
       <c r="D417" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E417" s="6" t="s">
         <v>186</v>
@@ -10171,7 +10171,7 @@
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B418" s="5">
         <v>1</v>
@@ -10180,7 +10180,7 @@
         <v>250</v>
       </c>
       <c r="D418" s="4" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E418" s="6" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
dc and stock update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30EF9AF-4F33-43EA-9372-9F0785D455B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE86BF5-6012-40BF-8979-F6DCA0CD23A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="1560" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -3069,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,7 +4887,7 @@
         <v>40</v>
       </c>
       <c r="B107" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C107" s="3">
         <v>350</v>
@@ -8321,7 +8321,7 @@
         <v>131</v>
       </c>
       <c r="B309" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C309" s="3">
         <v>265</v>

</xml_diff>

<commit_message>
New Category added, minibricks
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE63888-A272-40D5-A57F-166659E43A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4111082-7458-44FA-BC73-BEE4F09ECD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="1260" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="4560" yWindow="1935" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="896">
   <si>
     <t>Product</t>
   </si>
@@ -2515,6 +2515,213 @@
   </si>
   <si>
     <t>Ironman [MK85]</t>
+  </si>
+  <si>
+    <t>Pikachu MINI Bricks</t>
+  </si>
+  <si>
+    <t>pikachu bricks.jpg</t>
+  </si>
+  <si>
+    <t>Bricks</t>
+  </si>
+  <si>
+    <t>Jigglypuff MINI Bricks</t>
+  </si>
+  <si>
+    <t>Charizard MINI Bricks</t>
+  </si>
+  <si>
+    <t>Snorlax MINI Bricks</t>
+  </si>
+  <si>
+    <t>Eevee MINI Bricks</t>
+  </si>
+  <si>
+    <t>Venasaur MINI Bricks</t>
+  </si>
+  <si>
+    <t>Luffy MINI Bricks</t>
+  </si>
+  <si>
+    <t>Zoro MINI Bricks</t>
+  </si>
+  <si>
+    <t>Sanji MINI Bricks</t>
+  </si>
+  <si>
+    <t>Chopper MINI Bricks</t>
+  </si>
+  <si>
+    <t>Robin MINI Bricks</t>
+  </si>
+  <si>
+    <t>Sasuke MINI Bricks</t>
+  </si>
+  <si>
+    <t>Itachi MINI Bricks</t>
+  </si>
+  <si>
+    <t>Kakashi MINI Bricks</t>
+  </si>
+  <si>
+    <t>Goku MINI Bricks</t>
+  </si>
+  <si>
+    <t>Hello Kitty MINI Bricks</t>
+  </si>
+  <si>
+    <t>Ace MINI Bricks</t>
+  </si>
+  <si>
+    <t>Tanjiro MINI Bricks</t>
+  </si>
+  <si>
+    <t>Nezuko MINI Bricks</t>
+  </si>
+  <si>
+    <t>Zenitsu MINI Bricks</t>
+  </si>
+  <si>
+    <t>Giyuu MINI Bricks</t>
+  </si>
+  <si>
+    <t>Rengoku MINI Bricks</t>
+  </si>
+  <si>
+    <t>Tengen MINI Bricks</t>
+  </si>
+  <si>
+    <t>Shinobou MINI Bricks</t>
+  </si>
+  <si>
+    <t>Muichiro MINI Bricks</t>
+  </si>
+  <si>
+    <t>Kuromi MINI Bricks</t>
+  </si>
+  <si>
+    <t>Naruto MINI Bricks</t>
+  </si>
+  <si>
+    <t>Kitty bricks.jpg</t>
+  </si>
+  <si>
+    <t>kuromi bricks.jpg</t>
+  </si>
+  <si>
+    <t>jigglypuff bricks.jpg</t>
+  </si>
+  <si>
+    <t>charizard bricks.jpg</t>
+  </si>
+  <si>
+    <t>snorlax bricks.jpg</t>
+  </si>
+  <si>
+    <t>eevee bricks.jpg</t>
+  </si>
+  <si>
+    <t>venasaur bricks.jpg</t>
+  </si>
+  <si>
+    <t>luffy bricks.jpg</t>
+  </si>
+  <si>
+    <t>zoro bricks.jpg</t>
+  </si>
+  <si>
+    <t>sanji bricks.jpg</t>
+  </si>
+  <si>
+    <t>chopper bricks.jpg</t>
+  </si>
+  <si>
+    <t>robin bricks.jpg</t>
+  </si>
+  <si>
+    <t>ace bricks.jpg</t>
+  </si>
+  <si>
+    <t>naruto bricks.jpg</t>
+  </si>
+  <si>
+    <t>sasuke bricks.jpg</t>
+  </si>
+  <si>
+    <t>itachi bricks.jpg</t>
+  </si>
+  <si>
+    <t>kakashi bricks.jpg</t>
+  </si>
+  <si>
+    <t>goku bricks.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro bricks.jpg</t>
+  </si>
+  <si>
+    <t>nezuko bricks.jpg</t>
+  </si>
+  <si>
+    <t>zenitsu bricks.jpg</t>
+  </si>
+  <si>
+    <t>giyuu bricks.jpg</t>
+  </si>
+  <si>
+    <t>rengoku bricks.jpg</t>
+  </si>
+  <si>
+    <t>tengen bricks.jpg</t>
+  </si>
+  <si>
+    <t>shinobou bricks.jpg</t>
+  </si>
+  <si>
+    <t>muichiro bricks.jpg</t>
+  </si>
+  <si>
+    <t>Ash Ketchum [Hoenn]</t>
+  </si>
+  <si>
+    <t>Ash Ketchum [Sinnoh]</t>
+  </si>
+  <si>
+    <t>Ash Ketchum [Unova]</t>
+  </si>
+  <si>
+    <t>Ash Ketchum [Kalos]</t>
+  </si>
+  <si>
+    <t>ash hoenn.jpg</t>
+  </si>
+  <si>
+    <t>ash sinnoh.jpg</t>
+  </si>
+  <si>
+    <t>ash unova.jpg</t>
+  </si>
+  <si>
+    <t>ash kalos.jpg</t>
+  </si>
+  <si>
+    <t>Misty</t>
+  </si>
+  <si>
+    <t>Serena</t>
+  </si>
+  <si>
+    <t>Calem</t>
+  </si>
+  <si>
+    <t>misty.jpg</t>
+  </si>
+  <si>
+    <t>serena.jpg</t>
+  </si>
+  <si>
+    <t>calem.jpg</t>
   </si>
 </sst>
 </file>
@@ -3067,10 +3274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
-  <dimension ref="A1:E418"/>
+  <dimension ref="A1:E452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B384" sqref="B384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3513,7 @@
         <v>621</v>
       </c>
       <c r="B14" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="11">
         <v>280</v>
@@ -4887,7 +5094,7 @@
         <v>40</v>
       </c>
       <c r="B107" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C107" s="3">
         <v>350</v>
@@ -6808,7 +7015,7 @@
         <v>103</v>
       </c>
       <c r="B220" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C220" s="3">
         <v>250</v>
@@ -7267,7 +7474,7 @@
         <v>254</v>
       </c>
       <c r="B247" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C247" s="3">
         <v>250</v>
@@ -7420,7 +7627,7 @@
         <v>118</v>
       </c>
       <c r="B256" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C256" s="3">
         <v>350</v>
@@ -9596,7 +9803,7 @@
         <v>333</v>
       </c>
       <c r="B384" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C384" s="6">
         <v>800</v>
@@ -10184,6 +10391,584 @@
       </c>
       <c r="E418" s="6" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>827</v>
+      </c>
+      <c r="B419" s="5">
+        <v>1</v>
+      </c>
+      <c r="C419" s="6">
+        <v>200</v>
+      </c>
+      <c r="D419" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="E419" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>844</v>
+      </c>
+      <c r="B420" s="5">
+        <v>1</v>
+      </c>
+      <c r="C420" s="6">
+        <v>200</v>
+      </c>
+      <c r="D420" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="E420" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>854</v>
+      </c>
+      <c r="B421" s="5">
+        <v>1</v>
+      </c>
+      <c r="C421" s="6">
+        <v>200</v>
+      </c>
+      <c r="D421" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="E421" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>830</v>
+      </c>
+      <c r="B422" s="5">
+        <v>1</v>
+      </c>
+      <c r="C422" s="6">
+        <v>200</v>
+      </c>
+      <c r="D422" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="E422" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>831</v>
+      </c>
+      <c r="B423" s="5">
+        <v>1</v>
+      </c>
+      <c r="C423" s="6">
+        <v>200</v>
+      </c>
+      <c r="D423" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="E423" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>832</v>
+      </c>
+      <c r="B424" s="5">
+        <v>1</v>
+      </c>
+      <c r="C424" s="6">
+        <v>200</v>
+      </c>
+      <c r="D424" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="E424" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>833</v>
+      </c>
+      <c r="B425" s="5">
+        <v>1</v>
+      </c>
+      <c r="C425" s="6">
+        <v>200</v>
+      </c>
+      <c r="D425" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="E425" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>834</v>
+      </c>
+      <c r="B426" s="5">
+        <v>1</v>
+      </c>
+      <c r="C426" s="6">
+        <v>200</v>
+      </c>
+      <c r="D426" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="E426" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>835</v>
+      </c>
+      <c r="B427" s="5">
+        <v>2</v>
+      </c>
+      <c r="C427" s="6">
+        <v>200</v>
+      </c>
+      <c r="D427" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="E427" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>836</v>
+      </c>
+      <c r="B428" s="5">
+        <v>2</v>
+      </c>
+      <c r="C428" s="6">
+        <v>200</v>
+      </c>
+      <c r="D428" s="4" t="s">
+        <v>864</v>
+      </c>
+      <c r="E428" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>837</v>
+      </c>
+      <c r="B429" s="5">
+        <v>2</v>
+      </c>
+      <c r="C429" s="6">
+        <v>200</v>
+      </c>
+      <c r="D429" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="E429" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>838</v>
+      </c>
+      <c r="B430" s="5">
+        <v>1</v>
+      </c>
+      <c r="C430" s="6">
+        <v>200</v>
+      </c>
+      <c r="D430" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="E430" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>839</v>
+      </c>
+      <c r="B431" s="5">
+        <v>1</v>
+      </c>
+      <c r="C431" s="6">
+        <v>200</v>
+      </c>
+      <c r="D431" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="E431" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>845</v>
+      </c>
+      <c r="B432" s="5">
+        <v>1</v>
+      </c>
+      <c r="C432" s="6">
+        <v>200</v>
+      </c>
+      <c r="D432" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E432" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>855</v>
+      </c>
+      <c r="B433" s="5">
+        <v>2</v>
+      </c>
+      <c r="C433" s="6">
+        <v>200</v>
+      </c>
+      <c r="D433" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="E433" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>840</v>
+      </c>
+      <c r="B434" s="5">
+        <v>2</v>
+      </c>
+      <c r="C434" s="6">
+        <v>200</v>
+      </c>
+      <c r="D434" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="E434" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>841</v>
+      </c>
+      <c r="B435" s="5">
+        <v>2</v>
+      </c>
+      <c r="C435" s="6">
+        <v>200</v>
+      </c>
+      <c r="D435" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="E435" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>842</v>
+      </c>
+      <c r="B436" s="5">
+        <v>2</v>
+      </c>
+      <c r="C436" s="6">
+        <v>200</v>
+      </c>
+      <c r="D436" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="E436" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>843</v>
+      </c>
+      <c r="B437" s="5">
+        <v>2</v>
+      </c>
+      <c r="C437" s="6">
+        <v>200</v>
+      </c>
+      <c r="D437" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="E437" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>846</v>
+      </c>
+      <c r="B438" s="5">
+        <v>1</v>
+      </c>
+      <c r="C438" s="6">
+        <v>200</v>
+      </c>
+      <c r="D438" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="E438" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>847</v>
+      </c>
+      <c r="B439" s="5">
+        <v>2</v>
+      </c>
+      <c r="C439" s="6">
+        <v>200</v>
+      </c>
+      <c r="D439" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="E439" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>848</v>
+      </c>
+      <c r="B440" s="5">
+        <v>2</v>
+      </c>
+      <c r="C440" s="6">
+        <v>200</v>
+      </c>
+      <c r="D440" s="4" t="s">
+        <v>876</v>
+      </c>
+      <c r="E440" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>849</v>
+      </c>
+      <c r="B441" s="5">
+        <v>1</v>
+      </c>
+      <c r="C441" s="6">
+        <v>200</v>
+      </c>
+      <c r="D441" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="E441" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>850</v>
+      </c>
+      <c r="B442" s="5">
+        <v>1</v>
+      </c>
+      <c r="C442" s="6">
+        <v>200</v>
+      </c>
+      <c r="D442" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="E442" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>851</v>
+      </c>
+      <c r="B443" s="5">
+        <v>1</v>
+      </c>
+      <c r="C443" s="6">
+        <v>200</v>
+      </c>
+      <c r="D443" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="E443" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>852</v>
+      </c>
+      <c r="B444" s="5">
+        <v>1</v>
+      </c>
+      <c r="C444" s="6">
+        <v>200</v>
+      </c>
+      <c r="D444" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="E444" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>853</v>
+      </c>
+      <c r="B445" s="5">
+        <v>1</v>
+      </c>
+      <c r="C445" s="6">
+        <v>200</v>
+      </c>
+      <c r="D445" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="E445" s="6" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>882</v>
+      </c>
+      <c r="B446" s="5">
+        <v>1</v>
+      </c>
+      <c r="C446" s="6">
+        <v>200</v>
+      </c>
+      <c r="D446" s="4" t="s">
+        <v>886</v>
+      </c>
+      <c r="E446" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>883</v>
+      </c>
+      <c r="B447" s="5">
+        <v>1</v>
+      </c>
+      <c r="C447" s="6">
+        <v>200</v>
+      </c>
+      <c r="D447" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="E447" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>884</v>
+      </c>
+      <c r="B448" s="5">
+        <v>3</v>
+      </c>
+      <c r="C448" s="6">
+        <v>200</v>
+      </c>
+      <c r="D448" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="E448" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>885</v>
+      </c>
+      <c r="B449" s="5">
+        <v>3</v>
+      </c>
+      <c r="C449" s="6">
+        <v>200</v>
+      </c>
+      <c r="D449" s="4" t="s">
+        <v>889</v>
+      </c>
+      <c r="E449" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>890</v>
+      </c>
+      <c r="B450" s="5">
+        <v>1</v>
+      </c>
+      <c r="C450" s="6">
+        <v>150</v>
+      </c>
+      <c r="D450" s="4" t="s">
+        <v>893</v>
+      </c>
+      <c r="E450" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>891</v>
+      </c>
+      <c r="B451" s="5">
+        <v>4</v>
+      </c>
+      <c r="C451" s="6">
+        <v>150</v>
+      </c>
+      <c r="D451" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="E451" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>892</v>
+      </c>
+      <c r="B452" s="5">
+        <v>2</v>
+      </c>
+      <c r="C452" s="6">
+        <v>150</v>
+      </c>
+      <c r="D452" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="E452" s="6" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Keyring attachment feature added, stock update
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B48B322-863E-4F3F-9806-44339D3E8248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7269B909-5B50-423D-8672-7FF54B31797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="2085" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
+    <workbookView xWindow="0" yWindow="1035" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4074,8 +4074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E584"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B298" sqref="B298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5689,7 +5689,7 @@
         <v>714</v>
       </c>
       <c r="B95" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" s="3">
         <v>360</v>
@@ -5825,7 +5825,7 @@
         <v>884</v>
       </c>
       <c r="B103" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" s="3">
         <v>260</v>
@@ -5842,7 +5842,7 @@
         <v>885</v>
       </c>
       <c r="B104" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" s="3">
         <v>260</v>
@@ -5961,7 +5961,7 @@
         <v>892</v>
       </c>
       <c r="B111" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111" s="3">
         <v>260</v>
@@ -6284,7 +6284,7 @@
         <v>907</v>
       </c>
       <c r="B130" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C130" s="3">
         <v>280</v>
@@ -6930,7 +6930,7 @@
         <v>36</v>
       </c>
       <c r="B168" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C168" s="3">
         <v>300</v>
@@ -9106,7 +9106,7 @@
         <v>101</v>
       </c>
       <c r="B296" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C296" s="3">
         <v>260</v>
@@ -9140,7 +9140,7 @@
         <v>534</v>
       </c>
       <c r="B298" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C298" s="3">
         <v>280</v>
@@ -11486,7 +11486,7 @@
         <v>1104</v>
       </c>
       <c r="B436" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C436" s="3">
         <v>260</v>

</xml_diff>

<commit_message>
Add sitemap and robots.txt
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38A0562-CFA3-49B8-AB71-AF9E9F7F9FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEE8FFD-B668-4CDE-B26A-E59B118F3264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2955" yWindow="1680" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="1292">
   <si>
     <t>Product</t>
   </si>
@@ -3907,6 +3907,9 @@
   </si>
   <si>
     <t>dp.jpeg</t>
+  </si>
+  <si>
+    <t>Moonknight v3</t>
   </si>
 </sst>
 </file>
@@ -4461,8 +4464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E648"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A172" sqref="A172:XFD176"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4614,7 +4617,7 @@
         <v>1166</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3">
         <v>260</v>
@@ -6977,7 +6980,7 @@
         <v>908</v>
       </c>
       <c r="B148" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C148" s="3">
         <v>260</v>
@@ -7348,10 +7351,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>1144</v>
+        <v>1291</v>
       </c>
       <c r="B170" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C170" s="3">
         <v>260</v>
@@ -7402,7 +7405,7 @@
         <v>723</v>
       </c>
       <c r="B173" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C173" s="14">
         <v>270</v>

</xml_diff>

<commit_message>
stock update, how to order removed
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75D53C4-59ED-49D8-BD4A-5373AD14955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96836230-0112-4D97-9975-4714FE757EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="1380" windowWidth="21600" windowHeight="11250" xr2:uid="{FC0CBB84-858B-49F6-BA69-44D83C89F7C4}"/>
   </bookViews>
@@ -4023,9 +4023,6 @@
     <t>sentry1.jpeg</t>
   </si>
   <si>
-    <t>red.jpg</t>
-  </si>
-  <si>
     <t>usagent.jpeg</t>
   </si>
   <si>
@@ -4078,6 +4075,9 @@
   </si>
   <si>
     <t>One Piece, Others</t>
+  </si>
+  <si>
+    <t>red.jpeg</t>
   </si>
 </sst>
 </file>
@@ -4632,8 +4632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDC9875-9E8E-485C-910E-47B83A1F9902}">
   <dimension ref="A1:E674"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A655" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E654" sqref="E654:E656"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4662,93 +4662,93 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>560</v>
+      <c r="A2" s="7" t="s">
+        <v>1314</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3">
         <v>260</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>566</v>
+        <v>1316</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>561</v>
+      <c r="A3" s="7" t="s">
+        <v>1317</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
         <v>260</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>567</v>
+        <v>1315</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>562</v>
+      <c r="A4" s="7" t="s">
+        <v>1318</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>260</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>568</v>
+        <v>1324</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>563</v>
+      <c r="A5" s="7" t="s">
+        <v>1319</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>569</v>
+        <v>1328</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>564</v>
+      <c r="A6" s="7" t="s">
+        <v>1330</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
         <v>260</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>570</v>
+        <v>1325</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>565</v>
+      <c r="A7" s="7" t="s">
+        <v>1320</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -4757,7 +4757,7 @@
         <v>260</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>571</v>
+        <v>1326</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -4765,16 +4765,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>1159</v>
+        <v>1321</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
       </c>
       <c r="C8" s="3">
-        <v>550</v>
+        <v>260</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>1182</v>
+        <v>1347</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -4782,16 +4782,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>1160</v>
+        <v>1322</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
         <v>260</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>1177</v>
+        <v>1329</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
@@ -4799,24 +4799,24 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>1161</v>
+        <v>1323</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>1178</v>
+        <v>1327</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>1162</v>
+      <c r="A11" s="2" t="s">
+        <v>560</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -4825,24 +4825,24 @@
         <v>260</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>1179</v>
+        <v>566</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>1163</v>
+      <c r="A12" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>1180</v>
+        <v>567</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -4850,288 +4850,288 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>783</v>
+        <v>562</v>
       </c>
       <c r="B13" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>1346</v>
+        <v>568</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>784</v>
+        <v>563</v>
       </c>
       <c r="B14" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>789</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>1346</v>
+        <v>569</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>785</v>
+      <c r="A15" s="2" t="s">
+        <v>564</v>
       </c>
       <c r="B15" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>788</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>1346</v>
+        <v>570</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>791</v>
+      <c r="A16" s="2" t="s">
+        <v>565</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
       </c>
       <c r="C16" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>1346</v>
+        <v>571</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>786</v>
+      <c r="A17" s="7" t="s">
+        <v>1159</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
       <c r="C17" s="3">
+        <v>550</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>260</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
         <v>300</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D19" s="8" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>260</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>320</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="B22" s="3">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3">
+        <v>300</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>300</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>785</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3">
+        <v>300</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>300</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>300</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>792</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="E26" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>572</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B27" s="10">
         <v>4</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C27" s="11">
         <v>660</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="E27" s="6" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="B19" s="10">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11">
         <v>280</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>596</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>220</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>794</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>220</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3">
-        <v>360</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>560</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>180</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>180</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B26" s="3">
-        <v>3</v>
-      </c>
-      <c r="C26" s="3">
-        <v>200</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>180</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="3">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3">
-        <v>200</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>1284</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>1339</v>
+      <c r="E28" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="3">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>1283</v>
+        <v>133</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
@@ -5139,16 +5139,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>507</v>
+        <v>794</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3">
-        <v>260</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>251</v>
+        <v>220</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>1098</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
@@ -5156,16 +5156,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>588</v>
+        <v>498</v>
       </c>
       <c r="B31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>589</v>
+        <v>134</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -5173,16 +5173,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>246</v>
+        <v>771</v>
       </c>
       <c r="B32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="3">
-        <v>260</v>
+        <v>560</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>252</v>
+        <v>772</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
@@ -5190,16 +5190,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>590</v>
+        <v>7</v>
       </c>
       <c r="B33" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="3">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>591</v>
+        <v>135</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -5207,16 +5207,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>371</v>
+        <v>8</v>
       </c>
       <c r="B34" s="3">
         <v>0</v>
       </c>
       <c r="C34" s="3">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>370</v>
+        <v>136</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -5224,16 +5224,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>247</v>
+        <v>499</v>
       </c>
       <c r="B35" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35" s="3">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
@@ -5241,16 +5241,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>248</v>
+        <v>9</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="3">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>255</v>
+        <v>136</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
@@ -5258,33 +5258,33 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>368</v>
+        <v>10</v>
       </c>
       <c r="B37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="3">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>6</v>
+        <v>1284</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>1338</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>249</v>
+        <v>19</v>
       </c>
       <c r="B38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="3">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>253</v>
+        <v>1283</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>250</v>
+        <v>507</v>
       </c>
       <c r="B39" s="3">
         <v>0</v>
@@ -5301,7 +5301,7 @@
         <v>260</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
@@ -5309,16 +5309,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="3">
         <v>260</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -5326,16 +5326,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>593</v>
+        <v>246</v>
       </c>
       <c r="B41" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="3">
         <v>260</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>595</v>
+        <v>252</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
@@ -5343,16 +5343,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>372</v>
+        <v>590</v>
       </c>
       <c r="B42" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42" s="3">
         <v>260</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>373</v>
+        <v>591</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
@@ -5360,16 +5360,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>371</v>
       </c>
       <c r="B43" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>226</v>
+        <v>370</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -5377,16 +5377,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>12</v>
+        <v>247</v>
       </c>
       <c r="B44" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C44" s="3">
-        <v>220</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>1108</v>
+        <v>260</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
@@ -5394,16 +5394,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>13</v>
+        <v>248</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
       </c>
       <c r="C45" s="3">
-        <v>220</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>227</v>
+        <v>260</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
@@ -5411,16 +5411,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>14</v>
+        <v>368</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>228</v>
+        <v>369</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
@@ -5428,16 +5428,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>249</v>
       </c>
       <c r="B47" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
@@ -5445,16 +5445,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="B48" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
@@ -5462,16 +5462,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>17</v>
+        <v>592</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C49" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>231</v>
+        <v>594</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
@@ -5479,16 +5479,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>18</v>
+        <v>593</v>
       </c>
       <c r="B50" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>136</v>
+        <v>595</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
@@ -5496,16 +5496,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>20</v>
+        <v>372</v>
       </c>
       <c r="B51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>137</v>
+        <v>373</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
@@ -5513,16 +5513,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>674</v>
+        <v>226</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -5530,16 +5530,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B53" s="3">
         <v>3</v>
       </c>
       <c r="C53" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>673</v>
+        <v>1108</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>6</v>
@@ -5547,16 +5547,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B54" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>675</v>
+        <v>227</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>6</v>
@@ -5564,16 +5564,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>1130</v>
+        <v>14</v>
       </c>
       <c r="B55" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3">
-        <v>180</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>676</v>
+        <v>220</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>6</v>
@@ -5581,16 +5581,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>500</v>
+        <v>15</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
       </c>
       <c r="C56" s="3">
-        <v>180</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>677</v>
+        <v>220</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>6</v>
@@ -5598,16 +5598,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>501</v>
+        <v>16</v>
       </c>
       <c r="B57" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>678</v>
+        <v>230</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>6</v>
@@ -5615,16 +5615,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B58" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>679</v>
+        <v>231</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>6</v>
@@ -5632,16 +5632,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>630</v>
+        <v>18</v>
       </c>
       <c r="B59" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C59" s="3">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>631</v>
+        <v>136</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>6</v>
@@ -5649,16 +5649,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>1131</v>
+        <v>20</v>
       </c>
       <c r="B60" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="3">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>1132</v>
+        <v>137</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>6</v>
@@ -5666,16 +5666,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>502</v>
+        <v>21</v>
       </c>
       <c r="B61" s="3">
         <v>2</v>
       </c>
       <c r="C61" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>198</v>
+        <v>674</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>6</v>
@@ -5683,16 +5683,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>503</v>
+        <v>22</v>
       </c>
       <c r="B62" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="3">
-        <v>270</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>138</v>
+        <v>180</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>673</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>6</v>
@@ -5700,16 +5700,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>504</v>
+        <v>23</v>
       </c>
       <c r="B63" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C63" s="3">
-        <v>270</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>199</v>
+        <v>180</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>675</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
@@ -5717,16 +5717,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>25</v>
+        <v>1130</v>
       </c>
       <c r="B64" s="3">
         <v>2</v>
       </c>
       <c r="C64" s="3">
-        <v>460</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>200</v>
+        <v>180</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>676</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
@@ -5734,16 +5734,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>864</v>
+        <v>500</v>
       </c>
       <c r="B65" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65" s="3">
-        <v>460</v>
+        <v>180</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>915</v>
+        <v>677</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>6</v>
@@ -5751,16 +5751,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>865</v>
+        <v>501</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
       </c>
       <c r="C66" s="3">
-        <v>260</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>916</v>
+        <v>180</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>678</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>6</v>
@@ -5768,16 +5768,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>866</v>
+        <v>24</v>
       </c>
       <c r="B67" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" s="3">
-        <v>260</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>917</v>
+        <v>180</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>679</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>6</v>
@@ -5785,16 +5785,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>26</v>
+        <v>630</v>
       </c>
       <c r="B68" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C68" s="3">
-        <v>380</v>
+        <v>180</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>140</v>
+        <v>631</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>6</v>
@@ -5802,16 +5802,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>27</v>
+        <v>1131</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
       </c>
       <c r="C69" s="3">
-        <v>800</v>
+        <v>260</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>142</v>
+        <v>1132</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>6</v>
@@ -5819,16 +5819,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>28</v>
+        <v>502</v>
       </c>
       <c r="B70" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C70" s="3">
         <v>270</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>6</v>
@@ -5836,16 +5836,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>29</v>
+        <v>503</v>
       </c>
       <c r="B71" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C71" s="3">
         <v>270</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>6</v>
@@ -5853,16 +5853,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>30</v>
+        <v>504</v>
       </c>
       <c r="B72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" s="3">
         <v>270</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>6</v>
@@ -5870,16 +5870,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>505</v>
+        <v>25</v>
       </c>
       <c r="B73" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C73" s="3">
-        <v>260</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>390</v>
+        <v>460</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>6</v>
@@ -5887,16 +5887,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>31</v>
+        <v>864</v>
       </c>
       <c r="B74" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" s="3">
-        <v>850</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>141</v>
+        <v>460</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>915</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>6</v>
@@ -5904,16 +5904,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>1139</v>
+        <v>865</v>
       </c>
       <c r="B75" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="3">
         <v>260</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>168</v>
+      <c r="D75" s="8" t="s">
+        <v>916</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>6</v>
@@ -5921,16 +5921,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>1142</v>
+        <v>866</v>
       </c>
       <c r="B76" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C76" s="3">
         <v>260</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>201</v>
+      <c r="D76" s="8" t="s">
+        <v>917</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>6</v>
@@ -5938,16 +5938,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B77" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C77" s="3">
-        <v>260</v>
+        <v>380</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>202</v>
+        <v>140</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>6</v>
@@ -5955,16 +5955,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" s="3">
-        <v>260</v>
+        <v>800</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>6</v>
@@ -5972,16 +5972,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>276</v>
+        <v>28</v>
       </c>
       <c r="B79" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C79" s="3">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>6</v>
@@ -5989,16 +5989,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>1140</v>
+        <v>29</v>
       </c>
       <c r="B80" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C80" s="3">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>6</v>
@@ -6006,16 +6006,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>1141</v>
+        <v>30</v>
       </c>
       <c r="B81" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" s="3">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>6</v>
@@ -6023,16 +6023,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>277</v>
+        <v>505</v>
       </c>
       <c r="B82" s="3">
         <v>0</v>
       </c>
       <c r="C82" s="3">
-        <v>360</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>234</v>
+        <v>260</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>390</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>6</v>
@@ -6040,16 +6040,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="B83" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C83" s="3">
-        <v>360</v>
+        <v>850</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>235</v>
+        <v>141</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>6</v>
@@ -6057,50 +6057,50 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>204</v>
+        <v>1139</v>
       </c>
       <c r="B84" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84" s="3">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>506</v>
+      <c r="A85" s="1" t="s">
+        <v>1142</v>
       </c>
       <c r="B85" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C85" s="3">
         <v>260</v>
       </c>
-      <c r="D85" s="8" t="s">
-        <v>391</v>
+      <c r="D85" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>793</v>
+      <c r="A86" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B86" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C86" s="3">
         <v>260</v>
       </c>
-      <c r="D86" s="8" t="s">
-        <v>392</v>
+      <c r="D86" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>6</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>383</v>
+        <v>33</v>
       </c>
       <c r="B87" s="3">
         <v>0</v>
@@ -6116,8 +6116,8 @@
       <c r="C87" s="3">
         <v>260</v>
       </c>
-      <c r="D87" s="8" t="s">
-        <v>394</v>
+      <c r="D87" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>6</v>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>384</v>
+        <v>276</v>
       </c>
       <c r="B88" s="3">
         <v>2</v>
@@ -6133,42 +6133,42 @@
       <c r="C88" s="3">
         <v>260</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>395</v>
+      <c r="D88" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>388</v>
+      <c r="A89" s="1" t="s">
+        <v>1140</v>
       </c>
       <c r="B89" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C89" s="3">
-        <v>220</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>396</v>
+        <v>260</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
-        <v>389</v>
+      <c r="A90" s="1" t="s">
+        <v>1141</v>
       </c>
       <c r="B90" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C90" s="3">
         <v>260</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>136</v>
+      <c r="D90" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>6</v>
@@ -6176,33 +6176,33 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>385</v>
+        <v>277</v>
       </c>
       <c r="B91" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C91" s="3">
-        <v>260</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>397</v>
+        <v>360</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
-        <v>525</v>
+      <c r="A92" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="B92" s="3">
         <v>0</v>
       </c>
       <c r="C92" s="3">
-        <v>260</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>398</v>
+        <v>360</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>6</v>
@@ -6210,16 +6210,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>386</v>
+        <v>204</v>
       </c>
       <c r="B93" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C93" s="3">
-        <v>260</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>393</v>
+        <v>200</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>6</v>
@@ -6227,67 +6227,67 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="B94" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C94" s="3">
         <v>260</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>387</v>
+      <c r="A95" s="7" t="s">
+        <v>793</v>
       </c>
       <c r="B95" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C95" s="3">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>698</v>
+      <c r="A96" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="B96" s="3">
         <v>0</v>
       </c>
       <c r="C96" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>703</v>
+        <v>394</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
-        <v>699</v>
+      <c r="A97" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="B97" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C97" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>704</v>
+        <v>395</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>6</v>
@@ -6295,16 +6295,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>700</v>
+        <v>388</v>
       </c>
       <c r="B98" s="3">
         <v>0</v>
       </c>
       <c r="C98" s="3">
-        <v>360</v>
+        <v>220</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>706</v>
+        <v>396</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>6</v>
@@ -6312,33 +6312,33 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>701</v>
+        <v>389</v>
       </c>
       <c r="B99" s="3">
         <v>0</v>
       </c>
       <c r="C99" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>705</v>
+        <v>136</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>702</v>
+      <c r="A100" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="B100" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C100" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>729</v>
+        <v>397</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>6</v>
@@ -6346,33 +6346,33 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>730</v>
+        <v>525</v>
       </c>
       <c r="B101" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>731</v>
+        <v>398</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
-        <v>867</v>
+      <c r="A102" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="B102" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C102" s="3">
         <v>260</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>976</v>
+        <v>393</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>6</v>
@@ -6380,33 +6380,33 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>868</v>
+        <v>524</v>
       </c>
       <c r="B103" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C103" s="3">
         <v>260</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>977</v>
+        <v>399</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
-        <v>869</v>
+      <c r="A104" s="1" t="s">
+        <v>387</v>
       </c>
       <c r="B104" s="3">
         <v>1</v>
       </c>
       <c r="C104" s="3">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>987</v>
+        <v>400</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>6</v>
@@ -6414,16 +6414,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>1090</v>
+        <v>698</v>
       </c>
       <c r="B105" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>978</v>
+        <v>703</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>6</v>
@@ -6431,16 +6431,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>870</v>
+        <v>699</v>
       </c>
       <c r="B106" s="3">
         <v>0</v>
       </c>
       <c r="C106" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>988</v>
+        <v>704</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>6</v>
@@ -6448,16 +6448,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>871</v>
+        <v>700</v>
       </c>
       <c r="B107" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C107" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>979</v>
+        <v>706</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>6</v>
@@ -6465,16 +6465,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>872</v>
+        <v>701</v>
       </c>
       <c r="B108" s="3">
         <v>0</v>
       </c>
       <c r="C108" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>980</v>
+        <v>705</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>6</v>
@@ -6482,16 +6482,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>873</v>
+        <v>702</v>
       </c>
       <c r="B109" s="3">
         <v>0</v>
       </c>
       <c r="C109" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>981</v>
+        <v>729</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>6</v>
@@ -6499,16 +6499,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>874</v>
+        <v>730</v>
       </c>
       <c r="B110" s="3">
         <v>1</v>
       </c>
       <c r="C110" s="3">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>982</v>
+        <v>731</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>6</v>
@@ -6516,16 +6516,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="B111" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C111" s="3">
         <v>260</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>989</v>
+        <v>976</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>6</v>
@@ -6533,16 +6533,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="B112" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C112" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1113</v>
+        <v>977</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>6</v>
@@ -6550,16 +6550,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
       </c>
       <c r="C113" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>6</v>
@@ -6567,16 +6567,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>878</v>
+        <v>1090</v>
       </c>
       <c r="B114" s="3">
         <v>1</v>
       </c>
       <c r="C114" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>991</v>
+        <v>978</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>6</v>
@@ -6584,16 +6584,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="B115" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C115" s="3">
         <v>260</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>6</v>
@@ -6601,16 +6601,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
       <c r="B116" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C116" s="3">
         <v>260</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>993</v>
+        <v>979</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>6</v>
@@ -6618,16 +6618,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>1143</v>
+        <v>872</v>
       </c>
       <c r="B117" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="3">
         <v>260</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>994</v>
+        <v>980</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>6</v>
@@ -6635,16 +6635,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="B118" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118" s="3">
         <v>260</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>995</v>
+        <v>981</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>6</v>
@@ -6652,16 +6652,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="B119" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C119" s="3">
         <v>260</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>996</v>
+        <v>982</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>6</v>
@@ -6669,16 +6669,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="B120" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C120" s="3">
-        <v>150</v>
+        <v>260</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>6</v>
@@ -6686,16 +6686,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="B121" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C121" s="3">
-        <v>150</v>
+        <v>280</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>984</v>
+        <v>1113</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>6</v>
@@ -6703,16 +6703,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="B122" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122" s="3">
-        <v>360</v>
+        <v>280</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>985</v>
+        <v>990</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>6</v>
@@ -6720,16 +6720,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B123" s="3">
         <v>1</v>
       </c>
       <c r="C123" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>986</v>
+        <v>991</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>6</v>
@@ -6737,16 +6737,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="B124" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C124" s="3">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1128</v>
+        <v>992</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>6</v>
@@ -6754,16 +6754,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="B125" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C125" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>6</v>
@@ -6771,16 +6771,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>889</v>
+        <v>1143</v>
       </c>
       <c r="B126" s="3">
         <v>1</v>
       </c>
       <c r="C126" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>6</v>
@@ -6788,16 +6788,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
       </c>
       <c r="C127" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>6</v>
@@ -6805,16 +6805,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>1114</v>
+        <v>882</v>
       </c>
       <c r="B128" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C128" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1115</v>
+        <v>996</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>6</v>
@@ -6822,16 +6822,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>1082</v>
+        <v>883</v>
       </c>
       <c r="B129" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C129" s="3">
-        <v>280</v>
+        <v>150</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1000</v>
+        <v>983</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>6</v>
@@ -6839,16 +6839,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="B130" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C130" s="3">
-        <v>320</v>
+        <v>150</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1001</v>
+        <v>984</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>6</v>
@@ -6856,16 +6856,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="B131" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="3">
-        <v>280</v>
+        <v>360</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1002</v>
+        <v>985</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>6</v>
@@ -6873,16 +6873,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="B132" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C132" s="3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1003</v>
+        <v>986</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>6</v>
@@ -6890,16 +6890,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="B133" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C133" s="3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1004</v>
+        <v>1128</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>6</v>
@@ -6907,16 +6907,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>1096</v>
+        <v>888</v>
       </c>
       <c r="B134" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1097</v>
+        <v>997</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>6</v>
@@ -6924,16 +6924,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="B135" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C135" s="3">
         <v>280</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1005</v>
+        <v>998</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>6</v>
@@ -6941,16 +6941,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="B136" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C136" s="3">
         <v>280</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1006</v>
+        <v>999</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>6</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="B137" s="3">
         <v>1</v>
@@ -6967,7 +6967,7 @@
         <v>280</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1007</v>
+        <v>1115</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>6</v>
@@ -6975,16 +6975,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>897</v>
+        <v>1082</v>
       </c>
       <c r="B138" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C138" s="3">
         <v>280</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1008</v>
+        <v>1000</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>6</v>
@@ -6992,16 +6992,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="B139" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C139" s="3">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1009</v>
+        <v>1001</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>6</v>
@@ -7009,7 +7009,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="B140" s="3">
         <v>1</v>
@@ -7018,7 +7018,7 @@
         <v>280</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1010</v>
+        <v>1002</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>6</v>
@@ -7026,16 +7026,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="B141" s="3">
         <v>0</v>
       </c>
       <c r="C141" s="3">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1011</v>
+        <v>1003</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>6</v>
@@ -7043,16 +7043,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>901</v>
+        <v>894</v>
       </c>
       <c r="B142" s="3">
         <v>0</v>
       </c>
       <c r="C142" s="3">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1124</v>
+        <v>1004</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>6</v>
@@ -7060,16 +7060,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>902</v>
+        <v>1096</v>
       </c>
       <c r="B143" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C143" s="3">
         <v>260</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1012</v>
+        <v>1097</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>6</v>
@@ -7077,16 +7077,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>1126</v>
+        <v>895</v>
       </c>
       <c r="B144" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1125</v>
+        <v>1005</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>6</v>
@@ -7094,16 +7094,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>1144</v>
+        <v>896</v>
       </c>
       <c r="B145" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C145" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>6</v>
@@ -7111,16 +7111,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>1145</v>
+        <v>1107</v>
       </c>
       <c r="B146" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>1014</v>
+        <v>1007</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>6</v>
@@ -7128,16 +7128,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="B147" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1015</v>
+        <v>1008</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>6</v>
@@ -7145,16 +7145,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B148" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C148" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>6</v>
@@ -7162,16 +7162,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="B149" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C149" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>6</v>
@@ -7179,7 +7179,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="B150" s="3">
         <v>0</v>
@@ -7188,7 +7188,7 @@
         <v>260</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>1018</v>
+        <v>1011</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>6</v>
@@ -7196,16 +7196,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>1095</v>
+        <v>901</v>
       </c>
       <c r="B151" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C151" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>1019</v>
+        <v>1124</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>6</v>
@@ -7213,16 +7213,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="B152" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>1020</v>
+        <v>1012</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>6</v>
@@ -7230,16 +7230,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>908</v>
+        <v>1126</v>
       </c>
       <c r="B153" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C153" s="3">
         <v>260</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>1021</v>
+        <v>1125</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>6</v>
@@ -7247,16 +7247,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>909</v>
+        <v>1144</v>
       </c>
       <c r="B154" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C154" s="3">
         <v>260</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>6</v>
@@ -7264,16 +7264,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>910</v>
+        <v>1145</v>
       </c>
       <c r="B155" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155" s="3">
         <v>260</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>6</v>
@@ -7281,16 +7281,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="B156" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C156" s="3">
         <v>260</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>6</v>
@@ -7298,16 +7298,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="B157" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157" s="3">
         <v>260</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1025</v>
+        <v>1016</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>6</v>
@@ -7315,7 +7315,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="B158" s="3">
         <v>2</v>
@@ -7324,7 +7324,7 @@
         <v>260</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>6</v>
@@ -7332,16 +7332,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="B159" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="3">
         <v>260</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>1027</v>
+        <v>1018</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>6</v>
@@ -7349,16 +7349,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>1148</v>
+        <v>1095</v>
       </c>
       <c r="B160" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C160" s="3">
-        <v>400</v>
+        <v>280</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1165</v>
+        <v>1019</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>6</v>
@@ -7366,16 +7366,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>1149</v>
+        <v>907</v>
       </c>
       <c r="B161" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C161" s="3">
-        <v>280</v>
+        <v>360</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1166</v>
+        <v>1020</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>6</v>
@@ -7383,16 +7383,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>1150</v>
+        <v>908</v>
       </c>
       <c r="B162" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C162" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1167</v>
+        <v>1021</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>6</v>
@@ -7400,16 +7400,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>1151</v>
+        <v>909</v>
       </c>
       <c r="B163" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C163" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1168</v>
+        <v>1022</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>6</v>
@@ -7417,16 +7417,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>1152</v>
+        <v>910</v>
       </c>
       <c r="B164" s="3">
         <v>1</v>
       </c>
       <c r="C164" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1169</v>
+        <v>1023</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>6</v>
@@ -7434,16 +7434,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>1153</v>
+        <v>911</v>
       </c>
       <c r="B165" s="3">
         <v>2</v>
       </c>
       <c r="C165" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1170</v>
+        <v>1024</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>6</v>
@@ -7451,16 +7451,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>1154</v>
+        <v>912</v>
       </c>
       <c r="B166" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C166" s="3">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1171</v>
+        <v>1025</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>6</v>
@@ -7468,16 +7468,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>1155</v>
+        <v>913</v>
       </c>
       <c r="B167" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C167" s="3">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1172</v>
+        <v>1026</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>6</v>
@@ -7485,7 +7485,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>1156</v>
+        <v>914</v>
       </c>
       <c r="B168" s="3">
         <v>1</v>
@@ -7494,7 +7494,7 @@
         <v>260</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1173</v>
+        <v>1027</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>6</v>
@@ -7502,16 +7502,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="B169" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C169" s="3">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>6</v>
@@ -7519,16 +7519,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>1285</v>
+        <v>1149</v>
       </c>
       <c r="B170" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C170" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>6</v>
@@ -7536,16 +7536,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
       <c r="B171" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C171" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>6</v>
@@ -7553,16 +7553,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>1164</v>
+        <v>1151</v>
       </c>
       <c r="B172" s="3">
         <v>3</v>
       </c>
       <c r="C172" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1181</v>
+        <v>1168</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>6</v>
@@ -7570,16 +7570,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>1314</v>
+        <v>1152</v>
       </c>
       <c r="B173" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C173" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1316</v>
+        <v>1169</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>6</v>
@@ -7587,16 +7587,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>1317</v>
+        <v>1153</v>
       </c>
       <c r="B174" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C174" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1315</v>
+        <v>1170</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>6</v>
@@ -7604,16 +7604,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>1318</v>
+        <v>1154</v>
       </c>
       <c r="B175" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C175" s="3">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>1324</v>
+        <v>1171</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>6</v>
@@ -7621,16 +7621,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
-        <v>1319</v>
+        <v>1155</v>
       </c>
       <c r="B176" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C176" s="3">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1328</v>
+        <v>1172</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>6</v>
@@ -7638,16 +7638,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>1331</v>
+        <v>1156</v>
       </c>
       <c r="B177" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C177" s="3">
         <v>260</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1325</v>
+        <v>1173</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>6</v>
@@ -7655,16 +7655,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
-        <v>1320</v>
+        <v>1157</v>
       </c>
       <c r="B178" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178" s="3">
         <v>260</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1326</v>
+        <v>1174</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>6</v>
@@ -7672,16 +7672,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>1321</v>
+        <v>1285</v>
       </c>
       <c r="B179" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C179" s="3">
         <v>260</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1329</v>
+        <v>1175</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>6</v>
@@ -7689,16 +7689,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>1322</v>
+        <v>1158</v>
       </c>
       <c r="B180" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C180" s="3">
         <v>260</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1330</v>
+        <v>1176</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>6</v>
@@ -7706,16 +7706,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>1323</v>
+        <v>1164</v>
       </c>
       <c r="B181" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C181" s="3">
         <v>260</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1327</v>
+        <v>1181</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>6</v>
@@ -10327,7 +10327,7 @@
         <v>272</v>
       </c>
       <c r="B335" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C335" s="3">
         <v>280</v>
@@ -11939,7 +11939,7 @@
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B430" s="3">
         <v>2</v>
@@ -11948,7 +11948,7 @@
         <v>320</v>
       </c>
       <c r="D430" s="8" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="E430" s="3" t="s">
         <v>118</v>
@@ -11956,7 +11956,7 @@
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B431" s="3">
         <v>2</v>
@@ -11965,7 +11965,7 @@
         <v>320</v>
       </c>
       <c r="D431" s="8" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E431" s="3" t="s">
         <v>118</v>
@@ -11973,7 +11973,7 @@
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B432" s="3">
         <v>2</v>
@@ -11982,7 +11982,7 @@
         <v>320</v>
       </c>
       <c r="D432" s="8" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="E432" s="3" t="s">
         <v>118</v>
@@ -13073,7 +13073,7 @@
         <v>224</v>
       </c>
       <c r="E496" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -13090,7 +13090,7 @@
         <v>281</v>
       </c>
       <c r="E497" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
@@ -13447,7 +13447,7 @@
         <v>225</v>
       </c>
       <c r="E518" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
@@ -14730,7 +14730,7 @@
         <v>800</v>
       </c>
       <c r="B594" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C594" s="6">
         <v>200</v>
@@ -15232,7 +15232,7 @@
         <v>1065</v>
       </c>
       <c r="E623" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -15249,7 +15249,7 @@
         <v>1066</v>
       </c>
       <c r="E624" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -15266,7 +15266,7 @@
         <v>1067</v>
       </c>
       <c r="E625" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -15283,7 +15283,7 @@
         <v>1068</v>
       </c>
       <c r="E626" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -15300,7 +15300,7 @@
         <v>1069</v>
       </c>
       <c r="E627" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -15317,7 +15317,7 @@
         <v>1070</v>
       </c>
       <c r="E628" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -15334,7 +15334,7 @@
         <v>1071</v>
       </c>
       <c r="E629" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -15385,7 +15385,7 @@
         <v>1074</v>
       </c>
       <c r="E632" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
@@ -15402,7 +15402,7 @@
         <v>1075</v>
       </c>
       <c r="E633" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
@@ -15419,7 +15419,7 @@
         <v>1076</v>
       </c>
       <c r="E634" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
@@ -15436,7 +15436,7 @@
         <v>1077</v>
       </c>
       <c r="E635" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.25">
@@ -15453,7 +15453,7 @@
         <v>1078</v>
       </c>
       <c r="E636" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
@@ -15470,7 +15470,7 @@
         <v>1079</v>
       </c>
       <c r="E637" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
@@ -15487,7 +15487,7 @@
         <v>1080</v>
       </c>
       <c r="E638" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.25">
@@ -15538,7 +15538,7 @@
         <v>1081</v>
       </c>
       <c r="E641" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="642" spans="1:5" x14ac:dyDescent="0.25">
@@ -15555,7 +15555,7 @@
         <v>1086</v>
       </c>
       <c r="E642" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.25">
@@ -15572,7 +15572,7 @@
         <v>1088</v>
       </c>
       <c r="E643" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="644" spans="1:5" x14ac:dyDescent="0.25">
@@ -15589,7 +15589,7 @@
         <v>1106</v>
       </c>
       <c r="E644" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="645" spans="1:5" x14ac:dyDescent="0.25">
@@ -15606,7 +15606,7 @@
         <v>1256</v>
       </c>
       <c r="E645" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
@@ -15623,7 +15623,7 @@
         <v>1264</v>
       </c>
       <c r="E646" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="647" spans="1:5" x14ac:dyDescent="0.25">
@@ -15640,7 +15640,7 @@
         <v>1265</v>
       </c>
       <c r="E647" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="648" spans="1:5" x14ac:dyDescent="0.25">
@@ -15657,7 +15657,7 @@
         <v>1257</v>
       </c>
       <c r="E648" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.25">
@@ -15674,7 +15674,7 @@
         <v>1266</v>
       </c>
       <c r="E649" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.25">
@@ -15691,7 +15691,7 @@
         <v>1267</v>
       </c>
       <c r="E650" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="651" spans="1:5" x14ac:dyDescent="0.25">
@@ -15708,7 +15708,7 @@
         <v>1268</v>
       </c>
       <c r="E651" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.25">
@@ -15725,7 +15725,7 @@
         <v>1269</v>
       </c>
       <c r="E652" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.25">
@@ -15742,7 +15742,7 @@
         <v>1270</v>
       </c>
       <c r="E653" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="654" spans="1:5" x14ac:dyDescent="0.25">
@@ -15759,7 +15759,7 @@
         <v>1271</v>
       </c>
       <c r="E654" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.25">
@@ -15776,7 +15776,7 @@
         <v>1272</v>
       </c>
       <c r="E655" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
@@ -15793,7 +15793,7 @@
         <v>1273</v>
       </c>
       <c r="E656" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="657" spans="1:5" x14ac:dyDescent="0.25">
@@ -16053,7 +16053,7 @@
     </row>
     <row r="672" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B672" s="5">
         <v>1</v>
@@ -16062,15 +16062,15 @@
         <v>260</v>
       </c>
       <c r="D672" s="4" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E672" s="6" t="s">
         <v>1337</v>
-      </c>
-      <c r="E672" s="6" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B673" s="5">
         <v>1</v>
@@ -16079,27 +16079,27 @@
         <v>260</v>
       </c>
       <c r="D673" s="4" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E673" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B674" s="5">
+        <v>1</v>
+      </c>
+      <c r="C674" s="5">
+        <v>260</v>
+      </c>
+      <c r="D674" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="B674" s="5">
-        <v>1</v>
-      </c>
-      <c r="C674" s="5">
-        <v>260</v>
-      </c>
-      <c r="D674" s="4" t="s">
-        <v>1335</v>
-      </c>
       <c r="E674" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>